<commit_message>
Atualizacao de arquivos - 20/01/2026 17:02:23,07
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/NPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dash/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{669CBFB8-0322-4578-9E67-E4E6A92CABAA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="240">
   <si>
     <t>ID</t>
   </si>
@@ -513,6 +513,298 @@
   </si>
   <si>
     <t>Erro de Comunicação</t>
+  </si>
+  <si>
+    <t>O Purificador estava com defeito, passei o final de semana e estou até hoje sem agua filtrada pois ninguém veio repor até agora.</t>
+  </si>
+  <si>
+    <t>Tenho duas assinaturas de purificadores, um instalado na Rua Dr. Nunes,377,Olaria/RJ, e outro instalado na Rua Cleber de Souza Siqueira, 247, Barra de Guaratiba,RJ. No de Olaria a manutenção é realizada, porém a de Barra de Guaratiba não tem manutenção há muito tempo, a Brastemp agenda e não comparece, mas o pagamento do serviço é pago pontualmente.  Não sei o que fazer para resolver</t>
+  </si>
+  <si>
+    <t>Boa</t>
+  </si>
+  <si>
+    <t>O técnico veio atender a OS. 8005258502.10 no dia 09/01/2026, identificou problema no sensor de resfriamento, cortou os cabos e disse que voltaria ontem dia 12/01/2026.
+Não retornou o fechou o chamado. liguei na central e fui informado que só tem data para um novo agendamento dia 22/01/26;</t>
+  </si>
+  <si>
+    <t>Tem técnico que é muito ruim e ficam com preguiça de trocar o filtro. Só entram fazem a limpeza externa e vão embora. 
+Ontem o técnico que me atendeu foi muito PRESTATIVO e ATENCIOSO. É uma raridade, mas especialmente com ele eu gostei do atendimento.</t>
+  </si>
+  <si>
+    <t>Acho muito caro</t>
+  </si>
+  <si>
+    <t>Tenho um purificador há muito tempo e não tenho problemas com o aparelho. Só agendo visita para troca do filtro, no período esperado.</t>
+  </si>
+  <si>
+    <t>Eu sempre fui bem atendida por vocês mas, desde o Ano passado tenho sentido que não têm feito direito as manutenções, marcam e remarcam a toda hora, sem aviso a gente espera e não chega ninguém.  Está complicado</t>
+  </si>
+  <si>
+    <t>Problema não foi resolvido, ficaram de trocar o aparelho,  mas não deram data.</t>
+  </si>
+  <si>
+    <t>Pra expor de fato o que necessito, o atendimento automático é desgastante e após um tempo conseguimos falar com atendente humano e expus o problema do purificador  que nunca hoi higienizado de fato, internamente e a torneira, diante do ocorrido, solicitei a troca do aparelho e me foi informado que na visita técnica seria avaliado se o mesmo deveria ser trocado. 
+Na chegada do técnico, ele nem sabia que deveria avaliar a possível troca do purificador, informou que estava ali para troca da vela e ainda informou que não higienizam torneira e demais partes do purificador e que dificilmente trocam o purificador.
+Indignada tive que aceitar pra não ficar sem água e estarei repensando na continuação dessa parceria e me vem a dúvida, "será que a Vigilância Sanitária tem conhecimento deste fato?"</t>
+  </si>
+  <si>
+    <t>Estão demorando muito para fazer a manutenção. 
+A água fica com gosto ruim por causa da demora para fazer manutenção.</t>
+  </si>
+  <si>
+    <t>AT_ECO_RN_NATAL</t>
+  </si>
+  <si>
+    <t>O purificador é bom, mas demora para agendar a troca do filtro</t>
+  </si>
+  <si>
+    <t>O rapaz veio só trocar o filtro. 
+O reparo da tecla ou botão de água fria não foi trocado. 
+Continuo com problemas.</t>
+  </si>
+  <si>
+    <t>O refil do filtro deve ser trocado a cada 6 meses.
+Segundo o técnico que compareceu no local, o refil foi trocado a 6 meses.
+Questionado pq não ia fazer a troca do refil, ele informou que eu deveria ficar atenta e se a água tivesse mal gosto ligar para virem trocar o refil
+Pergunto se a troca é a cada 6 meses e já deu o prazo pq ele não trocou,?</t>
+  </si>
+  <si>
+    <t>Apresentou vazamento interno</t>
+  </si>
+  <si>
+    <t>Não gostei pq utilizou a mangueira de água que eu já tinha instalada de outro purificador meu para conectar o purificador de vocês. Agora vou ter que comprar a mangueira</t>
+  </si>
+  <si>
+    <t>Demorou um pouco para conseguir a data de instalação. A instalação foi tranquila e o uso está sendo ótimo.
+O único porém é que fiquei sabendo só depois de já pedir, que eu teria que comprar avulso os cilindros de gás (plano sparkling). Deveria já estar incluso no plano, uma vez que é uma assinatura completa</t>
+  </si>
+  <si>
+    <t>Não apareceu ninguém na minha casa.</t>
+  </si>
+  <si>
+    <t>Só abriram chamado para 1 purificador, sendo que temos 2.
+O técnico não fez a manutenção corretamente, não trocou o elemento filtrante e a água estava com gosto ruim. Péssimo atendimento!!!! Abri reclamação no SAC.</t>
+  </si>
+  <si>
+    <t>Sobre o último atendimento de VT para a manutenção do aparelho, senti muita diferença,  a técnica realizou teste de qualidade da água. Não fez limpeza e não tirou aparelho do lugar,  das outras vezes não foi assim.</t>
+  </si>
+  <si>
+    <t>tenho o purificador há aproximadamente 22 anos, até 3 anos atrás era bom, hoje com 1 mês de troca de elementos filtrantes, a água fica podre, contaminada, gosto e cheiro péssimos,equanto vcs não trocarem os aparelhos, mangueiras e etc, e ficarem apenas na troca dos elementos filtrantes, essa contaminação continuará acontecendo antes dos 6 meses.Essa foi a última vez que aceitei fazerem essa prática, tenho certeza que antes de 1 mês a água estará apodrecida de novo, ou seja, mesmo trocando os filtros não confiamos na água, já estou pesquisando outros filtros para cancelar minha assinatura pela falta de consideração da empresa Brastemp, pois já pedi a troca do aparelho e demais peças, mas o técnico chega e diz que foi agendado apenas a manutenção!</t>
+  </si>
+  <si>
+    <t>O rapaz que veio à empresa merece nota 10. A nota 8 refere‑se ao atendimento telefônico: realizamos três agendamentos e, em todos eles, por diferentes motivos atribuídos à própria Brastemp, o serviço não foi concluído. Em razão disso, estamos há 30 dias sem utilizar o purificador de água.</t>
+  </si>
+  <si>
+    <t>Data Distante</t>
+  </si>
+  <si>
+    <t>Porque pensei que iriao trocar no dia seguinte , vou tem que esperar 17 dias para fazer a troca e também não tem nenhum aparelho para substitui- lo.
+Estou correndo risco de incendiar meu apartamento , o calor está muito quente, não posso ficar sem beber água e sem fazer comida . Estou passando nervoso , tensão, danos psicológicos, brigando com meu irmão, não quer desligar o aparelho , estou estressado, não sei se vou continuar com este aparelho no futuro.
+Já não t em mais Active 3 temperaturas.. Só irão instalar novo aparelho 31/01 até lá pode incendiar.
+Está esquentando muito e fazendo barulho ...
+E não tem uma viva alma que faça meu irmão desligar este aparelho 
+O Francisco foi muito fraco na decisão...precisa falar com mão firmeza.
+Falar que não podia de jeito nenhum ligar este aparelho .
+Mas ele não se meteu pode pegar fogo, mas não é a casa dele.
+Estou muito chateada com este fato.
+Minha nota é 5 .
+Moro em apartamento e tem famílias ao redor e desdém com o ser humano.
+Não ajudou em nada o técnico em nada, nem uma palavra de dizer desligar o aparelho .
+Mas Deus está no controle te tudo.
+Também achei o dia 31/01 muito longe para trocar o aparelho.
+Segundo.o.Franciso tem em estoque.
+Não sei porque essa dia tão prolongado???
+Atenciosamente,
+Sulamita</t>
+  </si>
+  <si>
+    <t>Falta de estoque/peças</t>
+  </si>
+  <si>
+    <t>Tenho esse contrato a muitos anos já. Sempre fui bem atendida. Mas de 2025 pra cá foi muito descaso e falta de profissionalismo. Me deixaram esperando por meses para troca do meu filtro. Agendava e não compareciam. E o agendamento está muito distante. Levam muitos dias e meses pra resolver um problema.  Estou analisando se vou continuar com o serviço ou se vou pedir o cancelamento.</t>
+  </si>
+  <si>
+    <t>Temos o purificador de ar há alguns anos e foi a primeira vez q tivemos o problema da água não gelar, o q foi muito desagradável. Não sei se existe algum filtro da Brastemp mais moderno e q comporte um volume maior de água gelada para q não tenhamos esse problema de novo. Sei que no mercado já existem filtros q comportam um volume maior.</t>
+  </si>
+  <si>
+    <t>Tenho o produto faz um bom tempo, porém o atendimento caiu muito nos últimos anos.
+A qualidade dos serviços piorou muito.</t>
+  </si>
+  <si>
+    <t>Pior possível</t>
+  </si>
+  <si>
+    <t>O purificador foi entregue ontem porem  apresentou defeito na água com gás que falaram que iriam resolver em breve.
+Ainda não recebi o contato com a data da troca do aparelho e já iniciou meu plano que inclui a água com gás ou seja estou pagando por um serviço que ainda não recebi</t>
+  </si>
+  <si>
+    <t>Entao des de quando contratei o serviço nao usei o purificador agora que o técnico foi em casa e mexeu novamente espero que nao congele a agua mais infelizmente nao tive um experiência muito boa espero que funcione daqui para frente boa tarde</t>
+  </si>
+  <si>
+    <t>O filtro está congelado e segue com esse problema. Ficaram de retornar pra arrumar e ate agora nada.</t>
+  </si>
+  <si>
+    <t>Tenho ha alguns anos e gosto muito</t>
+  </si>
+  <si>
+    <t>Atende nossa necessidade.</t>
+  </si>
+  <si>
+    <t>o técnico muito bom, so que o serviço ainda nao foi resolvido estou no aguardo</t>
+  </si>
+  <si>
+    <t>A visita técnica agendada para ontem (15/01/26) não foi realizada porque o técnico não apareceu.
+Fiquei a tarde toda em casa aguardando. Liguei após as 18h para o SAC e registrei o ocorrido. O atendente realizou novo agendamento para o mês que vem em data que não me atende.
+Estou aguardando um retorno com uma nova data mais próxima e factível.</t>
+  </si>
+  <si>
+    <t>To ha 3 meses sem filtro pois voces ja furaram comigo 2 vezes!!!!!!!</t>
+  </si>
+  <si>
+    <t>Preciso de um retorno pois está com vazamento de água</t>
+  </si>
+  <si>
+    <t>Este último atendimento houve a troca de uma peça defeituosa por outra usada. Acho que deveria ser uma peça nova.</t>
+  </si>
+  <si>
+    <t>Minha última solicitação de serviço, não foi atendida, o técnico não apareceu e simplesmente Não deu Nenhuma Satisfação. Muito Ruim.</t>
+  </si>
+  <si>
+    <t>Filtro voltou a gelar , porém continua com vazamento</t>
+  </si>
+  <si>
+    <t>Tudo bom.</t>
+  </si>
+  <si>
+    <t>O custo é similar a um filtro comprado com a vantagem de não ter que se preocupar com a troca do refil.
+No caso, para a minha mãe, que ja tem bastante idade, funciona muito bem.</t>
+  </si>
+  <si>
+    <t>Tenho assinatura desde 2010. Entendo que com o avanço da tecnologia, a Brastemp deveria substituir periodicamente equipamentos antigos, pois se trata de um comodato, o qual deve garantir a qualidadade da água e do equipamento sempre perfeita.
+Não concordo apenas, com a situação durante as preventivas, de verificação de possível equipamento ou periféricos que possam estar apresentando indícios de falha e não seja indicada internamente a imediata correção, antes da ocorrência se concretizar e penalizar o cliente.
+Afirmar que as preventivas são apenas para garantir a qualidade da água é uma visão empresarial restrita, pois também se deve garantir a qualidade e funcionalidade do equipamento colocado à disposição do cliente em regime de comodato / aluguel com assinatura mensal.
+Se a área de atendimento ao cliente, posterior à esta pesquisa, não tem ação sobre essas necessidades e procedimentos interno, também denota, infelizmente, uma falha conceitual nos processos e no sistema de gestão.
+Se necessário, me coloco à disposição da Brastemp para fazer parte da equipe de gestão para implementar uma visão mais abrangente de atendimento, gestão interna e modernização de processos, para solidificação da marca no mercado perante seus clientes.</t>
+  </si>
+  <si>
+    <t>Em geral é muito bom. Só qdo tive q trocar o imóvel e transferir meu aparelho, foi bem ruim e demorado.</t>
+  </si>
+  <si>
+    <t>O tempo para agendar a manutenção e alto demais.</t>
+  </si>
+  <si>
+    <t>Fui muito bem atendido e o técnico muito bom. Porém, quandoa indicação do produto  fiz muito pouco uso, portanto não tenho conhecimento do mesmo</t>
+  </si>
+  <si>
+    <t>O Técnico fez uma gambiarra e não resolveu o problema de vazamento de água na borracha que  vai até a torneira !!! Sinceramente, nem parecia Técnico!! E a primeira vez que tenho esse tipo de problema com a Brastemp!! Isso em dois dias de visita !!</t>
+  </si>
+  <si>
+    <t>nao foram</t>
+  </si>
+  <si>
+    <t>Nós últimos 2 meses tivemos sérios problemas com o mal cheiro da água. Trocaram 2 vezes o elemento filtrante e o problema voltou. 
+Agora foi trocado pela 3ª vez.
+Vamos ver se o problema será solucionado.</t>
+  </si>
+  <si>
+    <t>O atendimento esta mto ruim....depois de 1 visita tecnica onde o tecnico nao trocou o refil...dias depois comecou a sair agua cinza entrei em contato com vcs ....e mesmo assim fiquei dede o dia 4 de janeiro sem ussr o filtro...espero que vcs a cada visita tecnica troque o refil...pois 130 reais por mes i o refil nao é nada...e nao desagrada o cliente...espero nao passar mais por isso....pois estou seriamente pensando em cancelar o produto....sem mais</t>
+  </si>
+  <si>
+    <t>Tive vários problemas com vcs !
+Fiquei 1 (um) ano sem receber manutenção e sem receber água de boa qualidade, por estar com o equipamento vazando e vcs não faziam a troca, mesmo eu sendo cliente antigo e adimplente. Pagando a mensalidade rigorosamente em dia, através de débito em conta.
+Depois de todo esse tempo consegui a troca do equipamento.
+Desejo saber: como posso ser ressarcido, dos pagamentos que fiz sem receber o serviço contratado ?
+Preciso ser ressarcido pelo menos com  um bom abatimento na minha mensalidade.
+AGUARDO RETORNO !</t>
+  </si>
+  <si>
+    <t>filtro com defeito, e não foi consertado</t>
+  </si>
+  <si>
+    <t>Não vou falar aqui sobre o atendimento do técnico, que foi regular. Mas vou falar da dificuldade de conseguir agendar o atendimento, que desde Novembro estou tentando a troca do purificador, sem poder usá-lo, gastando dinheiro com água mineral e a Brastemp não me atende. Depois de mais de 2 meses é que consegui atendimento. O serviço da Brastemp está muito ruim... NOTA ZERO!!!!</t>
+  </si>
+  <si>
+    <t>No período de um ano já manifestou problemas três vezes: duas por odor desagradável ( fétido) na água, descontrole do fluxo de água. Antes já havia apresentado vazamento. Cada problema desse nos deixa sem acesso a água purificada por mais de uma semana.</t>
+  </si>
+  <si>
+    <t>Problema não resolvido. Promessa de retorno em 2 dias úteis não cumpridas</t>
+  </si>
+  <si>
+    <t>O SLA do atendimento técnico foi rápido e prático, porém o atendimento do administrativo é péssimo. Todos os meses temos dificuldades com a envio das faturas com as datas erradas e para conseguir falar com alguém, não conseguimos.</t>
+  </si>
+  <si>
+    <t>AT_ECO_ES_VILA VELHA_2</t>
+  </si>
+  <si>
+    <t>O purificador foi verificado e só achei estranho que após 12 meses de uso, aí da não fizeram a substituição do elemento filtrante.</t>
+  </si>
+  <si>
+    <t>não resolveram meu problema</t>
+  </si>
+  <si>
+    <t>A demora em se conseguir um agendamento técnico é o maior problema de vocês. Só por isso não acho o serviço ótimo, uma pena.</t>
+  </si>
+  <si>
+    <t>Até o dia da visita, eram só problemas. Entretanto, ele foi resolvido pelo menos por enquanto, o suficiente para que eu acompanhe o andamento e possa revisar a minha prbabilidade de indicação.</t>
+  </si>
+  <si>
+    <t>O purificador esquenta e o custo é muito caro</t>
+  </si>
+  <si>
+    <t>O purificador deu problema. Acredito que o melhor seria ter sido trocado. Não eu ficar gastando minha água esperando do peça para o purificador. Es</t>
+  </si>
+  <si>
+    <t>Revisão conforme contrato e atendimento cordial do técnico.</t>
+  </si>
+  <si>
+    <t>O aparelho é muito bom, mas infelizmente o preço está muito alto!</t>
+  </si>
+  <si>
+    <t>O técnico veio para efetuar  a troca do equipamento, porém na testou, e nem explicou nada. Depois saiu a pessoa estava fortíssima e o purificador fazendo um barulho estranho e forte</t>
+  </si>
+  <si>
+    <t>Ruído</t>
+  </si>
+  <si>
+    <t>Tirando a demora do atendimento de um técnico não tenho do que reclamar . E tbm de na fazerem a troca do filtro nas visitas periódicas</t>
+  </si>
+  <si>
+    <t>FRQ_ECO_DF_BRASILIA_2</t>
+  </si>
+  <si>
+    <t>A manutenção aqui em Goiânia está péssima. MENTIRAM e a Brastemp acredita.
+Nenhum apoio ao cliente.
+Nenhum SAC para falarmos
+Milhares de confirmações a cada conversa no WhatsApp ou telefone.</t>
+  </si>
+  <si>
+    <t>UM BOTÃO DE AGUA GELADA VEIO COM UM LEVE PROBLEMA DE ACIONAMENTO</t>
+  </si>
+  <si>
+    <t>Muito bom, na maior parte do tempo. Porém, tem sofrido no verão, esquentando muito ao longo do dia. Tanto que tivemos que desligar algumas vezes, com medo de que pudesse ter algum problema elétrico.</t>
+  </si>
+  <si>
+    <t>O aparelho chegou ruim e não esta gelando.</t>
+  </si>
+  <si>
+    <t>É bacana mas acho que já poderiam
+Trocar o equipamento</t>
+  </si>
+  <si>
+    <t>O operador avisou q a máquina não funciona. Pediu substituição. Já estou há dias ela em água no meu estabelecimento.</t>
+  </si>
+  <si>
+    <t>O técnico não cumpriu o agendamento, visita de manutenção com duração de menos de 5 minutos.</t>
+  </si>
+  <si>
+    <t>Agendada a instalação para o dia 09/01, deixei uma pessoa das 8 às 15h para receber o instalador que não apareceu. O reagendamento foi um transtorno pois não conseguimos contato direto com o setor responsavel, querem que atendemos ligação telefônica mas não sabem informar que número ou pré fixo ligará. Eu não atendo ligação de número desconhecido devido a trote. A instalação ocorreu dia 19/01 mas o aparelho faz um barulho alto qdo aperta e desaperta os botões de saída de água, eu não estava no momento da instalação mas o técnico deveria ter feitos testes para já detectar esse barulho e arrumar.</t>
+  </si>
+  <si>
+    <t>Eu não entendo porque ligam agendando, pedem pra gente escolher um horário, passam uma senha, depois ligam pra confirmar se podem manter a visita, você confirma, chega no dia, vem em horario diferente e nem pedem senha.</t>
+  </si>
+  <si>
+    <t>Não fez a manutenção em todos os bebedouros necessários</t>
   </si>
 </sst>
 </file>
@@ -879,15 +1171,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:J176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -3798,6 +4090,2210 @@
         <v>22</v>
       </c>
     </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101">
+        <v>8005258743</v>
+      </c>
+      <c r="D101" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" t="s">
+        <v>159</v>
+      </c>
+      <c r="H101" t="s">
+        <v>35</v>
+      </c>
+      <c r="I101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102">
+        <v>8005252677</v>
+      </c>
+      <c r="D102" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E102" t="s">
+        <v>53</v>
+      </c>
+      <c r="F102" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" t="s">
+        <v>160</v>
+      </c>
+      <c r="H102" t="s">
+        <v>18</v>
+      </c>
+      <c r="I102" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>8005259921</v>
+      </c>
+      <c r="D103" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E103" t="s">
+        <v>27</v>
+      </c>
+      <c r="F103" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" t="s">
+        <v>161</v>
+      </c>
+      <c r="H103" t="s">
+        <v>13</v>
+      </c>
+      <c r="I103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104">
+        <v>8005258502</v>
+      </c>
+      <c r="D104" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E104" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" t="s">
+        <v>162</v>
+      </c>
+      <c r="H104" t="s">
+        <v>32</v>
+      </c>
+      <c r="I104" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105">
+        <v>8005223985</v>
+      </c>
+      <c r="D105" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E105" t="s">
+        <v>27</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" t="s">
+        <v>163</v>
+      </c>
+      <c r="H105" t="s">
+        <v>18</v>
+      </c>
+      <c r="I105" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106">
+        <v>8005255092</v>
+      </c>
+      <c r="D106" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E106" t="s">
+        <v>65</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" t="s">
+        <v>164</v>
+      </c>
+      <c r="H106" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>8005256600</v>
+      </c>
+      <c r="D107" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E107" t="s">
+        <v>53</v>
+      </c>
+      <c r="F107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" t="s">
+        <v>165</v>
+      </c>
+      <c r="H107" t="s">
+        <v>13</v>
+      </c>
+      <c r="I107" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108">
+        <v>8005192408</v>
+      </c>
+      <c r="D108" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E108" t="s">
+        <v>20</v>
+      </c>
+      <c r="F108" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" t="s">
+        <v>166</v>
+      </c>
+      <c r="H108" t="s">
+        <v>18</v>
+      </c>
+      <c r="I108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109">
+        <v>8005236526</v>
+      </c>
+      <c r="D109" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E109" t="s">
+        <v>27</v>
+      </c>
+      <c r="F109" t="s">
+        <v>11</v>
+      </c>
+      <c r="G109" t="s">
+        <v>161</v>
+      </c>
+      <c r="H109" t="s">
+        <v>13</v>
+      </c>
+      <c r="I109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>8005247515</v>
+      </c>
+      <c r="D110" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E110" t="s">
+        <v>70</v>
+      </c>
+      <c r="F110" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" t="s">
+        <v>167</v>
+      </c>
+      <c r="H110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>8005260859</v>
+      </c>
+      <c r="D111" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E111" t="s">
+        <v>20</v>
+      </c>
+      <c r="F111" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111" t="s">
+        <v>168</v>
+      </c>
+      <c r="H111" t="s">
+        <v>18</v>
+      </c>
+      <c r="I111" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112">
+        <v>8005231159</v>
+      </c>
+      <c r="D112" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E112" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" t="s">
+        <v>169</v>
+      </c>
+      <c r="H112" t="s">
+        <v>32</v>
+      </c>
+      <c r="I112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113">
+        <v>8005260278</v>
+      </c>
+      <c r="D113" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E113" t="s">
+        <v>170</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" t="s">
+        <v>171</v>
+      </c>
+      <c r="H113" t="s">
+        <v>32</v>
+      </c>
+      <c r="I113" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114">
+        <v>8005261736</v>
+      </c>
+      <c r="D114" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E114" t="s">
+        <v>53</v>
+      </c>
+      <c r="F114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>172</v>
+      </c>
+      <c r="H114" t="s">
+        <v>18</v>
+      </c>
+      <c r="I114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>8005230993</v>
+      </c>
+      <c r="D115" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E115" t="s">
+        <v>27</v>
+      </c>
+      <c r="F115" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" t="s">
+        <v>173</v>
+      </c>
+      <c r="H115" t="s">
+        <v>18</v>
+      </c>
+      <c r="I115" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>8005258595</v>
+      </c>
+      <c r="D116" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E116" t="s">
+        <v>23</v>
+      </c>
+      <c r="F116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" t="s">
+        <v>174</v>
+      </c>
+      <c r="H116" t="s">
+        <v>35</v>
+      </c>
+      <c r="I116" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117">
+        <v>8005230420</v>
+      </c>
+      <c r="D117" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E117" t="s">
+        <v>23</v>
+      </c>
+      <c r="F117" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117" t="s">
+        <v>175</v>
+      </c>
+      <c r="H117" t="s">
+        <v>18</v>
+      </c>
+      <c r="I117" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118">
+        <v>8005261166</v>
+      </c>
+      <c r="D118" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E118" t="s">
+        <v>91</v>
+      </c>
+      <c r="F118" t="s">
+        <v>11</v>
+      </c>
+      <c r="G118" t="s">
+        <v>176</v>
+      </c>
+      <c r="H118" t="s">
+        <v>63</v>
+      </c>
+      <c r="I118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <v>8005051220</v>
+      </c>
+      <c r="D119" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E119" t="s">
+        <v>53</v>
+      </c>
+      <c r="F119" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" t="s">
+        <v>177</v>
+      </c>
+      <c r="H119" t="s">
+        <v>18</v>
+      </c>
+      <c r="I119" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120">
+        <v>8005213337</v>
+      </c>
+      <c r="D120" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E120" t="s">
+        <v>23</v>
+      </c>
+      <c r="F120" t="s">
+        <v>16</v>
+      </c>
+      <c r="G120" t="s">
+        <v>178</v>
+      </c>
+      <c r="H120" t="s">
+        <v>18</v>
+      </c>
+      <c r="I120" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121">
+        <v>8005251602</v>
+      </c>
+      <c r="D121" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E121" t="s">
+        <v>27</v>
+      </c>
+      <c r="F121" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" t="s">
+        <v>179</v>
+      </c>
+      <c r="H121" t="s">
+        <v>18</v>
+      </c>
+      <c r="I121" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122">
+        <v>8005257329</v>
+      </c>
+      <c r="D122" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E122" t="s">
+        <v>23</v>
+      </c>
+      <c r="F122" t="s">
+        <v>16</v>
+      </c>
+      <c r="G122" t="s">
+        <v>180</v>
+      </c>
+      <c r="H122" t="s">
+        <v>35</v>
+      </c>
+      <c r="I122" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123">
+        <v>8005249656</v>
+      </c>
+      <c r="D123" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E123" t="s">
+        <v>20</v>
+      </c>
+      <c r="F123" t="s">
+        <v>11</v>
+      </c>
+      <c r="G123" t="s">
+        <v>181</v>
+      </c>
+      <c r="H123" t="s">
+        <v>32</v>
+      </c>
+      <c r="I123" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124">
+        <v>8005262815</v>
+      </c>
+      <c r="D124" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E124" t="s">
+        <v>20</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" t="s">
+        <v>183</v>
+      </c>
+      <c r="H124" t="s">
+        <v>154</v>
+      </c>
+      <c r="I124" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <v>8005256693</v>
+      </c>
+      <c r="D125" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E125" t="s">
+        <v>27</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" t="s">
+        <v>185</v>
+      </c>
+      <c r="H125" t="s">
+        <v>18</v>
+      </c>
+      <c r="I125" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>8005263205</v>
+      </c>
+      <c r="D126" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E126" t="s">
+        <v>23</v>
+      </c>
+      <c r="F126" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" t="s">
+        <v>186</v>
+      </c>
+      <c r="H126" t="s">
+        <v>35</v>
+      </c>
+      <c r="I126" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>8005223499</v>
+      </c>
+      <c r="D127" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E127" t="s">
+        <v>23</v>
+      </c>
+      <c r="F127" t="s">
+        <v>11</v>
+      </c>
+      <c r="G127" t="s">
+        <v>187</v>
+      </c>
+      <c r="H127" t="s">
+        <v>13</v>
+      </c>
+      <c r="I127" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128">
+        <v>8005265771</v>
+      </c>
+      <c r="D128" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E128" t="s">
+        <v>20</v>
+      </c>
+      <c r="F128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" t="s">
+        <v>188</v>
+      </c>
+      <c r="H128" t="s">
+        <v>13</v>
+      </c>
+      <c r="I128" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129">
+        <v>8005260479</v>
+      </c>
+      <c r="D129" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E129" t="s">
+        <v>20</v>
+      </c>
+      <c r="F129" t="s">
+        <v>11</v>
+      </c>
+      <c r="G129" t="s">
+        <v>189</v>
+      </c>
+      <c r="H129" t="s">
+        <v>63</v>
+      </c>
+      <c r="I129" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <v>8005223926</v>
+      </c>
+      <c r="D130" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E130" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" t="s">
+        <v>11</v>
+      </c>
+      <c r="G130" t="s">
+        <v>190</v>
+      </c>
+      <c r="H130" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>8005262985</v>
+      </c>
+      <c r="D131" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E131" t="s">
+        <v>44</v>
+      </c>
+      <c r="F131" t="s">
+        <v>11</v>
+      </c>
+      <c r="G131" t="s">
+        <v>191</v>
+      </c>
+      <c r="H131" t="s">
+        <v>35</v>
+      </c>
+      <c r="I131" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132">
+        <v>8005256837</v>
+      </c>
+      <c r="D132" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E132" t="s">
+        <v>15</v>
+      </c>
+      <c r="F132" t="s">
+        <v>11</v>
+      </c>
+      <c r="G132" t="s">
+        <v>192</v>
+      </c>
+      <c r="H132" t="s">
+        <v>13</v>
+      </c>
+      <c r="I132" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133">
+        <v>8005239673</v>
+      </c>
+      <c r="D133" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E133" t="s">
+        <v>20</v>
+      </c>
+      <c r="F133" t="s">
+        <v>11</v>
+      </c>
+      <c r="G133" t="s">
+        <v>193</v>
+      </c>
+      <c r="H133" t="s">
+        <v>13</v>
+      </c>
+      <c r="I133" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134">
+        <v>8005256643</v>
+      </c>
+      <c r="D134" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E134" t="s">
+        <v>27</v>
+      </c>
+      <c r="F134" t="s">
+        <v>11</v>
+      </c>
+      <c r="G134" t="s">
+        <v>194</v>
+      </c>
+      <c r="H134" t="s">
+        <v>18</v>
+      </c>
+      <c r="I134" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>8005244839</v>
+      </c>
+      <c r="D135" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E135" t="s">
+        <v>37</v>
+      </c>
+      <c r="F135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" t="s">
+        <v>195</v>
+      </c>
+      <c r="H135" t="s">
+        <v>18</v>
+      </c>
+      <c r="I135" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136">
+        <v>8005255168</v>
+      </c>
+      <c r="D136" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E136" t="s">
+        <v>37</v>
+      </c>
+      <c r="F136" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" t="s">
+        <v>196</v>
+      </c>
+      <c r="H136" t="s">
+        <v>18</v>
+      </c>
+      <c r="I136" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137">
+        <v>8005192192</v>
+      </c>
+      <c r="D137" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E137" t="s">
+        <v>37</v>
+      </c>
+      <c r="F137" t="s">
+        <v>11</v>
+      </c>
+      <c r="G137" t="s">
+        <v>197</v>
+      </c>
+      <c r="H137" t="s">
+        <v>35</v>
+      </c>
+      <c r="I137" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138">
+        <v>8005266175</v>
+      </c>
+      <c r="D138" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E138" t="s">
+        <v>98</v>
+      </c>
+      <c r="F138" t="s">
+        <v>16</v>
+      </c>
+      <c r="G138" t="s">
+        <v>198</v>
+      </c>
+      <c r="H138" t="s">
+        <v>154</v>
+      </c>
+      <c r="I138" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139">
+        <v>8005260318</v>
+      </c>
+      <c r="D139" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E139" t="s">
+        <v>53</v>
+      </c>
+      <c r="F139" t="s">
+        <v>11</v>
+      </c>
+      <c r="G139" t="s">
+        <v>199</v>
+      </c>
+      <c r="H139" t="s">
+        <v>18</v>
+      </c>
+      <c r="I139" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>8005262227</v>
+      </c>
+      <c r="D140" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E140" t="s">
+        <v>53</v>
+      </c>
+      <c r="F140" t="s">
+        <v>16</v>
+      </c>
+      <c r="G140" t="s">
+        <v>200</v>
+      </c>
+      <c r="H140" t="s">
+        <v>18</v>
+      </c>
+      <c r="I140" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>9</v>
+      </c>
+      <c r="C141">
+        <v>8005249800</v>
+      </c>
+      <c r="D141" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E141" t="s">
+        <v>20</v>
+      </c>
+      <c r="F141" t="s">
+        <v>11</v>
+      </c>
+      <c r="G141" t="s">
+        <v>201</v>
+      </c>
+      <c r="H141" t="s">
+        <v>13</v>
+      </c>
+      <c r="I141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142">
+        <v>8005229595</v>
+      </c>
+      <c r="D142" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E142" t="s">
+        <v>23</v>
+      </c>
+      <c r="F142" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142" t="s">
+        <v>202</v>
+      </c>
+      <c r="H142" t="s">
+        <v>13</v>
+      </c>
+      <c r="I142" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <v>8005266553</v>
+      </c>
+      <c r="D143" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E143" t="s">
+        <v>44</v>
+      </c>
+      <c r="F143" t="s">
+        <v>11</v>
+      </c>
+      <c r="G143" t="s">
+        <v>203</v>
+      </c>
+      <c r="H143" t="s">
+        <v>35</v>
+      </c>
+      <c r="I143" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144">
+        <v>8005267367</v>
+      </c>
+      <c r="D144" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E144" t="s">
+        <v>49</v>
+      </c>
+      <c r="F144" t="s">
+        <v>11</v>
+      </c>
+      <c r="G144" t="s">
+        <v>204</v>
+      </c>
+      <c r="H144" t="s">
+        <v>13</v>
+      </c>
+      <c r="I144" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145">
+        <v>8005216018</v>
+      </c>
+      <c r="D145" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E145" t="s">
+        <v>20</v>
+      </c>
+      <c r="F145" t="s">
+        <v>11</v>
+      </c>
+      <c r="G145" t="s">
+        <v>205</v>
+      </c>
+      <c r="H145" t="s">
+        <v>32</v>
+      </c>
+      <c r="I145" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>61</v>
+      </c>
+      <c r="C146">
+        <v>8005247989</v>
+      </c>
+      <c r="D146" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E146" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>11</v>
+      </c>
+      <c r="G146" t="s">
+        <v>206</v>
+      </c>
+      <c r="H146" t="s">
+        <v>13</v>
+      </c>
+      <c r="I146" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147">
+        <v>8005262662</v>
+      </c>
+      <c r="D147" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E147" t="s">
+        <v>53</v>
+      </c>
+      <c r="F147" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" t="s">
+        <v>207</v>
+      </c>
+      <c r="H147" t="s">
+        <v>18</v>
+      </c>
+      <c r="I147" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148">
+        <v>8005267113</v>
+      </c>
+      <c r="D148" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E148" t="s">
+        <v>98</v>
+      </c>
+      <c r="F148" t="s">
+        <v>16</v>
+      </c>
+      <c r="G148" t="s">
+        <v>208</v>
+      </c>
+      <c r="H148" t="s">
+        <v>18</v>
+      </c>
+      <c r="I148" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149">
+        <v>8005262718</v>
+      </c>
+      <c r="D149" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E149" t="s">
+        <v>23</v>
+      </c>
+      <c r="F149" t="s">
+        <v>16</v>
+      </c>
+      <c r="G149" t="s">
+        <v>209</v>
+      </c>
+      <c r="H149" t="s">
+        <v>18</v>
+      </c>
+      <c r="I149" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150">
+        <v>8005249868</v>
+      </c>
+      <c r="D150" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E150" t="s">
+        <v>27</v>
+      </c>
+      <c r="F150" t="s">
+        <v>16</v>
+      </c>
+      <c r="G150" t="s">
+        <v>210</v>
+      </c>
+      <c r="H150" t="s">
+        <v>18</v>
+      </c>
+      <c r="I150" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151">
+        <v>8005247595</v>
+      </c>
+      <c r="D151" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E151" t="s">
+        <v>53</v>
+      </c>
+      <c r="F151" t="s">
+        <v>11</v>
+      </c>
+      <c r="G151" t="s">
+        <v>211</v>
+      </c>
+      <c r="H151" t="s">
+        <v>18</v>
+      </c>
+      <c r="I151" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152">
+        <v>8005258890</v>
+      </c>
+      <c r="D152" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E152" t="s">
+        <v>20</v>
+      </c>
+      <c r="F152" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" t="s">
+        <v>212</v>
+      </c>
+      <c r="H152" t="s">
+        <v>18</v>
+      </c>
+      <c r="I152" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>9</v>
+      </c>
+      <c r="C153">
+        <v>8005260567</v>
+      </c>
+      <c r="D153" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E153" t="s">
+        <v>49</v>
+      </c>
+      <c r="F153" t="s">
+        <v>16</v>
+      </c>
+      <c r="G153" t="s">
+        <v>213</v>
+      </c>
+      <c r="H153" t="s">
+        <v>32</v>
+      </c>
+      <c r="I153" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154">
+        <v>8005262835</v>
+      </c>
+      <c r="D154" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E154" t="s">
+        <v>74</v>
+      </c>
+      <c r="F154" t="s">
+        <v>11</v>
+      </c>
+      <c r="G154" t="s">
+        <v>214</v>
+      </c>
+      <c r="H154" t="s">
+        <v>35</v>
+      </c>
+      <c r="I154" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <v>8005265282</v>
+      </c>
+      <c r="D155" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E155" t="s">
+        <v>20</v>
+      </c>
+      <c r="F155" t="s">
+        <v>16</v>
+      </c>
+      <c r="G155" t="s">
+        <v>215</v>
+      </c>
+      <c r="H155" t="s">
+        <v>18</v>
+      </c>
+      <c r="I155" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156">
+        <v>8005263865</v>
+      </c>
+      <c r="D156" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E156" t="s">
+        <v>98</v>
+      </c>
+      <c r="F156" t="s">
+        <v>11</v>
+      </c>
+      <c r="G156" t="s">
+        <v>216</v>
+      </c>
+      <c r="H156" t="s">
+        <v>13</v>
+      </c>
+      <c r="I156" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <v>8005252337</v>
+      </c>
+      <c r="D157" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E157" t="s">
+        <v>217</v>
+      </c>
+      <c r="F157" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157" t="s">
+        <v>218</v>
+      </c>
+      <c r="H157" t="s">
+        <v>18</v>
+      </c>
+      <c r="I157" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158">
+        <v>8005252920</v>
+      </c>
+      <c r="D158" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E158" t="s">
+        <v>23</v>
+      </c>
+      <c r="F158" t="s">
+        <v>16</v>
+      </c>
+      <c r="G158" t="s">
+        <v>219</v>
+      </c>
+      <c r="H158" t="s">
+        <v>18</v>
+      </c>
+      <c r="I158" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>9</v>
+      </c>
+      <c r="C159">
+        <v>8005235115</v>
+      </c>
+      <c r="D159" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E159" t="s">
+        <v>20</v>
+      </c>
+      <c r="F159" t="s">
+        <v>16</v>
+      </c>
+      <c r="G159" t="s">
+        <v>220</v>
+      </c>
+      <c r="H159" t="s">
+        <v>32</v>
+      </c>
+      <c r="I159" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160">
+        <v>8005265874</v>
+      </c>
+      <c r="D160" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E160" t="s">
+        <v>15</v>
+      </c>
+      <c r="F160" t="s">
+        <v>16</v>
+      </c>
+      <c r="G160" t="s">
+        <v>221</v>
+      </c>
+      <c r="H160" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161">
+        <v>8005266129</v>
+      </c>
+      <c r="D161" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E161" t="s">
+        <v>23</v>
+      </c>
+      <c r="F161" t="s">
+        <v>16</v>
+      </c>
+      <c r="G161" t="s">
+        <v>222</v>
+      </c>
+      <c r="H161" t="s">
+        <v>13</v>
+      </c>
+      <c r="I161" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <v>8005262794</v>
+      </c>
+      <c r="D162" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E162" t="s">
+        <v>53</v>
+      </c>
+      <c r="F162" t="s">
+        <v>16</v>
+      </c>
+      <c r="G162" t="s">
+        <v>223</v>
+      </c>
+      <c r="H162" t="s">
+        <v>154</v>
+      </c>
+      <c r="I162" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>9</v>
+      </c>
+      <c r="C163">
+        <v>8005271122</v>
+      </c>
+      <c r="D163" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E163" t="s">
+        <v>37</v>
+      </c>
+      <c r="F163" t="s">
+        <v>11</v>
+      </c>
+      <c r="G163" t="s">
+        <v>224</v>
+      </c>
+      <c r="H163" t="s">
+        <v>13</v>
+      </c>
+      <c r="I163" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>9</v>
+      </c>
+      <c r="C164">
+        <v>8005250540</v>
+      </c>
+      <c r="D164" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E164" t="s">
+        <v>74</v>
+      </c>
+      <c r="F164" t="s">
+        <v>11</v>
+      </c>
+      <c r="G164" t="s">
+        <v>225</v>
+      </c>
+      <c r="H164" t="s">
+        <v>13</v>
+      </c>
+      <c r="I164" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>9</v>
+      </c>
+      <c r="C165">
+        <v>8005255286</v>
+      </c>
+      <c r="D165" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E165" t="s">
+        <v>23</v>
+      </c>
+      <c r="F165" t="s">
+        <v>16</v>
+      </c>
+      <c r="G165" t="s">
+        <v>226</v>
+      </c>
+      <c r="H165" t="s">
+        <v>35</v>
+      </c>
+      <c r="I165" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>9</v>
+      </c>
+      <c r="C166">
+        <v>8005269827</v>
+      </c>
+      <c r="D166" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E166" t="s">
+        <v>20</v>
+      </c>
+      <c r="F166" t="s">
+        <v>11</v>
+      </c>
+      <c r="G166" t="s">
+        <v>228</v>
+      </c>
+      <c r="H166" t="s">
+        <v>18</v>
+      </c>
+      <c r="I166" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167">
+        <v>8005247586</v>
+      </c>
+      <c r="D167" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E167" t="s">
+        <v>229</v>
+      </c>
+      <c r="F167" t="s">
+        <v>16</v>
+      </c>
+      <c r="G167" t="s">
+        <v>230</v>
+      </c>
+      <c r="H167" t="s">
+        <v>13</v>
+      </c>
+      <c r="I167" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>61</v>
+      </c>
+      <c r="C168">
+        <v>8005264190</v>
+      </c>
+      <c r="D168" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E168" t="s">
+        <v>65</v>
+      </c>
+      <c r="F168" t="s">
+        <v>16</v>
+      </c>
+      <c r="G168" t="s">
+        <v>231</v>
+      </c>
+      <c r="H168" t="s">
+        <v>35</v>
+      </c>
+      <c r="I168" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>9</v>
+      </c>
+      <c r="C169">
+        <v>8005264743</v>
+      </c>
+      <c r="D169" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E169" t="s">
+        <v>10</v>
+      </c>
+      <c r="F169" t="s">
+        <v>11</v>
+      </c>
+      <c r="G169" t="s">
+        <v>232</v>
+      </c>
+      <c r="H169" t="s">
+        <v>35</v>
+      </c>
+      <c r="I169" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>61</v>
+      </c>
+      <c r="C170">
+        <v>8005260738</v>
+      </c>
+      <c r="D170" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E170" t="s">
+        <v>44</v>
+      </c>
+      <c r="F170" t="s">
+        <v>16</v>
+      </c>
+      <c r="G170" t="s">
+        <v>233</v>
+      </c>
+      <c r="H170" t="s">
+        <v>35</v>
+      </c>
+      <c r="I170" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>9</v>
+      </c>
+      <c r="C171">
+        <v>8005251414</v>
+      </c>
+      <c r="D171" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E171" t="s">
+        <v>23</v>
+      </c>
+      <c r="F171" t="s">
+        <v>11</v>
+      </c>
+      <c r="G171" t="s">
+        <v>234</v>
+      </c>
+      <c r="H171" t="s">
+        <v>13</v>
+      </c>
+      <c r="I171" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172">
+        <v>8005268202</v>
+      </c>
+      <c r="D172" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E172" t="s">
+        <v>27</v>
+      </c>
+      <c r="F172" t="s">
+        <v>16</v>
+      </c>
+      <c r="G172" t="s">
+        <v>235</v>
+      </c>
+      <c r="H172" t="s">
+        <v>35</v>
+      </c>
+      <c r="I172" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>9</v>
+      </c>
+      <c r="C173">
+        <v>8005242403</v>
+      </c>
+      <c r="D173" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E173" t="s">
+        <v>68</v>
+      </c>
+      <c r="F173" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" t="s">
+        <v>236</v>
+      </c>
+      <c r="H173" t="s">
+        <v>18</v>
+      </c>
+      <c r="I173" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>61</v>
+      </c>
+      <c r="C174">
+        <v>8005252879</v>
+      </c>
+      <c r="D174" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E174" t="s">
+        <v>23</v>
+      </c>
+      <c r="F174" t="s">
+        <v>16</v>
+      </c>
+      <c r="G174" t="s">
+        <v>237</v>
+      </c>
+      <c r="H174" t="s">
+        <v>63</v>
+      </c>
+      <c r="I174" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175">
+        <v>8005252367</v>
+      </c>
+      <c r="D175" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E175" t="s">
+        <v>49</v>
+      </c>
+      <c r="F175" t="s">
+        <v>16</v>
+      </c>
+      <c r="G175" t="s">
+        <v>238</v>
+      </c>
+      <c r="H175" t="s">
+        <v>18</v>
+      </c>
+      <c r="I175" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176">
+        <v>8005270235</v>
+      </c>
+      <c r="D176" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E176" t="s">
+        <v>23</v>
+      </c>
+      <c r="F176" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" t="s">
+        <v>239</v>
+      </c>
+      <c r="H176" t="s">
+        <v>18</v>
+      </c>
+      <c r="I176" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 21/01/2026 11:34:03,20
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dash/NPSMedalliaequaltricsculligan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboard/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{669CBFB8-0322-4578-9E67-E4E6A92CABAA}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39259433-E5F1-45C5-838B-A00394B33620}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="269">
   <si>
     <t>ID</t>
   </si>
@@ -805,6 +805,93 @@
   </si>
   <si>
     <t>Não fez a manutenção em todos os bebedouros necessários</t>
+  </si>
+  <si>
+    <t>Tecnico chegou num horário diferente do agendado. Eu estava de saida para outro compromisso e me atrasou. Sugiro que os agendamentos sejam cumpridos conforme o cliente demanda.</t>
+  </si>
+  <si>
+    <t>O técnico não compareceu. Não houve visita. Essa é a terceira vez seguida que acontece isso. Extremamente insatisfeito</t>
+  </si>
+  <si>
+    <t>Muito ruim. O instalador chegou de manhã mesmo combinando a tarde. Tocou o interfone e acordou minha mae de 85 anos. E deixou um serviço porco. Fio aparecendo.  Péssimo.  Uma vergonha</t>
+  </si>
+  <si>
+    <t>Houve demora para manutenção. O fluxo de água do meu aparelho é baixo.</t>
+  </si>
+  <si>
+    <t>Vazão/pressão da água</t>
+  </si>
+  <si>
+    <t>Pela quarta vez foi agendada a manutenção e o técnico não veio. Não há como avaliar algo que não aconteceu Inclusive solicito que verifiquem minha situação, pois é quarto agendamento que o técnico não vem e não recebi nenhuma explicação</t>
+  </si>
+  <si>
+    <t>Já fiz duas chamadas de técnico e não apareceu! Fico esperando, perdendo trabalho e A Brastemp não apareceu</t>
+  </si>
+  <si>
+    <t>Mais uma vez o técnico não veio . Estou exausta de reclamar. Já liguei, tentei cancelar . A atendente conseguiu baixar minha parcela, porém ainda com problemas em vir aqui e trocar o filtro. Já faltei trabalho, já deixei de ir a tratamentos médicos . Mas eu tenho compromisso. Nem satisfação me dão. Ou…. Chegam aqui em horários que eu não estou. Simplesmente assim.  Se eu deixasse de pagar, provavelmente muito rapidamente me cobrariam. Mas como eu pago em dia me tratam assim. Sinceramente .</t>
+  </si>
+  <si>
+    <t>Fiz a reclamação de nao terem feito a instalação do gas para agua, ficaram de vir no sabado no horário da manhã e de novo ninguem apareceu. Estou achando pessimo pq quis locar por conta da agua com gas e até agora nao tenho.</t>
+  </si>
+  <si>
+    <t>Caro, só reduz o preço depois da minha reclamação.Precisa mandar um lembrete um dia antes da manutençãoA forma de agendamento é irritante. Podia ser um whats. É horrível receber q ligação</t>
+  </si>
+  <si>
+    <t>_ Estou pedindo a visita do técnico para trocar o filtro do meu purificador e ele nunca vem. Tenho vários protocolos de pedido, e ninguém aparece:05/11/25 - Na parte da Tarde - entre 13:00 e 18:00hs - Ninguém apareceu Ordem de Serviço - N° 800519025016/01/26 - Na parte da Tarde - entre 13:00 e 18:00hs - Ninguém apareceu Ordem de Serviço - N° 8005190250Falta de profissionalismo, pessoal descompromissadoPago em dia as mensalidades do Purificador BRASTEMP, porém a Empresa não consegue fazer as manutenções no período combinado.</t>
+  </si>
+  <si>
+    <t>O serviço do suporte não atendeu minhas expectativas</t>
+  </si>
+  <si>
+    <t>Mais de 20 dias sem água gelada e a Brastemp não está  nem aí com o consumidor, mesmo ele sendo assinante mais de 10 anos. Uma vergonha.</t>
+  </si>
+  <si>
+    <t>Técnico não veio e não deu satisfação.</t>
+  </si>
+  <si>
+    <t>Não estou gostando, o problema sempre volta.O técnico saiu e o problema persistiu e ficou dando choque. Agora é que não quero mais.Quero entregar o aparelho e findar o meu aluguel.</t>
+  </si>
+  <si>
+    <t>Mais uma vez.. agendaram e não vieram</t>
+  </si>
+  <si>
+    <t>O problema não foi resolvido.</t>
+  </si>
+  <si>
+    <t>A disponibilidade de uma visita próxima foi ruim, passei quase 3 semanas com O purificador com cheiro e gosto ruim, porque não tinham disponibilidade antes.</t>
+  </si>
+  <si>
+    <t>Não houve visita tecnica</t>
+  </si>
+  <si>
+    <t>Não tive visita , o técnico não veio , estou muito insatisfeita , segunda vez agendo e nada</t>
+  </si>
+  <si>
+    <t>Na minha opinião o filtro deverá ser trocada semestralmente, principalmente pela qualidade d'água Sabesp tem piorado e muito, isso naturalmente exige mais do filtro e a cada 6 meses o técnico vem e diz que a agua esta bom, e quando peço para trocar eles não carregam esse filtro adicional, tenho que solicitar para dizer que a agua não esta boa mesmo. Acabo comprando agua no supermercado, porque além do cheiro desagradável apresenta coloração.</t>
+  </si>
+  <si>
+    <t>Não funcionou na instalação, solicitei novamente o técnico e o mesmo não veio.</t>
+  </si>
+  <si>
+    <t>O técnico não compareceu!</t>
+  </si>
+  <si>
+    <t>O técnico sugeriu, pela segunda vez, não trocar o filtro. Devido a nossa insistência, uma vez que na visita anterior a troca não foi feita, ele realizou a troca. Ou seja, qual é o critério técnico desta visita técnica? Talvez eu seja um dos clientes mais antigos do Purificador Brastemp, pela primeira vez, estou em dúvida sobre a qualidade do serviço.</t>
+  </si>
+  <si>
+    <t>Não foi feito o combinado em instalar o MIB geo</t>
+  </si>
+  <si>
+    <t>Muito simples a limpeza, nem ao menos um produtos tipo para desinfetar o filtro todo após o manuseio.</t>
+  </si>
+  <si>
+    <t>Não houve a visita.</t>
+  </si>
+  <si>
+    <t>FRQ_ECO_RS_PORTO ALEGRE_2</t>
+  </si>
+  <si>
+    <t>depois de 5 agendamentos e muitas ligações ocorreu o serviço</t>
   </si>
 </sst>
 </file>
@@ -1171,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I176"/>
+  <dimension ref="A1:I203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101:J176"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177:I203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6294,6 +6381,789 @@
         <v>51</v>
       </c>
     </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177">
+        <v>8005258758</v>
+      </c>
+      <c r="D177" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E177" t="s">
+        <v>53</v>
+      </c>
+      <c r="F177" t="s">
+        <v>16</v>
+      </c>
+      <c r="G177" t="s">
+        <v>240</v>
+      </c>
+      <c r="H177" t="s">
+        <v>18</v>
+      </c>
+      <c r="I177" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178">
+        <v>8005224647</v>
+      </c>
+      <c r="D178" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E178" t="s">
+        <v>53</v>
+      </c>
+      <c r="F178" t="s">
+        <v>16</v>
+      </c>
+      <c r="G178" t="s">
+        <v>241</v>
+      </c>
+      <c r="H178" t="s">
+        <v>18</v>
+      </c>
+      <c r="I178" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>61</v>
+      </c>
+      <c r="C179">
+        <v>8005267106</v>
+      </c>
+      <c r="D179" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E179" t="s">
+        <v>44</v>
+      </c>
+      <c r="F179" t="s">
+        <v>16</v>
+      </c>
+      <c r="G179" t="s">
+        <v>242</v>
+      </c>
+      <c r="H179" t="s">
+        <v>18</v>
+      </c>
+      <c r="I179" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180">
+        <v>8005234424</v>
+      </c>
+      <c r="D180" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E180" t="s">
+        <v>27</v>
+      </c>
+      <c r="F180" t="s">
+        <v>16</v>
+      </c>
+      <c r="G180" t="s">
+        <v>243</v>
+      </c>
+      <c r="H180" t="s">
+        <v>35</v>
+      </c>
+      <c r="I180" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181">
+        <v>8005271095</v>
+      </c>
+      <c r="D181" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E181" t="s">
+        <v>53</v>
+      </c>
+      <c r="F181" t="s">
+        <v>16</v>
+      </c>
+      <c r="G181" t="s">
+        <v>245</v>
+      </c>
+      <c r="H181" t="s">
+        <v>18</v>
+      </c>
+      <c r="I181" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>8005260391</v>
+      </c>
+      <c r="D182" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E182" t="s">
+        <v>53</v>
+      </c>
+      <c r="F182" t="s">
+        <v>16</v>
+      </c>
+      <c r="G182" t="s">
+        <v>246</v>
+      </c>
+      <c r="H182" t="s">
+        <v>18</v>
+      </c>
+      <c r="I182" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>9</v>
+      </c>
+      <c r="C183">
+        <v>8005218070</v>
+      </c>
+      <c r="D183" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E183" t="s">
+        <v>53</v>
+      </c>
+      <c r="F183" t="s">
+        <v>16</v>
+      </c>
+      <c r="G183" t="s">
+        <v>247</v>
+      </c>
+      <c r="H183" t="s">
+        <v>18</v>
+      </c>
+      <c r="I183" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184">
+        <v>8005267385</v>
+      </c>
+      <c r="D184" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E184" t="s">
+        <v>53</v>
+      </c>
+      <c r="F184" t="s">
+        <v>16</v>
+      </c>
+      <c r="G184" t="s">
+        <v>248</v>
+      </c>
+      <c r="H184" t="s">
+        <v>18</v>
+      </c>
+      <c r="I184" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>8005247512</v>
+      </c>
+      <c r="D185" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E185" t="s">
+        <v>20</v>
+      </c>
+      <c r="F185" t="s">
+        <v>11</v>
+      </c>
+      <c r="G185" t="s">
+        <v>249</v>
+      </c>
+      <c r="H185" t="s">
+        <v>13</v>
+      </c>
+      <c r="I185" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>9</v>
+      </c>
+      <c r="C186">
+        <v>8005190250</v>
+      </c>
+      <c r="D186" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E186" t="s">
+        <v>53</v>
+      </c>
+      <c r="F186" t="s">
+        <v>16</v>
+      </c>
+      <c r="G186" t="s">
+        <v>250</v>
+      </c>
+      <c r="H186" t="s">
+        <v>18</v>
+      </c>
+      <c r="I186" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187">
+        <v>8005267277</v>
+      </c>
+      <c r="D187" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E187" t="s">
+        <v>23</v>
+      </c>
+      <c r="F187" t="s">
+        <v>16</v>
+      </c>
+      <c r="G187" t="s">
+        <v>251</v>
+      </c>
+      <c r="H187" t="s">
+        <v>13</v>
+      </c>
+      <c r="I187" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>9</v>
+      </c>
+      <c r="C188">
+        <v>8005262536</v>
+      </c>
+      <c r="D188" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E188" t="s">
+        <v>53</v>
+      </c>
+      <c r="F188" t="s">
+        <v>16</v>
+      </c>
+      <c r="G188" t="s">
+        <v>252</v>
+      </c>
+      <c r="H188" t="s">
+        <v>32</v>
+      </c>
+      <c r="I188" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>9</v>
+      </c>
+      <c r="C189">
+        <v>8005263939</v>
+      </c>
+      <c r="D189" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E189" t="s">
+        <v>53</v>
+      </c>
+      <c r="F189" t="s">
+        <v>16</v>
+      </c>
+      <c r="G189" t="s">
+        <v>253</v>
+      </c>
+      <c r="H189" t="s">
+        <v>18</v>
+      </c>
+      <c r="I189" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190">
+        <v>8005238421</v>
+      </c>
+      <c r="D190" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E190" t="s">
+        <v>65</v>
+      </c>
+      <c r="F190" t="s">
+        <v>16</v>
+      </c>
+      <c r="G190" t="s">
+        <v>254</v>
+      </c>
+      <c r="H190" t="s">
+        <v>18</v>
+      </c>
+      <c r="I190" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
+        <v>9</v>
+      </c>
+      <c r="C191">
+        <v>8005266918</v>
+      </c>
+      <c r="D191" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E191" t="s">
+        <v>53</v>
+      </c>
+      <c r="F191" t="s">
+        <v>16</v>
+      </c>
+      <c r="G191" t="s">
+        <v>255</v>
+      </c>
+      <c r="H191" t="s">
+        <v>18</v>
+      </c>
+      <c r="I191" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
+        <v>9</v>
+      </c>
+      <c r="C192">
+        <v>8005273027</v>
+      </c>
+      <c r="D192" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E192" t="s">
+        <v>53</v>
+      </c>
+      <c r="F192" t="s">
+        <v>16</v>
+      </c>
+      <c r="G192" t="s">
+        <v>256</v>
+      </c>
+      <c r="H192" t="s">
+        <v>18</v>
+      </c>
+      <c r="I192" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193">
+        <v>8005251083</v>
+      </c>
+      <c r="D193" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E193" t="s">
+        <v>20</v>
+      </c>
+      <c r="F193" t="s">
+        <v>11</v>
+      </c>
+      <c r="G193" t="s">
+        <v>257</v>
+      </c>
+      <c r="H193" t="s">
+        <v>32</v>
+      </c>
+      <c r="I193" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>9</v>
+      </c>
+      <c r="C194">
+        <v>8005248857</v>
+      </c>
+      <c r="D194" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E194" t="s">
+        <v>53</v>
+      </c>
+      <c r="F194" t="s">
+        <v>16</v>
+      </c>
+      <c r="G194" t="s">
+        <v>258</v>
+      </c>
+      <c r="H194" t="s">
+        <v>18</v>
+      </c>
+      <c r="I194" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195">
+        <v>8005207126</v>
+      </c>
+      <c r="D195" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E195" t="s">
+        <v>53</v>
+      </c>
+      <c r="F195" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" t="s">
+        <v>259</v>
+      </c>
+      <c r="H195" t="s">
+        <v>18</v>
+      </c>
+      <c r="I195" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>9</v>
+      </c>
+      <c r="C196">
+        <v>8005267788</v>
+      </c>
+      <c r="D196" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E196" t="s">
+        <v>23</v>
+      </c>
+      <c r="F196" t="s">
+        <v>11</v>
+      </c>
+      <c r="G196" t="s">
+        <v>260</v>
+      </c>
+      <c r="H196" t="s">
+        <v>18</v>
+      </c>
+      <c r="I196" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>61</v>
+      </c>
+      <c r="C197">
+        <v>8005262682</v>
+      </c>
+      <c r="D197" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E197" t="s">
+        <v>27</v>
+      </c>
+      <c r="F197" t="s">
+        <v>16</v>
+      </c>
+      <c r="G197" t="s">
+        <v>261</v>
+      </c>
+      <c r="H197" t="s">
+        <v>18</v>
+      </c>
+      <c r="I197" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>9</v>
+      </c>
+      <c r="C198">
+        <v>8005261464</v>
+      </c>
+      <c r="D198" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E198" t="s">
+        <v>53</v>
+      </c>
+      <c r="F198" t="s">
+        <v>16</v>
+      </c>
+      <c r="G198" t="s">
+        <v>262</v>
+      </c>
+      <c r="H198" t="s">
+        <v>18</v>
+      </c>
+      <c r="I198" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>9</v>
+      </c>
+      <c r="C199">
+        <v>8005250369</v>
+      </c>
+      <c r="D199" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E199" t="s">
+        <v>20</v>
+      </c>
+      <c r="F199" t="s">
+        <v>16</v>
+      </c>
+      <c r="G199" t="s">
+        <v>263</v>
+      </c>
+      <c r="H199" t="s">
+        <v>18</v>
+      </c>
+      <c r="I199" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>9</v>
+      </c>
+      <c r="C200">
+        <v>8005243013</v>
+      </c>
+      <c r="D200" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E200" t="s">
+        <v>27</v>
+      </c>
+      <c r="F200" t="s">
+        <v>16</v>
+      </c>
+      <c r="G200" t="s">
+        <v>264</v>
+      </c>
+      <c r="H200" t="s">
+        <v>18</v>
+      </c>
+      <c r="I200" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>9</v>
+      </c>
+      <c r="C201">
+        <v>8005250128</v>
+      </c>
+      <c r="D201" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E201" t="s">
+        <v>20</v>
+      </c>
+      <c r="F201" t="s">
+        <v>16</v>
+      </c>
+      <c r="G201" t="s">
+        <v>265</v>
+      </c>
+      <c r="H201" t="s">
+        <v>18</v>
+      </c>
+      <c r="I201" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202">
+        <v>8005257348</v>
+      </c>
+      <c r="D202" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E202" t="s">
+        <v>53</v>
+      </c>
+      <c r="F202" t="s">
+        <v>16</v>
+      </c>
+      <c r="G202" t="s">
+        <v>266</v>
+      </c>
+      <c r="H202" t="s">
+        <v>18</v>
+      </c>
+      <c r="I202" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>9</v>
+      </c>
+      <c r="C203">
+        <v>8005250948</v>
+      </c>
+      <c r="D203" s="3">
+        <v>46023</v>
+      </c>
+      <c r="E203" t="s">
+        <v>267</v>
+      </c>
+      <c r="F203" t="s">
+        <v>16</v>
+      </c>
+      <c r="G203" t="s">
+        <v>268</v>
+      </c>
+      <c r="H203" t="s">
+        <v>32</v>
+      </c>
+      <c r="I203" t="s">
+        <v>182</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 03/02/2026 16:33:02,33
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{061A67B0-78B6-406F-B243-914D3B615D7D}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B511601-214E-4930-BC7D-308330A93810}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="391">
   <si>
     <t>ID</t>
   </si>
@@ -1129,6 +1129,153 @@
   </si>
   <si>
     <t>Pedi um reparo e somente no 3o agendamento o tecnico apareceu. Estou achando muito caro para uma manutenção semestral. Quero cancelar o plano, basta parar de pagar?</t>
+  </si>
+  <si>
+    <t>a visita foi boa mas tenho tentado contato com voces porque a tecnica recomendou a substituicao do filtro e nao consigo retorno</t>
+  </si>
+  <si>
+    <t>Marcam visita e não aparecem. Vc pede para trocar o filtro e precisa pagar! Estou com defeito no meu aparelho e até agora não veio ninguém! Agendei por duas vezes</t>
+  </si>
+  <si>
+    <t>Costuma dar algumas falhas</t>
+  </si>
+  <si>
+    <t>Estamos aguardando a troca do aparelho pois todo o tempo que estamos com ele ele não funciona, já pedimos a troca do aparelho em maio de 2025 e não foi trocado e agora pedimos a subustituicap do aparelho para o convencional e estamos aguardando essa troca</t>
+  </si>
+  <si>
+    <t>É satisfatório a qualidade do purificador e o serviço de assistência técnica. O valor da mensalidade é meio desestimulante.</t>
+  </si>
+  <si>
+    <t>Excelente, tenho há muitos anos. Porém agora o agendamento está demorando muito</t>
+  </si>
+  <si>
+    <t>Data Distante</t>
+  </si>
+  <si>
+    <t>Depois da visita no dia 05.01.2026 o filtro apresentou um problema no dia 26.
+O tecnico que nos visitou informou que nenhuma limpeza havia sido feita ate entao.
+Apesar de eu ja ter reportado redução do fluxo de agua ninguem fez nada.
+O tecnico trocou o filtro e mais alguns sensores eletronicos, e o filtro voltou a funcionar da mesma maneira, ou seja ainda esta com o fluxo baixo.
+Infelizmente deixou muito a desejar.</t>
+  </si>
+  <si>
+    <t>O tecnico nao apareceu</t>
+  </si>
+  <si>
+    <t>O único problema que tenho para relatar é o horário de chegada do técnico. Conforme agendado, estávamos esperando o técnico a partir das 13 h. Ele veio antes, por volta da 12 h que é o pico de atendimento da cozinha de nossa escola. Gostaríamos que fosse no horário agendado, digo, das 13 h às 18 h. Do resto tudo perfeito !</t>
+  </si>
+  <si>
+    <t>Experiência boa e satisfatória, porém o preço está muito alto.</t>
+  </si>
+  <si>
+    <t>A pessoa não veio.</t>
+  </si>
+  <si>
+    <t>boa</t>
+  </si>
+  <si>
+    <t>Da outra vez marcaram e ninguem apareceu e nem deu satisfaçao
+Desta vez foi tudo bem</t>
+  </si>
+  <si>
+    <t>Depois de um mês de espera, foi agendada a troca do purificador que não ocorreu. Agendada a troca pela segunda vez, foi instalado o purificador, porém a água está com gosto estranho e o controle de volume de água não está funcionando. Quero cancelar minha assinatura do purificador.</t>
+  </si>
+  <si>
+    <t>Ultimamente a Brastemp não comparece na data agendada para a manutenção da limpeza do filtro.
+Fico aguardando e não recebo nenhuma satisfação.
+É preciso reagendar e espero mais um mês.
+Sou profissional autônoma, o que me leva a cancelar meus compromissos no período que fico aguardando a Brastemp.
+Tenho prejuízo financeiro.</t>
+  </si>
+  <si>
+    <t>Demorou 4 dias para consertar e eu pagando água mineral</t>
+  </si>
+  <si>
+    <t>Mais uma vez o agendamento não foi cumprido.</t>
+  </si>
+  <si>
+    <t>Tecnico beinem casa e não resolveu o problema.</t>
+  </si>
+  <si>
+    <t>Não tive visita nenhuma, estou a meses solicitando um técnico e nada!! Tive q fazer mudança de endereço e paguei particular a instalação, vcs não me deram nenhuma atenção. Várias atendentes ligam e não conseguem nem mudar meu endereço. Atendimento péssimo</t>
+  </si>
+  <si>
+    <t>Marcaram pro sábado de manhã e o técnico veio na sexta à tarde. Por sorte eu estava em casa.</t>
+  </si>
+  <si>
+    <t>O técnico nao apareceu bao deu satisfação e continuo sem água no filtro que está com defeito. Muita insatisfeito.</t>
+  </si>
+  <si>
+    <t>O purificador não está funcionando e já faz um mês que não consigo resolver o problema.</t>
+  </si>
+  <si>
+    <t>Vcs estão fazendo a maior bagunça com essas marcações por secretária eletrônica.
+Chegou um rapaz aqui na semana passada na minha casa em Piratininga para fazer manutenção em meu filtro da casa.Nao deixei entrar porquê o que marquei foi para essa semana na próxima quinta feira no meu apartamento em Icaraí.
+Tenho 2 assinaturas e vcs fazem a maior confusão na hora de mandarem o técnico .
+Fico mal assistida nas duas</t>
+  </si>
+  <si>
+    <t>Infelizmente foi instalado com defeito sem funcionar o gelo liguei para consertar e mudar de lugar não pode fazer as duas solicitações então optei por mudar de lugar e depois vou pedir para consertar infelizmente muita burocracia</t>
+  </si>
+  <si>
+    <t>Estão demorando muito para trocar o sensor que tem gerado o congelamento do filtro.
+Estou sem usá-lo a quase três semanas</t>
+  </si>
+  <si>
+    <t>O Rapaz veio instalar o pressurizador e segundo ele veio a peça errada, ligou para uma pessoa para falar sobre, ficou de voltar no dia seguinte para instalar a peça correta e até hoje não retornou.</t>
+  </si>
+  <si>
+    <t>O técnico solicitou a troca do aparelho. Pois o mesmo ainda não se encontra funcionando.</t>
+  </si>
+  <si>
+    <t>Não posso utilizar. A água tem um gosto de óleo químico</t>
+  </si>
+  <si>
+    <t>Tenho o purificador desde 2014 ,houve um problema no filtro , pois este perdeu a validade fazendo com que a água ficasse com mal cheiro e gosto desagradável. Diante do exposto solicitei um técnico com urgência pois tenho criança mas infelizmente levei mais de 15 dias para um técnico trocasse o mesmo.</t>
+  </si>
+  <si>
+    <t>Péssimo atendimento, estou extremamente decepcionado, sou cliente a mais de 15 anos e estou tendo uma dificuldade enorme para ter o meu filtro operacional novamente. Primeiramente a demora em conseguir uma visita técnica, mesmo assim aguardamos, porém o técnico veio, não deu o laudo condenando o filtro (não está gelando a água a mais de duas semanas), o técnico efetuou alguma manutenção mal feita e foi embora do local dizendo que em 20 minutos estaria gelando, porém isso não aconteceu, o filtro continua sem gelar. Pagamos por um serviço que não está sendo entregue. Já ligamos novamente e só tem data para uma nova visita para daqui a uma semana!!!</t>
+  </si>
+  <si>
+    <t>Não respondem e-mails, agendamentos errados.
+Estamos com equipamento parado a meses.  Solicitamos o contato do nosso gerente de conta e não tivemos retorno,  gostaríamos de mais informações sobre o equipamento de água gaseificada.  Mas a Brastemp parece que não quer vender serviços</t>
+  </si>
+  <si>
+    <t>Precisei ligar para fazer agendamento sendo que cada semestre a própria Brastemp marcava o agendamento</t>
+  </si>
+  <si>
+    <t>a demora mais de um mês para o técnico trocar um filtro.
+sem cabimento não demorou 10 minutos.
+péssimo atendimento.</t>
+  </si>
+  <si>
+    <t>Gosto muito do filtro da Brastemp, mas ultimamente as visitas emergenciais por algum problema  no aparelho demoram muito. Cheguei a ficar 1 mês sem filtro, o mesmo estava com a água quente, ontem 02/02 o técnico foi muito atencioso e trocou o sensor, gostaria de uma atendimento mais eficaz porque pago mensalmente sempre sem dever nada a empresa, gostaria de ser tratada da mesma forma.</t>
+  </si>
+  <si>
+    <t>Sou cliente a mais de 10 anos e pasmem, até hj continuo c o mesmo aparelho, que já apresentou problemas de aquecimento varias vezes e a desculpa a cd manutenção é a mesma, troca-se uma peça e aguarde pois estaremos solicitando a troca do aparelho, até pq em 10 anos já sairam inúmeras versões certamente + modernas, eficazes ... já avisei que irei fz o cancelamento, o antepenúltimo técnico que esteve fz a manutenção ficou p um bom tempo em ligação confirmando que seria trocado o aparelho e passado 1 ano, continuo na mesma ...o filtro foi trocado pouquissimas vezes e qual garantia temos que está sendo benéfico? o teste do copo???? caso n seja trocado o aparelho, estarei procedendo ao cancelamento.</t>
+  </si>
+  <si>
+    <t>O técnico fez duas visitas e não resolveu o problema</t>
+  </si>
+  <si>
+    <t>O único senão é  que quando falta luz ele não funciona. A manutenção dele foi negligenciada pois desde 2023 não  recebi aviso que estava na hora da manutenção.  Vieram agora para cessar o vazamento mas a vistoria,  manutenção  nada foi feito.</t>
+  </si>
+  <si>
+    <t>Foi muito bom ,só que marquei a tarde e foi cedo</t>
+  </si>
+  <si>
+    <t>Meu filtro continua sem funcionar desde o dia da instalação!!!! Solicito troca imediata do equipamento.</t>
+  </si>
+  <si>
+    <t>Tenho a assinatura ininterrupta há mais de 22 anos, ou seja, desde o início desse serviço aqui em Campinas.
+Esta última manutenção foi feita de maneira muito rápida, parecendo não se atentar para todos os itens protocolares.
+O preço da assinatura está muito alto, pelo que reinvidico desconto, tendo em vista a fidelização!</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>A visita não resolveu meu problema, é preciso mudar o aparelho.</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I286"/>
+  <dimension ref="A1:I328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H292" sqref="H292"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287:I328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9810,6 +9957,1224 @@
         <v>29</v>
       </c>
     </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>286</v>
+      </c>
+      <c r="B287" t="s">
+        <v>9</v>
+      </c>
+      <c r="C287">
+        <v>8005274938</v>
+      </c>
+      <c r="D287" s="3">
+        <v>46052.493726851862</v>
+      </c>
+      <c r="E287" t="s">
+        <v>20</v>
+      </c>
+      <c r="F287" t="s">
+        <v>16</v>
+      </c>
+      <c r="G287" t="s">
+        <v>348</v>
+      </c>
+      <c r="H287" t="s">
+        <v>35</v>
+      </c>
+      <c r="I287" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>287</v>
+      </c>
+      <c r="B288" t="s">
+        <v>9</v>
+      </c>
+      <c r="C288">
+        <v>8005266618</v>
+      </c>
+      <c r="D288" s="3">
+        <v>46052.501435185193</v>
+      </c>
+      <c r="E288" t="s">
+        <v>27</v>
+      </c>
+      <c r="F288" t="s">
+        <v>16</v>
+      </c>
+      <c r="G288" t="s">
+        <v>349</v>
+      </c>
+      <c r="H288" t="s">
+        <v>18</v>
+      </c>
+      <c r="I288" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>288</v>
+      </c>
+      <c r="B289" t="s">
+        <v>9</v>
+      </c>
+      <c r="C289">
+        <v>8005265640</v>
+      </c>
+      <c r="D289" s="3">
+        <v>46052.510208333333</v>
+      </c>
+      <c r="E289" t="s">
+        <v>23</v>
+      </c>
+      <c r="F289" t="s">
+        <v>11</v>
+      </c>
+      <c r="G289" t="s">
+        <v>350</v>
+      </c>
+      <c r="H289" t="s">
+        <v>35</v>
+      </c>
+      <c r="I289" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>289</v>
+      </c>
+      <c r="B290" t="s">
+        <v>9</v>
+      </c>
+      <c r="C290">
+        <v>8005260783</v>
+      </c>
+      <c r="D290" s="3">
+        <v>46052.518680555557</v>
+      </c>
+      <c r="E290" t="s">
+        <v>23</v>
+      </c>
+      <c r="F290" t="s">
+        <v>16</v>
+      </c>
+      <c r="G290" t="s">
+        <v>351</v>
+      </c>
+      <c r="H290" t="s">
+        <v>35</v>
+      </c>
+      <c r="I290" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>290</v>
+      </c>
+      <c r="B291" t="s">
+        <v>9</v>
+      </c>
+      <c r="C291">
+        <v>8005259067</v>
+      </c>
+      <c r="D291" s="3">
+        <v>46052.547754629632</v>
+      </c>
+      <c r="E291" t="s">
+        <v>20</v>
+      </c>
+      <c r="F291" t="s">
+        <v>11</v>
+      </c>
+      <c r="G291" t="s">
+        <v>352</v>
+      </c>
+      <c r="H291" t="s">
+        <v>13</v>
+      </c>
+      <c r="I291" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>291</v>
+      </c>
+      <c r="B292" t="s">
+        <v>9</v>
+      </c>
+      <c r="C292">
+        <v>8005265612</v>
+      </c>
+      <c r="D292" s="3">
+        <v>46052.554444444453</v>
+      </c>
+      <c r="E292" t="s">
+        <v>27</v>
+      </c>
+      <c r="F292" t="s">
+        <v>16</v>
+      </c>
+      <c r="G292" t="s">
+        <v>353</v>
+      </c>
+      <c r="H292" t="s">
+        <v>32</v>
+      </c>
+      <c r="I292" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>292</v>
+      </c>
+      <c r="B293" t="s">
+        <v>9</v>
+      </c>
+      <c r="C293">
+        <v>8005283885</v>
+      </c>
+      <c r="D293" s="3">
+        <v>46052.573472222219</v>
+      </c>
+      <c r="E293" t="s">
+        <v>15</v>
+      </c>
+      <c r="F293" t="s">
+        <v>16</v>
+      </c>
+      <c r="G293" t="s">
+        <v>355</v>
+      </c>
+      <c r="H293" t="s">
+        <v>35</v>
+      </c>
+      <c r="I293" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>293</v>
+      </c>
+      <c r="B294" t="s">
+        <v>9</v>
+      </c>
+      <c r="C294">
+        <v>8005274068</v>
+      </c>
+      <c r="D294" s="3">
+        <v>46052.574293981481</v>
+      </c>
+      <c r="E294" t="s">
+        <v>20</v>
+      </c>
+      <c r="F294" t="s">
+        <v>16</v>
+      </c>
+      <c r="G294" t="s">
+        <v>356</v>
+      </c>
+      <c r="H294" t="s">
+        <v>18</v>
+      </c>
+      <c r="I294" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>294</v>
+      </c>
+      <c r="B295" t="s">
+        <v>9</v>
+      </c>
+      <c r="C295">
+        <v>8005283397</v>
+      </c>
+      <c r="D295" s="3">
+        <v>46052.64603009259</v>
+      </c>
+      <c r="E295" t="s">
+        <v>20</v>
+      </c>
+      <c r="F295" t="s">
+        <v>11</v>
+      </c>
+      <c r="G295" t="s">
+        <v>357</v>
+      </c>
+      <c r="H295" t="s">
+        <v>18</v>
+      </c>
+      <c r="I295" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>295</v>
+      </c>
+      <c r="B296" t="s">
+        <v>9</v>
+      </c>
+      <c r="C296">
+        <v>8005278837</v>
+      </c>
+      <c r="D296" s="3">
+        <v>46052.827280092592</v>
+      </c>
+      <c r="E296" t="s">
+        <v>15</v>
+      </c>
+      <c r="F296" t="s">
+        <v>11</v>
+      </c>
+      <c r="G296" t="s">
+        <v>358</v>
+      </c>
+      <c r="H296" t="s">
+        <v>13</v>
+      </c>
+      <c r="I296" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>296</v>
+      </c>
+      <c r="B297" t="s">
+        <v>9</v>
+      </c>
+      <c r="C297">
+        <v>8005279298</v>
+      </c>
+      <c r="D297" s="3">
+        <v>46053.400891203702</v>
+      </c>
+      <c r="E297" t="s">
+        <v>53</v>
+      </c>
+      <c r="F297" t="s">
+        <v>16</v>
+      </c>
+      <c r="G297" t="s">
+        <v>359</v>
+      </c>
+      <c r="H297" t="s">
+        <v>18</v>
+      </c>
+      <c r="I297" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>297</v>
+      </c>
+      <c r="B298" t="s">
+        <v>9</v>
+      </c>
+      <c r="C298">
+        <v>8005265467</v>
+      </c>
+      <c r="D298" s="3">
+        <v>46053.435358796298</v>
+      </c>
+      <c r="E298" t="s">
+        <v>23</v>
+      </c>
+      <c r="F298" t="s">
+        <v>11</v>
+      </c>
+      <c r="G298" t="s">
+        <v>360</v>
+      </c>
+      <c r="H298" t="s">
+        <v>13</v>
+      </c>
+      <c r="I298" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>298</v>
+      </c>
+      <c r="B299" t="s">
+        <v>9</v>
+      </c>
+      <c r="C299">
+        <v>8005245207</v>
+      </c>
+      <c r="D299" s="3">
+        <v>46053.436574074083</v>
+      </c>
+      <c r="E299" t="s">
+        <v>20</v>
+      </c>
+      <c r="F299" t="s">
+        <v>11</v>
+      </c>
+      <c r="G299" t="s">
+        <v>361</v>
+      </c>
+      <c r="H299" t="s">
+        <v>18</v>
+      </c>
+      <c r="I299" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>9</v>
+      </c>
+      <c r="C300">
+        <v>8005253746</v>
+      </c>
+      <c r="D300" s="3">
+        <v>46053.854456018518</v>
+      </c>
+      <c r="E300" t="s">
+        <v>20</v>
+      </c>
+      <c r="F300" t="s">
+        <v>16</v>
+      </c>
+      <c r="G300" t="s">
+        <v>362</v>
+      </c>
+      <c r="H300" t="s">
+        <v>154</v>
+      </c>
+      <c r="I300" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>61</v>
+      </c>
+      <c r="C301">
+        <v>8005256304</v>
+      </c>
+      <c r="D301" s="3">
+        <v>46054.640370370369</v>
+      </c>
+      <c r="E301" t="s">
+        <v>53</v>
+      </c>
+      <c r="F301" t="s">
+        <v>11</v>
+      </c>
+      <c r="G301" t="s">
+        <v>363</v>
+      </c>
+      <c r="H301" t="s">
+        <v>18</v>
+      </c>
+      <c r="I301" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>9</v>
+      </c>
+      <c r="C302">
+        <v>8005280499</v>
+      </c>
+      <c r="D302" s="3">
+        <v>46054.72960648148</v>
+      </c>
+      <c r="E302" t="s">
+        <v>65</v>
+      </c>
+      <c r="F302" t="s">
+        <v>16</v>
+      </c>
+      <c r="G302" t="s">
+        <v>364</v>
+      </c>
+      <c r="H302" t="s">
+        <v>18</v>
+      </c>
+      <c r="I302" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>9</v>
+      </c>
+      <c r="C303">
+        <v>8005282675</v>
+      </c>
+      <c r="D303" s="3">
+        <v>46054.959293981483</v>
+      </c>
+      <c r="E303" t="s">
+        <v>53</v>
+      </c>
+      <c r="F303" t="s">
+        <v>16</v>
+      </c>
+      <c r="G303" t="s">
+        <v>365</v>
+      </c>
+      <c r="H303" t="s">
+        <v>18</v>
+      </c>
+      <c r="I303" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>303</v>
+      </c>
+      <c r="B304" t="s">
+        <v>9</v>
+      </c>
+      <c r="C304">
+        <v>8005277668</v>
+      </c>
+      <c r="D304" s="3">
+        <v>46055.378750000003</v>
+      </c>
+      <c r="E304" t="s">
+        <v>20</v>
+      </c>
+      <c r="F304" t="s">
+        <v>16</v>
+      </c>
+      <c r="G304" t="s">
+        <v>366</v>
+      </c>
+      <c r="H304" t="s">
+        <v>18</v>
+      </c>
+      <c r="I304" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>304</v>
+      </c>
+      <c r="B305" t="s">
+        <v>9</v>
+      </c>
+      <c r="C305">
+        <v>8005258927</v>
+      </c>
+      <c r="D305" s="3">
+        <v>46055.390648148154</v>
+      </c>
+      <c r="E305" t="s">
+        <v>37</v>
+      </c>
+      <c r="F305" t="s">
+        <v>16</v>
+      </c>
+      <c r="G305" t="s">
+        <v>367</v>
+      </c>
+      <c r="H305" t="s">
+        <v>82</v>
+      </c>
+      <c r="I305" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>305</v>
+      </c>
+      <c r="B306" t="s">
+        <v>9</v>
+      </c>
+      <c r="C306">
+        <v>8005211570</v>
+      </c>
+      <c r="D306" s="3">
+        <v>46055.400266203702</v>
+      </c>
+      <c r="E306" t="s">
+        <v>224</v>
+      </c>
+      <c r="F306" t="s">
+        <v>11</v>
+      </c>
+      <c r="G306" t="s">
+        <v>368</v>
+      </c>
+      <c r="H306" t="s">
+        <v>18</v>
+      </c>
+      <c r="I306" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>306</v>
+      </c>
+      <c r="B307" t="s">
+        <v>9</v>
+      </c>
+      <c r="C307">
+        <v>8005285049</v>
+      </c>
+      <c r="D307" s="3">
+        <v>46055.502395833333</v>
+      </c>
+      <c r="E307" t="s">
+        <v>37</v>
+      </c>
+      <c r="F307" t="s">
+        <v>16</v>
+      </c>
+      <c r="G307" t="s">
+        <v>369</v>
+      </c>
+      <c r="H307" t="s">
+        <v>18</v>
+      </c>
+      <c r="I307" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>307</v>
+      </c>
+      <c r="B308" t="s">
+        <v>9</v>
+      </c>
+      <c r="C308">
+        <v>8005281526</v>
+      </c>
+      <c r="D308" s="3">
+        <v>46055.511180555557</v>
+      </c>
+      <c r="E308" t="s">
+        <v>20</v>
+      </c>
+      <c r="F308" t="s">
+        <v>16</v>
+      </c>
+      <c r="G308" t="s">
+        <v>370</v>
+      </c>
+      <c r="H308" t="s">
+        <v>18</v>
+      </c>
+      <c r="I308" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>308</v>
+      </c>
+      <c r="B309" t="s">
+        <v>9</v>
+      </c>
+      <c r="C309">
+        <v>8005284507</v>
+      </c>
+      <c r="D309" s="3">
+        <v>46055.512384259258</v>
+      </c>
+      <c r="E309" t="s">
+        <v>53</v>
+      </c>
+      <c r="F309" t="s">
+        <v>16</v>
+      </c>
+      <c r="G309" t="s">
+        <v>371</v>
+      </c>
+      <c r="H309" t="s">
+        <v>18</v>
+      </c>
+      <c r="I309" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>309</v>
+      </c>
+      <c r="B310" t="s">
+        <v>9</v>
+      </c>
+      <c r="C310">
+        <v>8005278395</v>
+      </c>
+      <c r="D310" s="3">
+        <v>46055.512511574067</v>
+      </c>
+      <c r="E310" t="s">
+        <v>37</v>
+      </c>
+      <c r="F310" t="s">
+        <v>16</v>
+      </c>
+      <c r="G310" t="s">
+        <v>372</v>
+      </c>
+      <c r="H310" t="s">
+        <v>35</v>
+      </c>
+      <c r="I310" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>310</v>
+      </c>
+      <c r="B311" t="s">
+        <v>9</v>
+      </c>
+      <c r="C311">
+        <v>8005251148</v>
+      </c>
+      <c r="D311" s="3">
+        <v>46055.540162037039</v>
+      </c>
+      <c r="E311" t="s">
+        <v>27</v>
+      </c>
+      <c r="F311" t="s">
+        <v>16</v>
+      </c>
+      <c r="G311" t="s">
+        <v>373</v>
+      </c>
+      <c r="H311" t="s">
+        <v>154</v>
+      </c>
+      <c r="I311" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>311</v>
+      </c>
+      <c r="B312" t="s">
+        <v>9</v>
+      </c>
+      <c r="C312">
+        <v>8005278311</v>
+      </c>
+      <c r="D312" s="3">
+        <v>46055.592326388891</v>
+      </c>
+      <c r="E312" t="s">
+        <v>27</v>
+      </c>
+      <c r="F312" t="s">
+        <v>16</v>
+      </c>
+      <c r="G312" t="s">
+        <v>374</v>
+      </c>
+      <c r="H312" t="s">
+        <v>18</v>
+      </c>
+      <c r="I312" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>312</v>
+      </c>
+      <c r="B313" t="s">
+        <v>9</v>
+      </c>
+      <c r="C313">
+        <v>8005275635</v>
+      </c>
+      <c r="D313" s="3">
+        <v>46055.703217592592</v>
+      </c>
+      <c r="E313" t="s">
+        <v>27</v>
+      </c>
+      <c r="F313" t="s">
+        <v>16</v>
+      </c>
+      <c r="G313" t="s">
+        <v>375</v>
+      </c>
+      <c r="H313" t="s">
+        <v>154</v>
+      </c>
+      <c r="I313" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>313</v>
+      </c>
+      <c r="B314" t="s">
+        <v>61</v>
+      </c>
+      <c r="C314">
+        <v>8005280530</v>
+      </c>
+      <c r="D314" s="3">
+        <v>46055.800706018519</v>
+      </c>
+      <c r="E314" t="s">
+        <v>20</v>
+      </c>
+      <c r="F314" t="s">
+        <v>16</v>
+      </c>
+      <c r="G314" t="s">
+        <v>376</v>
+      </c>
+      <c r="H314" t="s">
+        <v>35</v>
+      </c>
+      <c r="I314" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>314</v>
+      </c>
+      <c r="B315" t="s">
+        <v>9</v>
+      </c>
+      <c r="C315">
+        <v>8005272119</v>
+      </c>
+      <c r="D315" s="3">
+        <v>46055.870787037027</v>
+      </c>
+      <c r="E315" t="s">
+        <v>74</v>
+      </c>
+      <c r="F315" t="s">
+        <v>11</v>
+      </c>
+      <c r="G315" t="s">
+        <v>377</v>
+      </c>
+      <c r="H315" t="s">
+        <v>32</v>
+      </c>
+      <c r="I315" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>315</v>
+      </c>
+      <c r="B316" t="s">
+        <v>9</v>
+      </c>
+      <c r="C316">
+        <v>8005282966</v>
+      </c>
+      <c r="D316" s="3">
+        <v>46056.384085648147</v>
+      </c>
+      <c r="E316" t="s">
+        <v>53</v>
+      </c>
+      <c r="F316" t="s">
+        <v>16</v>
+      </c>
+      <c r="G316" t="s">
+        <v>378</v>
+      </c>
+      <c r="H316" t="s">
+        <v>35</v>
+      </c>
+      <c r="I316" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>316</v>
+      </c>
+      <c r="B317" t="s">
+        <v>9</v>
+      </c>
+      <c r="C317">
+        <v>8005254036</v>
+      </c>
+      <c r="D317" s="3">
+        <v>46056.384328703702</v>
+      </c>
+      <c r="E317" t="s">
+        <v>27</v>
+      </c>
+      <c r="F317" t="s">
+        <v>16</v>
+      </c>
+      <c r="G317" t="s">
+        <v>379</v>
+      </c>
+      <c r="H317" t="s">
+        <v>82</v>
+      </c>
+      <c r="I317" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>317</v>
+      </c>
+      <c r="B318" t="s">
+        <v>9</v>
+      </c>
+      <c r="C318">
+        <v>8005253400</v>
+      </c>
+      <c r="D318" s="3">
+        <v>46056.391793981478</v>
+      </c>
+      <c r="E318" t="s">
+        <v>98</v>
+      </c>
+      <c r="F318" t="s">
+        <v>16</v>
+      </c>
+      <c r="G318" t="s">
+        <v>380</v>
+      </c>
+      <c r="H318" t="s">
+        <v>82</v>
+      </c>
+      <c r="I318" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>318</v>
+      </c>
+      <c r="B319" t="s">
+        <v>9</v>
+      </c>
+      <c r="C319">
+        <v>8005277186</v>
+      </c>
+      <c r="D319" s="3">
+        <v>46056.411921296298</v>
+      </c>
+      <c r="E319" t="s">
+        <v>53</v>
+      </c>
+      <c r="F319" t="s">
+        <v>16</v>
+      </c>
+      <c r="G319" t="s">
+        <v>381</v>
+      </c>
+      <c r="H319" t="s">
+        <v>18</v>
+      </c>
+      <c r="I319" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>319</v>
+      </c>
+      <c r="B320" t="s">
+        <v>9</v>
+      </c>
+      <c r="C320">
+        <v>8005262693</v>
+      </c>
+      <c r="D320" s="3">
+        <v>46056.420810185176</v>
+      </c>
+      <c r="E320" t="s">
+        <v>15</v>
+      </c>
+      <c r="F320" t="s">
+        <v>16</v>
+      </c>
+      <c r="G320" t="s">
+        <v>382</v>
+      </c>
+      <c r="H320" t="s">
+        <v>154</v>
+      </c>
+      <c r="I320" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>320</v>
+      </c>
+      <c r="B321" t="s">
+        <v>9</v>
+      </c>
+      <c r="C321">
+        <v>8005247370</v>
+      </c>
+      <c r="D321" s="3">
+        <v>46056.456076388888</v>
+      </c>
+      <c r="E321" t="s">
+        <v>23</v>
+      </c>
+      <c r="F321" t="s">
+        <v>16</v>
+      </c>
+      <c r="G321" t="s">
+        <v>383</v>
+      </c>
+      <c r="H321" t="s">
+        <v>35</v>
+      </c>
+      <c r="I321" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>321</v>
+      </c>
+      <c r="B322" t="s">
+        <v>9</v>
+      </c>
+      <c r="C322">
+        <v>8005282361</v>
+      </c>
+      <c r="D322" s="3">
+        <v>46056.502210648148</v>
+      </c>
+      <c r="E322" t="s">
+        <v>23</v>
+      </c>
+      <c r="F322" t="s">
+        <v>16</v>
+      </c>
+      <c r="G322" t="s">
+        <v>384</v>
+      </c>
+      <c r="H322" t="s">
+        <v>18</v>
+      </c>
+      <c r="I322" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>322</v>
+      </c>
+      <c r="B323" t="s">
+        <v>9</v>
+      </c>
+      <c r="C323">
+        <v>8005287614</v>
+      </c>
+      <c r="D323" s="3">
+        <v>46056.504351851851</v>
+      </c>
+      <c r="E323" t="s">
+        <v>23</v>
+      </c>
+      <c r="F323" t="s">
+        <v>11</v>
+      </c>
+      <c r="G323" t="s">
+        <v>385</v>
+      </c>
+      <c r="H323" t="s">
+        <v>35</v>
+      </c>
+      <c r="I323" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>323</v>
+      </c>
+      <c r="B324" t="s">
+        <v>9</v>
+      </c>
+      <c r="C324">
+        <v>8005285952</v>
+      </c>
+      <c r="D324" s="3">
+        <v>46056.510185185187</v>
+      </c>
+      <c r="E324" t="s">
+        <v>15</v>
+      </c>
+      <c r="F324" t="s">
+        <v>11</v>
+      </c>
+      <c r="G324" t="s">
+        <v>386</v>
+      </c>
+      <c r="H324" t="s">
+        <v>18</v>
+      </c>
+      <c r="I324" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>324</v>
+      </c>
+      <c r="B325" t="s">
+        <v>9</v>
+      </c>
+      <c r="C325">
+        <v>8005275703</v>
+      </c>
+      <c r="D325" s="3">
+        <v>46056.579317129632</v>
+      </c>
+      <c r="E325" t="s">
+        <v>27</v>
+      </c>
+      <c r="F325" t="s">
+        <v>16</v>
+      </c>
+      <c r="G325" t="s">
+        <v>387</v>
+      </c>
+      <c r="H325" t="s">
+        <v>18</v>
+      </c>
+      <c r="I325" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>325</v>
+      </c>
+      <c r="B326" t="s">
+        <v>9</v>
+      </c>
+      <c r="C326">
+        <v>8005285741</v>
+      </c>
+      <c r="D326" s="3">
+        <v>46056.581597222219</v>
+      </c>
+      <c r="E326" t="s">
+        <v>15</v>
+      </c>
+      <c r="F326" t="s">
+        <v>16</v>
+      </c>
+      <c r="G326" t="s">
+        <v>388</v>
+      </c>
+      <c r="H326" t="s">
+        <v>18</v>
+      </c>
+      <c r="I326" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>326</v>
+      </c>
+      <c r="B327" t="s">
+        <v>9</v>
+      </c>
+      <c r="C327">
+        <v>8005265966</v>
+      </c>
+      <c r="D327" s="3">
+        <v>46056.589722222219</v>
+      </c>
+      <c r="E327" t="s">
+        <v>49</v>
+      </c>
+      <c r="F327" t="s">
+        <v>11</v>
+      </c>
+      <c r="G327" t="s">
+        <v>389</v>
+      </c>
+      <c r="H327" t="s">
+        <v>13</v>
+      </c>
+      <c r="I327" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>327</v>
+      </c>
+      <c r="B328" t="s">
+        <v>9</v>
+      </c>
+      <c r="C328">
+        <v>8005255071</v>
+      </c>
+      <c r="D328" s="3">
+        <v>46056.61986111111</v>
+      </c>
+      <c r="E328" t="s">
+        <v>37</v>
+      </c>
+      <c r="F328" t="s">
+        <v>11</v>
+      </c>
+      <c r="G328" t="s">
+        <v>390</v>
+      </c>
+      <c r="H328" t="s">
+        <v>18</v>
+      </c>
+      <c r="I328" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 09/02/2026 15:56:51,86
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B511601-214E-4930-BC7D-308330A93810}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F89DFF2C-2719-4668-914D-37E7D7D4BC58}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$286</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$390</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="453">
   <si>
     <t>ID</t>
   </si>
@@ -1276,6 +1276,192 @@
   </si>
   <si>
     <t>A visita não resolveu meu problema, é preciso mudar o aparelho.</t>
+  </si>
+  <si>
+    <t>Terrível assistência técnica, vou já agora para o 4º chamado tentando o conserto do mesmo purificador, que desta vez o técnico simplesmente deixou inutilizado.</t>
+  </si>
+  <si>
+    <t>A ultima visita tecnica foi muito ruim. abaixo da minha expectativa para o padrao Brastemp esperado</t>
+  </si>
+  <si>
+    <t>O atendimento por telelefone é sofrível.</t>
+  </si>
+  <si>
+    <t>Com o purificador não temos nada a reclamar, apesar de que com muita freqüencia o filtro satura muito rápido em poucos meses e com isso a água sai muita fraca.Mas o atendimento do técnico nesse dia ficou a desejar, deixou os copos que estavam disposto para uso em cima do purificador no balcão sem retornar para onde se encontrava e alguns copos com água sem fazer seu devido descarte no lixo.</t>
+  </si>
+  <si>
+    <t>a manutenção teve que ser reagendada 3 vezes, pois não foi cumprido o primeiro prazo e não havia data próxima para reagendamento.</t>
+  </si>
+  <si>
+    <t>O atendimento para manutenção do purificador está péssimo, o contato telefônico é demorado, as visitas são agendadas com o prazo enorme para solução do problema, é necessário entrar em contato mais que uma vez para tentar resolver o mesmo problema e conseguir um agendamento com uma data data razoável. Revejam o atendimento do purificador, pois esta bem ruim.por exemplo a troca do purificador estava agendada para 28/02/2026 , isso é um absurdo, aqui é uma loja não tem condições no alto verão não ter água gelada.</t>
+  </si>
+  <si>
+    <t>O purificador é ótimo mas, o valor mensal é muito alto.</t>
+  </si>
+  <si>
+    <t>Novamente, aconteceu o mesmo problema da minha reclamação anterior! Reclamação aberta - Brastemp - 8005265717 - 8005270132 - Luciane. Agendei a manutenção para os nossos 2 "dois" purificadores que estavam apresentando gosto ruim na água. A técnica Amanda Braga da Silva, chegou após o horário agendado que era das 8h às 13h - ela chegou 13h36. Somente verificou 1 purificador, não queria trocar o elemento filtrante... só trocou após a minha reclamação.  Permaneceu na empresa até as 14h03, ou seja. menos de meia hora.Comprometimento zero, péssimo atendimento.</t>
+  </si>
+  <si>
+    <t>A manutenção é demorada, e o custo alto.</t>
+  </si>
+  <si>
+    <t>Visita técnica é uma novela! Ligam para agendar para quase 30 dias depois e quando chega a data, o técnico não vem. Uma vergonha! Tive que agendar novamente e o técnico veio e não realizou a troca do filtro que foi pedida. Estou indo para a 3° visita e vamos ver o que a brastemp vai aprontar essa vez</t>
+  </si>
+  <si>
+    <t>Estou aguardando o retorno do técnico pq o filtro estava com gelo e não trocou a peça.</t>
+  </si>
+  <si>
+    <t>A comunicação com a Brastemp não tem sido a melhor. Há dificuldade de contato (humano) e atendimento da demanda. Com 15 dias de uso o gás do purificador acabou. Pode ter sido por consumo, mas suponho que não. Com menos de 1 mês de uso, apresentou defeito. Consegui acessar a assistência e a vinda do técnico foi rápida</t>
+  </si>
+  <si>
+    <t>Neste momento não estou satisfeita com o atendimento pois tentei solicitar isenção do boleto com vencimento em 10/02/26, pois estava com o purificador desligado desde 25/12/25 até 27/02/26 e não consegui.</t>
+  </si>
+  <si>
+    <t>O purificador é um ótimo produto, mas o atendimento de vocês é péssimo</t>
+  </si>
+  <si>
+    <t>Estamos tendo dificuldades com vocês para assinar o contrato (saúde e segurança), o qual já expliquei via email, um dos nossos Seguranças do trabalho já explicou por telefone que ficaram de ver com o Jurídico e nos daria um Posicionamento, todos já estão cientes, que sem o contrato assinado não tem como o técnico fazer as manutenções, e mesmo assim enviaram o técnico, que acabou ficando a manhã toda aguardando na Portaria devido a falta de envio deste documento assinado. Foi aberto uma exceção porque o Profissional já estava lá e precisávamos dos itens funcionando adequadamente, mas não podemos mais liberar na próxima caso o documento não seja enviado assinado pelo Representante que assina pela Culligan.Por isso desta vez a minha nota será zero, devido a todos esse estresse que estou passando com vocês.</t>
+  </si>
+  <si>
+    <t>Péssima!Filtro congela toda hora e zero de suporte, seja atendente ou técnico!!!</t>
+  </si>
+  <si>
+    <t>Instalação ótima.  Técnicos atenciosos. Mas o aparelho faz barulho toda vez que esta que o botão da agua é acionado</t>
+  </si>
+  <si>
+    <t>O equipamento está com a parte de cima desgastada e o técnico não resolveu o problema.</t>
+  </si>
+  <si>
+    <t>O problema persiste e não é o atendimento.  Ele apenas tem que ajudar a resolver e endereçar a vocês as reclamações que faço.</t>
+  </si>
+  <si>
+    <t>Muito util, mas sempre pode melhorar.</t>
+  </si>
+  <si>
+    <t>O purificador é bom mas, fazer contato com a Central, caso queira alguma coisa é péssimo.</t>
+  </si>
+  <si>
+    <t>Dificuldade na solicitação de visita técnica fora do período semestral. Na visita o técnico confirmou o problema no filtro.</t>
+  </si>
+  <si>
+    <t>Fiquei insatisfeito com a falta de flexibilidade para o atendimento emergencial Pois de uma hora pra outra a minha água ficou com um cheiro horrível/insuportável e não consegui um atendimento emergencial tive que aguardar a agenda.Fiquei tendo que comprar água em galão vários dias.</t>
+  </si>
+  <si>
+    <t>Quanto ao produto estou muito satisfeita, mas a dificuldade em falar: ser atendido por vocês é enorme. Sempre estão com problemas no sistema, não localizam o CPF, muito desgaste pra conseguir ser atendido</t>
+  </si>
+  <si>
+    <t>Não compareceu ontem conforme marcado a visita</t>
+  </si>
+  <si>
+    <t>Tudo bem mas está ficando caro , por todos estes anos .</t>
+  </si>
+  <si>
+    <t>No dia a dia funciona bem a manutenção, mas se houver um problema ou emergência e precisar de suporte técnico rápido é péssimo!E na Central de Atendimento vc não ter a opção de conversar, só o robô ou alguém digitando é muito ruim!!</t>
+  </si>
+  <si>
+    <t>Tempo de resposta</t>
+  </si>
+  <si>
+    <t>Já possuímos o purificador há mais de 5 anos. Durante esse tempo houveram alguns defeitos que foram corrigidos. A equipe de técnicos que atende é muito variável, durante  esses 5 anos, uns técnicos são ótimos e educados e outros grosseiros e até racista com a empregada que o atendeu.</t>
+  </si>
+  <si>
+    <t>acho pratico, e muito bom!</t>
+  </si>
+  <si>
+    <t>Em relação a manutenção efetiva no aparelho foi boa, agora em relação à cumprir o horário / período agendado foi totalmente o oposto. Agendamos a visita técnica para o dia: 02/02/2026 no período da TARDE, e o técnico foi no primeiro horário da manhã (08h30).</t>
+  </si>
+  <si>
+    <t>De dois anos para cá o atendimento de mamutencao, que era automático a cada seis meses, deixou de existir. Não indicaria a ninguém esse filtro, já que surgiram novas marcas para escolher. O problema que tive (de vazamento) demorou um mês para ser resolvido, pois não fui informada da mudança de empresa de manutenção (era Multicenter). Só fui atendida quando liguei diretamente para a Brastemp e ameacei cancelar o contrato.</t>
+  </si>
+  <si>
+    <t>Marca o período da tarde e vai em outro horário e não resolve Estamos sem água a mais de 1 mês e pagando a mensalidade</t>
+  </si>
+  <si>
+    <t>Não obtive a visita técnica</t>
+  </si>
+  <si>
+    <t>O problema não foi resolvido, precisava trocar uma peça que ela não tinha. Teve que solicitar nova visita e ainda não foi agendada.</t>
+  </si>
+  <si>
+    <t>O técnico compareceu no dia 02/02, mas o problema não foi resolvido, pois precisa colocar um pressurizador, e até agora não retornaram para colocar a peça.</t>
+  </si>
+  <si>
+    <t>A Bobina queima com frequencia, nessa troca o tecnico não trocou o Filtro que tb não foi trocado na ultima!</t>
+  </si>
+  <si>
+    <t>Solicitei um reparo no botão do filtro que não esta funcionando, impossibilitando de sair agua, e o técnico chegou com peças nada a ver com o solicitado, ou seja o problema não foi resolvido, e eu continuo aqui com o filtro sem funcionar, e sabe lá Deus quando vai vir alguém pra resolver.</t>
+  </si>
+  <si>
+    <t>O técnico que esteve na minha casa não fez nada , tirou um copo de água do filtro falou que estica bom e foi embora , nem olhou o filtro</t>
+  </si>
+  <si>
+    <t>Até agora tô gostando</t>
+  </si>
+  <si>
+    <t>Achei pessimo! A agua com gás trava o tempo todo, chamei o tecnico, e nos foi passado que é assim mesmo, depois de dois copos ela trava e pode ficar até 15 min sem sair agua.</t>
+  </si>
+  <si>
+    <t>O profissional foi educado e muito rápido no procedimento. Porém, não houve a limpeza do equipamento como os outros profissionais faziam antes.Ele inclusive, identificou uma sujeira, que pensávamos que fosse da caixa d'água, porém remontou o aparelho sem higienizá-lo.</t>
+  </si>
+  <si>
+    <t>Avalio como uma boa experiência. Somente no último agendamento da visita técnica que houve dificuldade, pois tive que agendar 3 vezes, para que na última o técnico aparecesse.</t>
+  </si>
+  <si>
+    <t>EM SEGUNDOS FEZ A VISITA, ENTRA PEDE 1 COPO COLOCA AGUA PINGA 1 GOTA TRANSPARENTE E DIZ ESTA OTIMO.</t>
+  </si>
+  <si>
+    <t>serviço caro e encarecendo</t>
+  </si>
+  <si>
+    <t>Ele vai bem, porém, marcar visita técnica e ninguém aparecer e não dar satisfação é bem corriqueiro. Só na terceira marcação consegui que viessem e fora do horario marcado</t>
+  </si>
+  <si>
+    <t>Ele é ótimo recomendo</t>
+  </si>
+  <si>
+    <t>A empresa peca no atendimento aos agendamentos Toda vez que agendo, eles atrasam. Foram 2 chamadas, as quais o agendamento inicial não foi cumprido.</t>
+  </si>
+  <si>
+    <t>Não foi resolvido, técnico não executou o serviço e por mais uma vez o agendamento foi jogado para outro dia</t>
+  </si>
+  <si>
+    <t>O técnico compareceu, fez à manutenção, e o purificador ficou pingando água, o que não estava. Disse o técnico estava solicitando a troca do purificador, tudo bem desde que seja do mesmo modelo que tenho.</t>
+  </si>
+  <si>
+    <t>Preciso de suporte com urgência</t>
+  </si>
+  <si>
+    <t>Marcado para de tarde funcionário chega de manhã pq diz ser melhor para ele!  Não se editificou. Terceira vez que isso acontece.  Não se identificou na recibo do serviço.</t>
+  </si>
+  <si>
+    <t>Sempre gostei muito! Hoje não mais!!!Não indico pra ninguém!!!!Detesto falar com robô!!!Nada se resolve!!!!!Amava a Brastemp! Mas infelizmente pra nós … idosos vcs dificultam muito!!!!! Estou aguardando a troca!!!!!Estou comprando água pois ele esquenta muito!!!!!</t>
+  </si>
+  <si>
+    <t>Correu bem.</t>
+  </si>
+  <si>
+    <t>Muitos problemas, segunda troca de equipamento que tive.</t>
+  </si>
+  <si>
+    <t>Veio três vezes e o problema não foi resolvido</t>
+  </si>
+  <si>
+    <t>Péssima experiência, esperei um mês para trocarem a máquina e acho absurdo ter que pagar a mensalidade de um serviço que não tive</t>
+  </si>
+  <si>
+    <t>Por enquanto não mto satisfeito, foi instalado dia 6/2/26 dia 7/2/26 não sai mais água gelada ! Estou aguardando a vista técnica !</t>
+  </si>
+  <si>
+    <t>Estou aguardando a troca que o técnico falou que faria</t>
+  </si>
+  <si>
+    <t>Estava sem usar o purificador desde começo de janeiro pois o cheiro e sabor da agua estavam horríveis , comprei agua até o dia que finalmenteo técnico veio,  foi na sexta 06/02,  um mês para agendar uma visita técnica , gostaria de um desconto na minha mensalidade devido ao tempo sem uso</t>
+  </si>
+  <si>
+    <t>O tempo da última manutenção para essa, extrapolou os 6 meses, e para conseguir essa que recebi tive que ligar e reclamar muito.</t>
+  </si>
+  <si>
+    <t>Desmarquei pelo WhatsApp e mesmo assim o consultor compareceu no endereço e não pode entrar para realizar a manutenção porque não havia ninguém no local, motivo pelo qual eu havia suspendido o agendamento.</t>
   </si>
 </sst>
 </file>
@@ -1644,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I328"/>
+  <dimension ref="A1:I390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A287" sqref="A287:I328"/>
+    <sheetView tabSelected="1" topLeftCell="B154" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11175,6 +11361,1804 @@
         <v>22</v>
       </c>
     </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>328</v>
+      </c>
+      <c r="B329" t="s">
+        <v>9</v>
+      </c>
+      <c r="C329">
+        <v>8005276745</v>
+      </c>
+      <c r="D329" s="3">
+        <v>46056.655347222222</v>
+      </c>
+      <c r="E329" t="s">
+        <v>44</v>
+      </c>
+      <c r="F329" t="s">
+        <v>16</v>
+      </c>
+      <c r="G329" t="s">
+        <v>391</v>
+      </c>
+      <c r="H329" t="s">
+        <v>18</v>
+      </c>
+      <c r="I329" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>329</v>
+      </c>
+      <c r="B330" t="s">
+        <v>9</v>
+      </c>
+      <c r="C330">
+        <v>8005255287</v>
+      </c>
+      <c r="D330" s="3">
+        <v>46056.662187499998</v>
+      </c>
+      <c r="E330" t="s">
+        <v>15</v>
+      </c>
+      <c r="F330" t="s">
+        <v>16</v>
+      </c>
+      <c r="G330" t="s">
+        <v>392</v>
+      </c>
+      <c r="H330" t="s">
+        <v>18</v>
+      </c>
+      <c r="I330" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>330</v>
+      </c>
+      <c r="B331" t="s">
+        <v>9</v>
+      </c>
+      <c r="C331">
+        <v>8005219847</v>
+      </c>
+      <c r="D331" s="3">
+        <v>46056.827719907407</v>
+      </c>
+      <c r="E331" t="s">
+        <v>53</v>
+      </c>
+      <c r="F331" t="s">
+        <v>16</v>
+      </c>
+      <c r="G331" t="s">
+        <v>393</v>
+      </c>
+      <c r="H331" t="s">
+        <v>82</v>
+      </c>
+      <c r="I331" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>331</v>
+      </c>
+      <c r="B332" t="s">
+        <v>9</v>
+      </c>
+      <c r="C332">
+        <v>8005287679</v>
+      </c>
+      <c r="D332" s="3">
+        <v>46057.39466435185</v>
+      </c>
+      <c r="E332" t="s">
+        <v>20</v>
+      </c>
+      <c r="F332" t="s">
+        <v>11</v>
+      </c>
+      <c r="G332" t="s">
+        <v>394</v>
+      </c>
+      <c r="H332" t="s">
+        <v>18</v>
+      </c>
+      <c r="I332" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>332</v>
+      </c>
+      <c r="B333" t="s">
+        <v>9</v>
+      </c>
+      <c r="C333">
+        <v>8005265280</v>
+      </c>
+      <c r="D333" s="3">
+        <v>46057.410937499997</v>
+      </c>
+      <c r="E333" t="s">
+        <v>53</v>
+      </c>
+      <c r="F333" t="s">
+        <v>11</v>
+      </c>
+      <c r="G333" t="s">
+        <v>395</v>
+      </c>
+      <c r="H333" t="s">
+        <v>18</v>
+      </c>
+      <c r="I333" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>333</v>
+      </c>
+      <c r="B334" t="s">
+        <v>9</v>
+      </c>
+      <c r="C334">
+        <v>8005279610</v>
+      </c>
+      <c r="D334" s="3">
+        <v>46057.417337962957</v>
+      </c>
+      <c r="E334" t="s">
+        <v>20</v>
+      </c>
+      <c r="F334" t="s">
+        <v>16</v>
+      </c>
+      <c r="G334" t="s">
+        <v>396</v>
+      </c>
+      <c r="H334" t="s">
+        <v>32</v>
+      </c>
+      <c r="I334" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>334</v>
+      </c>
+      <c r="B335" t="s">
+        <v>9</v>
+      </c>
+      <c r="C335">
+        <v>8005250512</v>
+      </c>
+      <c r="D335" s="3">
+        <v>46057.452245370368</v>
+      </c>
+      <c r="E335" t="s">
+        <v>15</v>
+      </c>
+      <c r="F335" t="s">
+        <v>11</v>
+      </c>
+      <c r="G335" t="s">
+        <v>397</v>
+      </c>
+      <c r="H335" t="s">
+        <v>13</v>
+      </c>
+      <c r="I335" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>335</v>
+      </c>
+      <c r="B336" t="s">
+        <v>9</v>
+      </c>
+      <c r="C336">
+        <v>8005213338</v>
+      </c>
+      <c r="D336" s="3">
+        <v>46057.482256944437</v>
+      </c>
+      <c r="E336" t="s">
+        <v>23</v>
+      </c>
+      <c r="F336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336" t="s">
+        <v>398</v>
+      </c>
+      <c r="H336" t="s">
+        <v>18</v>
+      </c>
+      <c r="I336" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>336</v>
+      </c>
+      <c r="B337" t="s">
+        <v>9</v>
+      </c>
+      <c r="C337">
+        <v>8005250287</v>
+      </c>
+      <c r="D337" s="3">
+        <v>46057.523344907408</v>
+      </c>
+      <c r="E337" t="s">
+        <v>20</v>
+      </c>
+      <c r="F337" t="s">
+        <v>16</v>
+      </c>
+      <c r="G337" t="s">
+        <v>399</v>
+      </c>
+      <c r="H337" t="s">
+        <v>13</v>
+      </c>
+      <c r="I337" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>337</v>
+      </c>
+      <c r="B338" t="s">
+        <v>9</v>
+      </c>
+      <c r="C338">
+        <v>8005250478</v>
+      </c>
+      <c r="D338" s="3">
+        <v>46057.52375</v>
+      </c>
+      <c r="E338" t="s">
+        <v>27</v>
+      </c>
+      <c r="F338" t="s">
+        <v>16</v>
+      </c>
+      <c r="G338" t="s">
+        <v>400</v>
+      </c>
+      <c r="H338" t="s">
+        <v>32</v>
+      </c>
+      <c r="I338" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>338</v>
+      </c>
+      <c r="B339" t="s">
+        <v>9</v>
+      </c>
+      <c r="C339">
+        <v>8005289163</v>
+      </c>
+      <c r="D339" s="3">
+        <v>46057.534016203703</v>
+      </c>
+      <c r="E339" t="s">
+        <v>37</v>
+      </c>
+      <c r="F339" t="s">
+        <v>11</v>
+      </c>
+      <c r="G339" t="s">
+        <v>401</v>
+      </c>
+      <c r="H339" t="s">
+        <v>18</v>
+      </c>
+      <c r="I339" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>339</v>
+      </c>
+      <c r="B340" t="s">
+        <v>9</v>
+      </c>
+      <c r="C340">
+        <v>8005290613</v>
+      </c>
+      <c r="D340" s="3">
+        <v>46057.587951388887</v>
+      </c>
+      <c r="E340" t="s">
+        <v>125</v>
+      </c>
+      <c r="F340" t="s">
+        <v>16</v>
+      </c>
+      <c r="G340" t="s">
+        <v>402</v>
+      </c>
+      <c r="H340" t="s">
+        <v>35</v>
+      </c>
+      <c r="I340" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>340</v>
+      </c>
+      <c r="B341" t="s">
+        <v>9</v>
+      </c>
+      <c r="C341">
+        <v>8005289827</v>
+      </c>
+      <c r="D341" s="3">
+        <v>46057.659155092602</v>
+      </c>
+      <c r="E341" t="s">
+        <v>15</v>
+      </c>
+      <c r="F341" t="s">
+        <v>11</v>
+      </c>
+      <c r="G341" t="s">
+        <v>403</v>
+      </c>
+      <c r="H341" t="s">
+        <v>13</v>
+      </c>
+      <c r="I341" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>341</v>
+      </c>
+      <c r="B342" t="s">
+        <v>9</v>
+      </c>
+      <c r="C342">
+        <v>8005267134</v>
+      </c>
+      <c r="D342" s="3">
+        <v>46057.888796296298</v>
+      </c>
+      <c r="E342" t="s">
+        <v>15</v>
+      </c>
+      <c r="F342" t="s">
+        <v>16</v>
+      </c>
+      <c r="G342" t="s">
+        <v>404</v>
+      </c>
+      <c r="H342" t="s">
+        <v>13</v>
+      </c>
+      <c r="I342" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>342</v>
+      </c>
+      <c r="B343" t="s">
+        <v>9</v>
+      </c>
+      <c r="C343">
+        <v>8005280047</v>
+      </c>
+      <c r="D343" s="3">
+        <v>46057.941817129627</v>
+      </c>
+      <c r="E343" t="s">
+        <v>44</v>
+      </c>
+      <c r="F343" t="s">
+        <v>16</v>
+      </c>
+      <c r="G343" t="s">
+        <v>405</v>
+      </c>
+      <c r="H343" t="s">
+        <v>13</v>
+      </c>
+      <c r="I343" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>343</v>
+      </c>
+      <c r="B344" t="s">
+        <v>61</v>
+      </c>
+      <c r="C344">
+        <v>8005271235</v>
+      </c>
+      <c r="D344" s="3">
+        <v>46058.276307870372</v>
+      </c>
+      <c r="E344" t="s">
+        <v>23</v>
+      </c>
+      <c r="F344" t="s">
+        <v>16</v>
+      </c>
+      <c r="G344" t="s">
+        <v>406</v>
+      </c>
+      <c r="H344" t="s">
+        <v>35</v>
+      </c>
+      <c r="I344" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>344</v>
+      </c>
+      <c r="B345" t="s">
+        <v>61</v>
+      </c>
+      <c r="C345">
+        <v>8005290332</v>
+      </c>
+      <c r="D345" s="3">
+        <v>46058.38689814815</v>
+      </c>
+      <c r="E345" t="s">
+        <v>10</v>
+      </c>
+      <c r="F345" t="s">
+        <v>11</v>
+      </c>
+      <c r="G345" t="s">
+        <v>407</v>
+      </c>
+      <c r="H345" t="s">
+        <v>35</v>
+      </c>
+      <c r="I345" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>345</v>
+      </c>
+      <c r="B346" t="s">
+        <v>9</v>
+      </c>
+      <c r="C346">
+        <v>8005266452</v>
+      </c>
+      <c r="D346" s="3">
+        <v>46058.396249999998</v>
+      </c>
+      <c r="E346" t="s">
+        <v>53</v>
+      </c>
+      <c r="F346" t="s">
+        <v>16</v>
+      </c>
+      <c r="G346" t="s">
+        <v>408</v>
+      </c>
+      <c r="H346" t="s">
+        <v>18</v>
+      </c>
+      <c r="I346" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>346</v>
+      </c>
+      <c r="B347" t="s">
+        <v>9</v>
+      </c>
+      <c r="C347">
+        <v>8005275248</v>
+      </c>
+      <c r="D347" s="3">
+        <v>46058.416481481479</v>
+      </c>
+      <c r="E347" t="s">
+        <v>20</v>
+      </c>
+      <c r="F347" t="s">
+        <v>16</v>
+      </c>
+      <c r="G347" t="s">
+        <v>409</v>
+      </c>
+      <c r="H347" t="s">
+        <v>18</v>
+      </c>
+      <c r="I347" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>347</v>
+      </c>
+      <c r="B348" t="s">
+        <v>9</v>
+      </c>
+      <c r="C348">
+        <v>8005224762</v>
+      </c>
+      <c r="D348" s="3">
+        <v>46058.449525462973</v>
+      </c>
+      <c r="E348" t="s">
+        <v>53</v>
+      </c>
+      <c r="F348" t="s">
+        <v>11</v>
+      </c>
+      <c r="G348" t="s">
+        <v>410</v>
+      </c>
+      <c r="H348" t="s">
+        <v>13</v>
+      </c>
+      <c r="I348" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>348</v>
+      </c>
+      <c r="B349" t="s">
+        <v>9</v>
+      </c>
+      <c r="C349">
+        <v>8005287514</v>
+      </c>
+      <c r="D349" s="3">
+        <v>46058.477210648147</v>
+      </c>
+      <c r="E349" t="s">
+        <v>53</v>
+      </c>
+      <c r="F349" t="s">
+        <v>16</v>
+      </c>
+      <c r="G349" t="s">
+        <v>411</v>
+      </c>
+      <c r="H349" t="s">
+        <v>82</v>
+      </c>
+      <c r="I349" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>349</v>
+      </c>
+      <c r="B350" t="s">
+        <v>9</v>
+      </c>
+      <c r="C350">
+        <v>8005291296</v>
+      </c>
+      <c r="D350" s="3">
+        <v>46058.507337962961</v>
+      </c>
+      <c r="E350" t="s">
+        <v>65</v>
+      </c>
+      <c r="F350" t="s">
+        <v>11</v>
+      </c>
+      <c r="G350" t="s">
+        <v>412</v>
+      </c>
+      <c r="H350" t="s">
+        <v>82</v>
+      </c>
+      <c r="I350" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>350</v>
+      </c>
+      <c r="B351" t="s">
+        <v>9</v>
+      </c>
+      <c r="C351">
+        <v>8005280544</v>
+      </c>
+      <c r="D351" s="3">
+        <v>46058.507708333331</v>
+      </c>
+      <c r="E351" t="s">
+        <v>20</v>
+      </c>
+      <c r="F351" t="s">
+        <v>16</v>
+      </c>
+      <c r="G351" t="s">
+        <v>413</v>
+      </c>
+      <c r="H351" t="s">
+        <v>32</v>
+      </c>
+      <c r="I351" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>351</v>
+      </c>
+      <c r="B352" t="s">
+        <v>9</v>
+      </c>
+      <c r="C352">
+        <v>8005292236</v>
+      </c>
+      <c r="D352" s="3">
+        <v>46058.50949074074</v>
+      </c>
+      <c r="E352" t="s">
+        <v>15</v>
+      </c>
+      <c r="F352" t="s">
+        <v>11</v>
+      </c>
+      <c r="G352" t="s">
+        <v>414</v>
+      </c>
+      <c r="H352" t="s">
+        <v>82</v>
+      </c>
+      <c r="I352" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>352</v>
+      </c>
+      <c r="B353" t="s">
+        <v>9</v>
+      </c>
+      <c r="C353">
+        <v>8005291362</v>
+      </c>
+      <c r="D353" s="3">
+        <v>46058.510358796288</v>
+      </c>
+      <c r="E353" t="s">
+        <v>15</v>
+      </c>
+      <c r="F353" t="s">
+        <v>16</v>
+      </c>
+      <c r="G353" t="s">
+        <v>415</v>
+      </c>
+      <c r="H353" t="s">
+        <v>18</v>
+      </c>
+      <c r="I353" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>353</v>
+      </c>
+      <c r="B354" t="s">
+        <v>9</v>
+      </c>
+      <c r="C354">
+        <v>8005271620</v>
+      </c>
+      <c r="D354" s="3">
+        <v>46058.511145833327</v>
+      </c>
+      <c r="E354" t="s">
+        <v>49</v>
+      </c>
+      <c r="F354" t="s">
+        <v>11</v>
+      </c>
+      <c r="G354" t="s">
+        <v>416</v>
+      </c>
+      <c r="H354" t="s">
+        <v>13</v>
+      </c>
+      <c r="I354" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>354</v>
+      </c>
+      <c r="B355" t="s">
+        <v>9</v>
+      </c>
+      <c r="C355">
+        <v>8005290312</v>
+      </c>
+      <c r="D355" s="3">
+        <v>46058.539513888893</v>
+      </c>
+      <c r="E355" t="s">
+        <v>20</v>
+      </c>
+      <c r="F355" t="s">
+        <v>16</v>
+      </c>
+      <c r="G355" t="s">
+        <v>417</v>
+      </c>
+      <c r="H355" t="s">
+        <v>82</v>
+      </c>
+      <c r="I355" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>355</v>
+      </c>
+      <c r="B356" t="s">
+        <v>9</v>
+      </c>
+      <c r="C356">
+        <v>8005277045</v>
+      </c>
+      <c r="D356" s="3">
+        <v>46058.559039351851</v>
+      </c>
+      <c r="E356" t="s">
+        <v>15</v>
+      </c>
+      <c r="F356" t="s">
+        <v>11</v>
+      </c>
+      <c r="G356" t="s">
+        <v>419</v>
+      </c>
+      <c r="H356" t="s">
+        <v>18</v>
+      </c>
+      <c r="I356" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>356</v>
+      </c>
+      <c r="B357" t="s">
+        <v>9</v>
+      </c>
+      <c r="C357">
+        <v>8005268370</v>
+      </c>
+      <c r="D357" s="3">
+        <v>46058.671689814822</v>
+      </c>
+      <c r="E357" t="s">
+        <v>27</v>
+      </c>
+      <c r="F357" t="s">
+        <v>11</v>
+      </c>
+      <c r="G357" t="s">
+        <v>420</v>
+      </c>
+      <c r="H357" t="s">
+        <v>13</v>
+      </c>
+      <c r="I357" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>357</v>
+      </c>
+      <c r="B358" t="s">
+        <v>9</v>
+      </c>
+      <c r="C358">
+        <v>8005253679</v>
+      </c>
+      <c r="D358" s="3">
+        <v>46058.686516203707</v>
+      </c>
+      <c r="E358" t="s">
+        <v>15</v>
+      </c>
+      <c r="F358" t="s">
+        <v>16</v>
+      </c>
+      <c r="G358" t="s">
+        <v>421</v>
+      </c>
+      <c r="H358" t="s">
+        <v>18</v>
+      </c>
+      <c r="I358" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>358</v>
+      </c>
+      <c r="B359" t="s">
+        <v>9</v>
+      </c>
+      <c r="C359">
+        <v>8005290743</v>
+      </c>
+      <c r="D359" s="3">
+        <v>46058.825671296298</v>
+      </c>
+      <c r="E359" t="s">
+        <v>20</v>
+      </c>
+      <c r="F359" t="s">
+        <v>16</v>
+      </c>
+      <c r="G359" t="s">
+        <v>422</v>
+      </c>
+      <c r="H359" t="s">
+        <v>32</v>
+      </c>
+      <c r="I359" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>359</v>
+      </c>
+      <c r="B360" t="s">
+        <v>9</v>
+      </c>
+      <c r="C360">
+        <v>8005272197</v>
+      </c>
+      <c r="D360" s="3">
+        <v>46058.954733796287</v>
+      </c>
+      <c r="E360" t="s">
+        <v>20</v>
+      </c>
+      <c r="F360" t="s">
+        <v>16</v>
+      </c>
+      <c r="G360" t="s">
+        <v>423</v>
+      </c>
+      <c r="H360" t="s">
+        <v>18</v>
+      </c>
+      <c r="I360" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>360</v>
+      </c>
+      <c r="B361" t="s">
+        <v>9</v>
+      </c>
+      <c r="C361">
+        <v>8005289127</v>
+      </c>
+      <c r="D361" s="3">
+        <v>46059.385150462957</v>
+      </c>
+      <c r="E361" t="s">
+        <v>20</v>
+      </c>
+      <c r="F361" t="s">
+        <v>16</v>
+      </c>
+      <c r="G361" t="s">
+        <v>424</v>
+      </c>
+      <c r="H361" t="s">
+        <v>18</v>
+      </c>
+      <c r="I361" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>361</v>
+      </c>
+      <c r="B362" t="s">
+        <v>9</v>
+      </c>
+      <c r="C362">
+        <v>8005291671</v>
+      </c>
+      <c r="D362" s="3">
+        <v>46059.409444444442</v>
+      </c>
+      <c r="E362" t="s">
+        <v>37</v>
+      </c>
+      <c r="F362" t="s">
+        <v>16</v>
+      </c>
+      <c r="G362" t="s">
+        <v>425</v>
+      </c>
+      <c r="H362" t="s">
+        <v>154</v>
+      </c>
+      <c r="I362" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>362</v>
+      </c>
+      <c r="B363" t="s">
+        <v>9</v>
+      </c>
+      <c r="C363">
+        <v>8005284690</v>
+      </c>
+      <c r="D363" s="3">
+        <v>46059.418437499997</v>
+      </c>
+      <c r="E363" t="s">
+        <v>20</v>
+      </c>
+      <c r="F363" t="s">
+        <v>16</v>
+      </c>
+      <c r="G363" t="s">
+        <v>426</v>
+      </c>
+      <c r="H363" t="s">
+        <v>154</v>
+      </c>
+      <c r="I363" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>363</v>
+      </c>
+      <c r="B364" t="s">
+        <v>9</v>
+      </c>
+      <c r="C364">
+        <v>8005282594</v>
+      </c>
+      <c r="D364" s="3">
+        <v>46059.447951388887</v>
+      </c>
+      <c r="E364" t="s">
+        <v>44</v>
+      </c>
+      <c r="F364" t="s">
+        <v>16</v>
+      </c>
+      <c r="G364" t="s">
+        <v>427</v>
+      </c>
+      <c r="H364" t="s">
+        <v>18</v>
+      </c>
+      <c r="I364" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>364</v>
+      </c>
+      <c r="B365" t="s">
+        <v>9</v>
+      </c>
+      <c r="C365">
+        <v>8005283263</v>
+      </c>
+      <c r="D365" s="3">
+        <v>46059.461215277777</v>
+      </c>
+      <c r="E365" t="s">
+        <v>27</v>
+      </c>
+      <c r="F365" t="s">
+        <v>16</v>
+      </c>
+      <c r="G365" t="s">
+        <v>428</v>
+      </c>
+      <c r="H365" t="s">
+        <v>18</v>
+      </c>
+      <c r="I365" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>365</v>
+      </c>
+      <c r="B366" t="s">
+        <v>9</v>
+      </c>
+      <c r="C366">
+        <v>8005288790</v>
+      </c>
+      <c r="D366" s="3">
+        <v>46059.501458333332</v>
+      </c>
+      <c r="E366" t="s">
+        <v>23</v>
+      </c>
+      <c r="F366" t="s">
+        <v>11</v>
+      </c>
+      <c r="G366" t="s">
+        <v>157</v>
+      </c>
+      <c r="H366" t="s">
+        <v>13</v>
+      </c>
+      <c r="I366" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>366</v>
+      </c>
+      <c r="B367" t="s">
+        <v>9</v>
+      </c>
+      <c r="C367">
+        <v>8005285589</v>
+      </c>
+      <c r="D367" s="3">
+        <v>46059.501863425918</v>
+      </c>
+      <c r="E367" t="s">
+        <v>53</v>
+      </c>
+      <c r="F367" t="s">
+        <v>16</v>
+      </c>
+      <c r="G367" t="s">
+        <v>429</v>
+      </c>
+      <c r="H367" t="s">
+        <v>18</v>
+      </c>
+      <c r="I367" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>367</v>
+      </c>
+      <c r="B368" t="s">
+        <v>9</v>
+      </c>
+      <c r="C368">
+        <v>8005280490</v>
+      </c>
+      <c r="D368" s="3">
+        <v>46059.502754629633</v>
+      </c>
+      <c r="E368" t="s">
+        <v>53</v>
+      </c>
+      <c r="F368" t="s">
+        <v>11</v>
+      </c>
+      <c r="G368" t="s">
+        <v>430</v>
+      </c>
+      <c r="H368" t="s">
+        <v>13</v>
+      </c>
+      <c r="I368" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>368</v>
+      </c>
+      <c r="B369" t="s">
+        <v>9</v>
+      </c>
+      <c r="C369">
+        <v>8005273490</v>
+      </c>
+      <c r="D369" s="3">
+        <v>46059.528171296297</v>
+      </c>
+      <c r="E369" t="s">
+        <v>15</v>
+      </c>
+      <c r="F369" t="s">
+        <v>16</v>
+      </c>
+      <c r="G369" t="s">
+        <v>431</v>
+      </c>
+      <c r="H369" t="s">
+        <v>35</v>
+      </c>
+      <c r="I369" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>369</v>
+      </c>
+      <c r="B370" t="s">
+        <v>9</v>
+      </c>
+      <c r="C370">
+        <v>8005291034</v>
+      </c>
+      <c r="D370" s="3">
+        <v>46059.529131944437</v>
+      </c>
+      <c r="E370" t="s">
+        <v>23</v>
+      </c>
+      <c r="F370" t="s">
+        <v>11</v>
+      </c>
+      <c r="G370" t="s">
+        <v>432</v>
+      </c>
+      <c r="H370" t="s">
+        <v>18</v>
+      </c>
+      <c r="I370" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>370</v>
+      </c>
+      <c r="B371" t="s">
+        <v>9</v>
+      </c>
+      <c r="C371">
+        <v>8005287892</v>
+      </c>
+      <c r="D371" s="3">
+        <v>46059.615405092591</v>
+      </c>
+      <c r="E371" t="s">
+        <v>53</v>
+      </c>
+      <c r="F371" t="s">
+        <v>11</v>
+      </c>
+      <c r="G371" t="s">
+        <v>433</v>
+      </c>
+      <c r="H371" t="s">
+        <v>18</v>
+      </c>
+      <c r="I371" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>371</v>
+      </c>
+      <c r="B372" t="s">
+        <v>9</v>
+      </c>
+      <c r="C372">
+        <v>8005258086</v>
+      </c>
+      <c r="D372" s="3">
+        <v>46059.830243055563</v>
+      </c>
+      <c r="E372" t="s">
+        <v>53</v>
+      </c>
+      <c r="F372" t="s">
+        <v>16</v>
+      </c>
+      <c r="G372" t="s">
+        <v>434</v>
+      </c>
+      <c r="H372" t="s">
+        <v>18</v>
+      </c>
+      <c r="I372" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>372</v>
+      </c>
+      <c r="B373" t="s">
+        <v>9</v>
+      </c>
+      <c r="C373">
+        <v>8005269640</v>
+      </c>
+      <c r="D373" s="3">
+        <v>46059.954722222217</v>
+      </c>
+      <c r="E373" t="s">
+        <v>23</v>
+      </c>
+      <c r="F373" t="s">
+        <v>11</v>
+      </c>
+      <c r="G373" t="s">
+        <v>435</v>
+      </c>
+      <c r="H373" t="s">
+        <v>13</v>
+      </c>
+      <c r="I373" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>373</v>
+      </c>
+      <c r="B374" t="s">
+        <v>9</v>
+      </c>
+      <c r="C374">
+        <v>8005217388</v>
+      </c>
+      <c r="D374" s="3">
+        <v>46060.337106481478</v>
+      </c>
+      <c r="E374" t="s">
+        <v>53</v>
+      </c>
+      <c r="F374" t="s">
+        <v>11</v>
+      </c>
+      <c r="G374" t="s">
+        <v>436</v>
+      </c>
+      <c r="H374" t="s">
+        <v>18</v>
+      </c>
+      <c r="I374" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>374</v>
+      </c>
+      <c r="B375" t="s">
+        <v>9</v>
+      </c>
+      <c r="C375">
+        <v>8005284186</v>
+      </c>
+      <c r="D375" s="3">
+        <v>46060.876087962963</v>
+      </c>
+      <c r="E375" t="s">
+        <v>224</v>
+      </c>
+      <c r="F375" t="s">
+        <v>11</v>
+      </c>
+      <c r="G375" t="s">
+        <v>437</v>
+      </c>
+      <c r="H375" t="s">
+        <v>13</v>
+      </c>
+      <c r="I375" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>375</v>
+      </c>
+      <c r="B376" t="s">
+        <v>9</v>
+      </c>
+      <c r="C376">
+        <v>8005286476</v>
+      </c>
+      <c r="D376" s="3">
+        <v>46061.361377314817</v>
+      </c>
+      <c r="E376" t="s">
+        <v>53</v>
+      </c>
+      <c r="F376" t="s">
+        <v>16</v>
+      </c>
+      <c r="G376" t="s">
+        <v>438</v>
+      </c>
+      <c r="H376" t="s">
+        <v>18</v>
+      </c>
+      <c r="I376" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>376</v>
+      </c>
+      <c r="B377" t="s">
+        <v>9</v>
+      </c>
+      <c r="C377">
+        <v>8005282933</v>
+      </c>
+      <c r="D377" s="3">
+        <v>46061.825578703712</v>
+      </c>
+      <c r="E377" t="s">
+        <v>27</v>
+      </c>
+      <c r="F377" t="s">
+        <v>16</v>
+      </c>
+      <c r="G377" t="s">
+        <v>439</v>
+      </c>
+      <c r="H377" t="s">
+        <v>18</v>
+      </c>
+      <c r="I377" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>377</v>
+      </c>
+      <c r="B378" t="s">
+        <v>9</v>
+      </c>
+      <c r="C378">
+        <v>8005285132</v>
+      </c>
+      <c r="D378" s="3">
+        <v>46061.927384259259</v>
+      </c>
+      <c r="E378" t="s">
+        <v>15</v>
+      </c>
+      <c r="F378" t="s">
+        <v>11</v>
+      </c>
+      <c r="G378" t="s">
+        <v>440</v>
+      </c>
+      <c r="H378" t="s">
+        <v>18</v>
+      </c>
+      <c r="I378" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>378</v>
+      </c>
+      <c r="B379" t="s">
+        <v>9</v>
+      </c>
+      <c r="C379">
+        <v>8005291510</v>
+      </c>
+      <c r="D379" s="3">
+        <v>46062.364710648151</v>
+      </c>
+      <c r="E379" t="s">
+        <v>37</v>
+      </c>
+      <c r="F379" t="s">
+        <v>16</v>
+      </c>
+      <c r="G379" t="s">
+        <v>441</v>
+      </c>
+      <c r="H379" t="s">
+        <v>13</v>
+      </c>
+      <c r="I379" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>379</v>
+      </c>
+      <c r="B380" t="s">
+        <v>9</v>
+      </c>
+      <c r="C380">
+        <v>8005154756</v>
+      </c>
+      <c r="D380" s="3">
+        <v>46062.367152777777</v>
+      </c>
+      <c r="E380" t="s">
+        <v>53</v>
+      </c>
+      <c r="F380" t="s">
+        <v>16</v>
+      </c>
+      <c r="G380" t="s">
+        <v>442</v>
+      </c>
+      <c r="H380" t="s">
+        <v>18</v>
+      </c>
+      <c r="I380" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>380</v>
+      </c>
+      <c r="B381" t="s">
+        <v>9</v>
+      </c>
+      <c r="C381">
+        <v>8005276882</v>
+      </c>
+      <c r="D381" s="3">
+        <v>46062.386388888888</v>
+      </c>
+      <c r="E381" t="s">
+        <v>27</v>
+      </c>
+      <c r="F381" t="s">
+        <v>16</v>
+      </c>
+      <c r="G381" t="s">
+        <v>443</v>
+      </c>
+      <c r="H381" t="s">
+        <v>82</v>
+      </c>
+      <c r="I381" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>381</v>
+      </c>
+      <c r="B382" t="s">
+        <v>9</v>
+      </c>
+      <c r="C382">
+        <v>8005286209</v>
+      </c>
+      <c r="D382" s="3">
+        <v>46062.400393518517</v>
+      </c>
+      <c r="E382" t="s">
+        <v>53</v>
+      </c>
+      <c r="F382" t="s">
+        <v>11</v>
+      </c>
+      <c r="G382" t="s">
+        <v>444</v>
+      </c>
+      <c r="H382" t="s">
+        <v>13</v>
+      </c>
+      <c r="I382" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>382</v>
+      </c>
+      <c r="B383" t="s">
+        <v>9</v>
+      </c>
+      <c r="C383">
+        <v>8005274558</v>
+      </c>
+      <c r="D383" s="3">
+        <v>46062.457048611112</v>
+      </c>
+      <c r="E383" t="s">
+        <v>41</v>
+      </c>
+      <c r="F383" t="s">
+        <v>16</v>
+      </c>
+      <c r="G383" t="s">
+        <v>445</v>
+      </c>
+      <c r="H383" t="s">
+        <v>35</v>
+      </c>
+      <c r="I383" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>383</v>
+      </c>
+      <c r="B384" t="s">
+        <v>9</v>
+      </c>
+      <c r="C384">
+        <v>8005292022</v>
+      </c>
+      <c r="D384" s="3">
+        <v>46062.495081018518</v>
+      </c>
+      <c r="E384" t="s">
+        <v>23</v>
+      </c>
+      <c r="F384" t="s">
+        <v>16</v>
+      </c>
+      <c r="G384" t="s">
+        <v>446</v>
+      </c>
+      <c r="H384" t="s">
+        <v>18</v>
+      </c>
+      <c r="I384" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>384</v>
+      </c>
+      <c r="B385" t="s">
+        <v>9</v>
+      </c>
+      <c r="C385">
+        <v>8005264187</v>
+      </c>
+      <c r="D385" s="3">
+        <v>46062.500902777778</v>
+      </c>
+      <c r="E385" t="s">
+        <v>23</v>
+      </c>
+      <c r="F385" t="s">
+        <v>16</v>
+      </c>
+      <c r="G385" t="s">
+        <v>447</v>
+      </c>
+      <c r="H385" t="s">
+        <v>32</v>
+      </c>
+      <c r="I385" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>385</v>
+      </c>
+      <c r="B386" t="s">
+        <v>61</v>
+      </c>
+      <c r="C386">
+        <v>8005292181</v>
+      </c>
+      <c r="D386" s="3">
+        <v>46062.501157407409</v>
+      </c>
+      <c r="E386" t="s">
+        <v>27</v>
+      </c>
+      <c r="F386" t="s">
+        <v>16</v>
+      </c>
+      <c r="G386" t="s">
+        <v>448</v>
+      </c>
+      <c r="H386" t="s">
+        <v>35</v>
+      </c>
+      <c r="I386" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>386</v>
+      </c>
+      <c r="B387" t="s">
+        <v>9</v>
+      </c>
+      <c r="C387">
+        <v>8005270840</v>
+      </c>
+      <c r="D387" s="3">
+        <v>46062.508506944447</v>
+      </c>
+      <c r="E387" t="s">
+        <v>23</v>
+      </c>
+      <c r="F387" t="s">
+        <v>11</v>
+      </c>
+      <c r="G387" t="s">
+        <v>449</v>
+      </c>
+      <c r="H387" t="s">
+        <v>154</v>
+      </c>
+      <c r="I387" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>387</v>
+      </c>
+      <c r="B388" t="s">
+        <v>9</v>
+      </c>
+      <c r="C388">
+        <v>8005255500</v>
+      </c>
+      <c r="D388" s="3">
+        <v>46062.522870370369</v>
+      </c>
+      <c r="E388" t="s">
+        <v>27</v>
+      </c>
+      <c r="F388" t="s">
+        <v>11</v>
+      </c>
+      <c r="G388" t="s">
+        <v>450</v>
+      </c>
+      <c r="H388" t="s">
+        <v>32</v>
+      </c>
+      <c r="I388" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>388</v>
+      </c>
+      <c r="B389" t="s">
+        <v>9</v>
+      </c>
+      <c r="C389">
+        <v>8005260276</v>
+      </c>
+      <c r="D389" s="3">
+        <v>46062.555034722223</v>
+      </c>
+      <c r="E389" t="s">
+        <v>27</v>
+      </c>
+      <c r="F389" t="s">
+        <v>11</v>
+      </c>
+      <c r="G389" t="s">
+        <v>451</v>
+      </c>
+      <c r="H389" t="s">
+        <v>32</v>
+      </c>
+      <c r="I389" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>389</v>
+      </c>
+      <c r="B390" t="s">
+        <v>9</v>
+      </c>
+      <c r="C390">
+        <v>8005263943</v>
+      </c>
+      <c r="D390" s="3">
+        <v>46062.558807870373</v>
+      </c>
+      <c r="E390" t="s">
+        <v>23</v>
+      </c>
+      <c r="F390" t="s">
+        <v>16</v>
+      </c>
+      <c r="G390" t="s">
+        <v>452</v>
+      </c>
+      <c r="H390" t="s">
+        <v>82</v>
+      </c>
+      <c r="I390" t="s">
+        <v>418</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 11/02/2026 16:18:06,47
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F89DFF2C-2719-4668-914D-37E7D7D4BC58}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAD60D4-4B8D-45B2-8B5C-69AC8D0DAE96}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="480">
   <si>
     <t>ID</t>
   </si>
@@ -1462,6 +1462,87 @@
   </si>
   <si>
     <t>Desmarquei pelo WhatsApp e mesmo assim o consultor compareceu no endereço e não pode entrar para realizar a manutenção porque não havia ninguém no local, motivo pelo qual eu havia suspendido o agendamento.</t>
+  </si>
+  <si>
+    <t>Boa. As vezes não dá para conciliar disponibilidade de visita</t>
+  </si>
+  <si>
+    <t>A água está com um gosto (horrível) forte de “plástico com bicarbonato”. Está praticamente impossível beber. Já tirei litros e litros e não sai o gosto.</t>
+  </si>
+  <si>
+    <t>Purificador foi entregue com vazamento na conexão, após o registro. Ao abrir a solicitação com o time de vendas, não suportam, ao ligar na central após uma ura grande, consegui falar, contudo, não temos site, app ou forma para acompanhar o serviço, sendo a recomendação trazida, até que o ajuste possa ser feito (dia 11/2, sendo que foi instalado dia 06/2), foi de estrangular a mangueira, algo que aumentaria a pressão e não diminuiria a mesma. Sinceramente, a experiência de compra foi muito bom, de instalação razoável, pois ocorreu atraso e não somos informados, e o pós vendas deixando a desejar.</t>
+  </si>
+  <si>
+    <t>O atendimento é excelente, extremamente profissional. Entretanto, o que tem incomodado é que horário marcado é sistematicamente descumprido, inclusive invertendo o turno solicitado. Reforço que o técnico presta uma excelente serviço.</t>
+  </si>
+  <si>
+    <t>A instalação foi super tranquila!</t>
+  </si>
+  <si>
+    <t>gostamos do purificador mas ele é caro e estamos com dificuldade na cobrança</t>
+  </si>
+  <si>
+    <t>Ainda não resolveu o meu problema.</t>
+  </si>
+  <si>
+    <t>Foram feitos 3 ou 4 agendamentos anteriores onde ninguém apareceu. Nem avisou que não iriam. Precisei agendar novamente todas as outras vezes. Até conseguir esse último tecnico que foi essa semana. Alem disso o tecnico foi no periodo da manhã e estava agendado de tarde. Por sorte tinha gente em casa, senão seria mais um “cano”</t>
+  </si>
+  <si>
+    <t>O vazamento na parte de baixo esta sendo recorrente.Mais uma vez terá que trocar o aparelho.Ainda não foi feita a troca e continua vazando.</t>
+  </si>
+  <si>
+    <t>O técnico esteve aqui e disse que em 05 dias viria alguém para trocar o purificador. Ninguém veio. Péssimo atendimento.</t>
+  </si>
+  <si>
+    <t>acho muito bom mas acho que vou cancelar a mensalidade esta alta pra mim se houver possibilidade de acordo podemos conversar</t>
+  </si>
+  <si>
+    <t>AT_ECO_SP_BAURU</t>
+  </si>
+  <si>
+    <t>Boa tarde. O técnico foi atenciosao e veio dentro do horario marcado.Preciso que o técnico retorne ao meu apto, o purificador está fazendo barulho quando acionado.Outra coisa que me chamou atenção,  foi que ele fez a troca do purificador mas não trocou o elemento filtrante externo.Moro em um prédio com tubulação em ferro e só o interno não é suficiente.Aguardo manifestação de vcs.</t>
+  </si>
+  <si>
+    <t>Nao tenho problema com a qualidade da agua. Os aparelhos atuais dao problemas mecânicos mais rapido que o antigo.</t>
+  </si>
+  <si>
+    <t>Acho que o valor do serviço é muito alto</t>
+  </si>
+  <si>
+    <t>Demorou um mês entre minha ligação e o agendamento da visita, é a primeira vez que demora este período longo.</t>
+  </si>
+  <si>
+    <t>O Técnico habitual está de férias e o seu substituto deixou a desejar.Em 5 minutos trocou o filtro e não testou quimicamente a água,  nem purgou o ar do aparelho.Ao chegar, não se apresentou; não reparou na abertura da válvula de água  e deixou o material utilizado espalhados sobre o balcão. Creio que, por ser novato e por cobrir a ausência daquele que está de férias, não julgou necessário valorizar o atendimento. Tomara que a experiência lhe traga mais comprometimento com a imagem da companhia.</t>
+  </si>
+  <si>
+    <t>Como vou avaliar uma coisa que não teve.Atendimento pessímo, não indico.</t>
+  </si>
+  <si>
+    <t>Eu estava em casa o rapaz nao veio e depois quando veio disse que precisa de um pressurizador em vez da Brastemp já deixar com o tecnico precisa aguardar mais de 10 dias. Sinceramente nao tem 1 semana e ja me arrependi amargamente</t>
+  </si>
+  <si>
+    <t>Gosto muito, só acho o valor um pouco alto e demora para agendar visita técnica</t>
+  </si>
+  <si>
+    <t>Pela pontualidade, foi marcado na parte da manhã , isto é, 8 às 13h. Fiquei esperando , amanhã toda. Abrir mão de outras coisas, para ficar a disposição. Só chegou após 13:20h. Estou insatisfeito com atendimento.</t>
+  </si>
+  <si>
+    <t>Purificador fornece água bem filtrada,límpida,sem gosto de cloro.O problema é o atendimento virtual.Quando liga para marcar pergunta se é o responsável,resposta SIM.Pergunta novamente,várias vezes,e nada.Desliga.Quando novo contato,oferece data vencida.Até conseguir agendar,toma muito tempo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atendimento </t>
+  </si>
+  <si>
+    <t>Bom</t>
+  </si>
+  <si>
+    <t>Aluguei o purificador recentemente (2 meses) e o aparelho apresentou defeito, segundo o técnico, falta de gás. O atendimento do técnico foi muito bom porém o agendamento para a visita e agendamento para substituição do  purificador é demorada. Quando reinstalarem pedirei o abatimento no boleto dos duas que fiquei sem o purificador pois não quero pagar por algo que contratei e a Brastemp não está fornecendo.</t>
+  </si>
+  <si>
+    <t>O técnico não sabia o número da ordem de serviço e nem a senha, o que é muito importante por questões de segurança.</t>
+  </si>
+  <si>
+    <t>A água é muito boa, porém em caso de falta de energia elétrica, morremos de sede….</t>
   </si>
 </sst>
 </file>
@@ -1830,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I390"/>
+  <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B154" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="E406" sqref="E406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13159,6 +13240,731 @@
         <v>418</v>
       </c>
     </row>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>390</v>
+      </c>
+      <c r="B391" t="s">
+        <v>9</v>
+      </c>
+      <c r="C391">
+        <v>8005230093</v>
+      </c>
+      <c r="D391" s="3">
+        <v>46062.708587962959</v>
+      </c>
+      <c r="E391" t="s">
+        <v>20</v>
+      </c>
+      <c r="F391" t="s">
+        <v>11</v>
+      </c>
+      <c r="G391" t="s">
+        <v>453</v>
+      </c>
+      <c r="H391" t="s">
+        <v>32</v>
+      </c>
+      <c r="I391" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>391</v>
+      </c>
+      <c r="B392" t="s">
+        <v>61</v>
+      </c>
+      <c r="C392">
+        <v>8005284763</v>
+      </c>
+      <c r="D392" s="3">
+        <v>46062.929074074083</v>
+      </c>
+      <c r="E392" t="s">
+        <v>125</v>
+      </c>
+      <c r="F392" t="s">
+        <v>16</v>
+      </c>
+      <c r="G392" t="s">
+        <v>454</v>
+      </c>
+      <c r="H392" t="s">
+        <v>35</v>
+      </c>
+      <c r="I392" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>392</v>
+      </c>
+      <c r="B393" t="s">
+        <v>61</v>
+      </c>
+      <c r="C393">
+        <v>8005290922</v>
+      </c>
+      <c r="D393" s="3">
+        <v>46063.387881944444</v>
+      </c>
+      <c r="E393" t="s">
+        <v>15</v>
+      </c>
+      <c r="F393" t="s">
+        <v>11</v>
+      </c>
+      <c r="G393" t="s">
+        <v>455</v>
+      </c>
+      <c r="H393" t="s">
+        <v>18</v>
+      </c>
+      <c r="I393" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>393</v>
+      </c>
+      <c r="B394" t="s">
+        <v>9</v>
+      </c>
+      <c r="C394">
+        <v>8005286290</v>
+      </c>
+      <c r="D394" s="3">
+        <v>46063.43414351852</v>
+      </c>
+      <c r="E394" t="s">
+        <v>224</v>
+      </c>
+      <c r="F394" t="s">
+        <v>11</v>
+      </c>
+      <c r="G394" t="s">
+        <v>456</v>
+      </c>
+      <c r="H394" t="s">
+        <v>18</v>
+      </c>
+      <c r="I394" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>394</v>
+      </c>
+      <c r="B395" t="s">
+        <v>61</v>
+      </c>
+      <c r="C395">
+        <v>8005292540</v>
+      </c>
+      <c r="D395" s="3">
+        <v>46063.443912037037</v>
+      </c>
+      <c r="E395" t="s">
+        <v>125</v>
+      </c>
+      <c r="F395" t="s">
+        <v>11</v>
+      </c>
+      <c r="G395" t="s">
+        <v>457</v>
+      </c>
+      <c r="H395" t="s">
+        <v>13</v>
+      </c>
+      <c r="I395" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>395</v>
+      </c>
+      <c r="B396" t="s">
+        <v>9</v>
+      </c>
+      <c r="C396">
+        <v>8005285322</v>
+      </c>
+      <c r="D396" s="3">
+        <v>46063.468449074076</v>
+      </c>
+      <c r="E396" t="s">
+        <v>224</v>
+      </c>
+      <c r="F396" t="s">
+        <v>11</v>
+      </c>
+      <c r="G396" t="s">
+        <v>458</v>
+      </c>
+      <c r="H396" t="s">
+        <v>13</v>
+      </c>
+      <c r="I396" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>396</v>
+      </c>
+      <c r="B397" t="s">
+        <v>9</v>
+      </c>
+      <c r="C397">
+        <v>8005296436</v>
+      </c>
+      <c r="D397" s="3">
+        <v>46063.501562500001</v>
+      </c>
+      <c r="E397" t="s">
+        <v>27</v>
+      </c>
+      <c r="F397" t="s">
+        <v>16</v>
+      </c>
+      <c r="G397" t="s">
+        <v>459</v>
+      </c>
+      <c r="H397" t="s">
+        <v>18</v>
+      </c>
+      <c r="I397" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>397</v>
+      </c>
+      <c r="B398" t="s">
+        <v>9</v>
+      </c>
+      <c r="C398">
+        <v>8005293020</v>
+      </c>
+      <c r="D398" s="3">
+        <v>46063.521145833343</v>
+      </c>
+      <c r="E398" t="s">
+        <v>23</v>
+      </c>
+      <c r="F398" t="s">
+        <v>16</v>
+      </c>
+      <c r="G398" t="s">
+        <v>460</v>
+      </c>
+      <c r="H398" t="s">
+        <v>18</v>
+      </c>
+      <c r="I398" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>398</v>
+      </c>
+      <c r="B399" t="s">
+        <v>9</v>
+      </c>
+      <c r="C399">
+        <v>8005299854</v>
+      </c>
+      <c r="D399" s="3">
+        <v>46063.522476851853</v>
+      </c>
+      <c r="E399" t="s">
+        <v>53</v>
+      </c>
+      <c r="F399" t="s">
+        <v>11</v>
+      </c>
+      <c r="G399" t="s">
+        <v>461</v>
+      </c>
+      <c r="H399" t="s">
+        <v>18</v>
+      </c>
+      <c r="I399" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>399</v>
+      </c>
+      <c r="B400" t="s">
+        <v>9</v>
+      </c>
+      <c r="C400">
+        <v>8005297911</v>
+      </c>
+      <c r="D400" s="3">
+        <v>46063.522777777784</v>
+      </c>
+      <c r="E400" t="s">
+        <v>53</v>
+      </c>
+      <c r="F400" t="s">
+        <v>16</v>
+      </c>
+      <c r="G400" t="s">
+        <v>462</v>
+      </c>
+      <c r="H400" t="s">
+        <v>18</v>
+      </c>
+      <c r="I400" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>400</v>
+      </c>
+      <c r="B401" t="s">
+        <v>9</v>
+      </c>
+      <c r="C401">
+        <v>8005263938</v>
+      </c>
+      <c r="D401" s="3">
+        <v>46063.591886574082</v>
+      </c>
+      <c r="E401" t="s">
+        <v>23</v>
+      </c>
+      <c r="F401" t="s">
+        <v>11</v>
+      </c>
+      <c r="G401" t="s">
+        <v>463</v>
+      </c>
+      <c r="H401" t="s">
+        <v>13</v>
+      </c>
+      <c r="I401" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>401</v>
+      </c>
+      <c r="B402" t="s">
+        <v>9</v>
+      </c>
+      <c r="C402">
+        <v>8005286964</v>
+      </c>
+      <c r="D402" s="3">
+        <v>46063.629861111112</v>
+      </c>
+      <c r="E402" t="s">
+        <v>464</v>
+      </c>
+      <c r="F402" t="s">
+        <v>11</v>
+      </c>
+      <c r="G402" t="s">
+        <v>465</v>
+      </c>
+      <c r="H402" t="s">
+        <v>18</v>
+      </c>
+      <c r="I402" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>402</v>
+      </c>
+      <c r="B403" t="s">
+        <v>9</v>
+      </c>
+      <c r="C403">
+        <v>8005292458</v>
+      </c>
+      <c r="D403" s="3">
+        <v>46063.795659722222</v>
+      </c>
+      <c r="E403" t="s">
+        <v>23</v>
+      </c>
+      <c r="F403" t="s">
+        <v>11</v>
+      </c>
+      <c r="G403" t="s">
+        <v>466</v>
+      </c>
+      <c r="H403" t="s">
+        <v>35</v>
+      </c>
+      <c r="I403" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>403</v>
+      </c>
+      <c r="B404" t="s">
+        <v>9</v>
+      </c>
+      <c r="C404">
+        <v>8005284928</v>
+      </c>
+      <c r="D404" s="3">
+        <v>46063.810046296298</v>
+      </c>
+      <c r="E404" t="s">
+        <v>53</v>
+      </c>
+      <c r="F404" t="s">
+        <v>16</v>
+      </c>
+      <c r="G404" t="s">
+        <v>467</v>
+      </c>
+      <c r="H404" t="s">
+        <v>13</v>
+      </c>
+      <c r="I404" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>404</v>
+      </c>
+      <c r="B405" t="s">
+        <v>9</v>
+      </c>
+      <c r="C405">
+        <v>8005262658</v>
+      </c>
+      <c r="D405" s="3">
+        <v>46064.367974537039</v>
+      </c>
+      <c r="E405" t="s">
+        <v>27</v>
+      </c>
+      <c r="F405" t="s">
+        <v>11</v>
+      </c>
+      <c r="G405" t="s">
+        <v>468</v>
+      </c>
+      <c r="H405" t="s">
+        <v>32</v>
+      </c>
+      <c r="I405" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>405</v>
+      </c>
+      <c r="B406" t="s">
+        <v>9</v>
+      </c>
+      <c r="C406">
+        <v>8005286061</v>
+      </c>
+      <c r="D406" s="3">
+        <v>46064.431423611109</v>
+      </c>
+      <c r="E406" t="s">
+        <v>53</v>
+      </c>
+      <c r="F406" t="s">
+        <v>11</v>
+      </c>
+      <c r="G406" t="s">
+        <v>469</v>
+      </c>
+      <c r="H406" t="s">
+        <v>18</v>
+      </c>
+      <c r="I406" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>406</v>
+      </c>
+      <c r="B407" t="s">
+        <v>9</v>
+      </c>
+      <c r="C407">
+        <v>8005298244</v>
+      </c>
+      <c r="D407" s="3">
+        <v>46064.435601851852</v>
+      </c>
+      <c r="E407" t="s">
+        <v>53</v>
+      </c>
+      <c r="F407" t="s">
+        <v>16</v>
+      </c>
+      <c r="G407" t="s">
+        <v>470</v>
+      </c>
+      <c r="H407" t="s">
+        <v>18</v>
+      </c>
+      <c r="I407" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>407</v>
+      </c>
+      <c r="B408" t="s">
+        <v>61</v>
+      </c>
+      <c r="C408">
+        <v>8005297440</v>
+      </c>
+      <c r="D408" s="3">
+        <v>46064.474849537037</v>
+      </c>
+      <c r="E408" t="s">
+        <v>37</v>
+      </c>
+      <c r="F408" t="s">
+        <v>16</v>
+      </c>
+      <c r="G408" t="s">
+        <v>471</v>
+      </c>
+      <c r="H408" t="s">
+        <v>18</v>
+      </c>
+      <c r="I408" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>408</v>
+      </c>
+      <c r="B409" t="s">
+        <v>9</v>
+      </c>
+      <c r="C409">
+        <v>8005269484</v>
+      </c>
+      <c r="D409" s="3">
+        <v>46064.502465277779</v>
+      </c>
+      <c r="E409" t="s">
+        <v>27</v>
+      </c>
+      <c r="F409" t="s">
+        <v>11</v>
+      </c>
+      <c r="G409" t="s">
+        <v>472</v>
+      </c>
+      <c r="H409" t="s">
+        <v>32</v>
+      </c>
+      <c r="I409" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>409</v>
+      </c>
+      <c r="B410" t="s">
+        <v>9</v>
+      </c>
+      <c r="C410">
+        <v>8005290057</v>
+      </c>
+      <c r="D410" s="3">
+        <v>46064.505196759259</v>
+      </c>
+      <c r="E410" t="s">
+        <v>53</v>
+      </c>
+      <c r="F410" t="s">
+        <v>16</v>
+      </c>
+      <c r="G410" t="s">
+        <v>473</v>
+      </c>
+      <c r="H410" t="s">
+        <v>18</v>
+      </c>
+      <c r="I410" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>410</v>
+      </c>
+      <c r="B411" t="s">
+        <v>9</v>
+      </c>
+      <c r="C411">
+        <v>8005285756</v>
+      </c>
+      <c r="D411" s="3">
+        <v>46064.515173611107</v>
+      </c>
+      <c r="E411" t="s">
+        <v>37</v>
+      </c>
+      <c r="F411" t="s">
+        <v>11</v>
+      </c>
+      <c r="G411" t="s">
+        <v>474</v>
+      </c>
+      <c r="H411" t="s">
+        <v>475</v>
+      </c>
+      <c r="I411" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>411</v>
+      </c>
+      <c r="B412" t="s">
+        <v>9</v>
+      </c>
+      <c r="C412">
+        <v>8005264422</v>
+      </c>
+      <c r="D412" s="3">
+        <v>46064.535173611112</v>
+      </c>
+      <c r="E412" t="s">
+        <v>20</v>
+      </c>
+      <c r="F412" t="s">
+        <v>11</v>
+      </c>
+      <c r="G412" t="s">
+        <v>476</v>
+      </c>
+      <c r="H412" t="s">
+        <v>13</v>
+      </c>
+      <c r="I412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>412</v>
+      </c>
+      <c r="B413" t="s">
+        <v>9</v>
+      </c>
+      <c r="C413">
+        <v>8005296356</v>
+      </c>
+      <c r="D413" s="3">
+        <v>46064.545416666668</v>
+      </c>
+      <c r="E413" t="s">
+        <v>49</v>
+      </c>
+      <c r="F413" t="s">
+        <v>11</v>
+      </c>
+      <c r="G413" t="s">
+        <v>477</v>
+      </c>
+      <c r="H413" t="s">
+        <v>35</v>
+      </c>
+      <c r="I413" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>413</v>
+      </c>
+      <c r="B414" t="s">
+        <v>9</v>
+      </c>
+      <c r="C414">
+        <v>8005273187</v>
+      </c>
+      <c r="D414" s="3">
+        <v>46064.558206018519</v>
+      </c>
+      <c r="E414" t="s">
+        <v>23</v>
+      </c>
+      <c r="F414" t="s">
+        <v>11</v>
+      </c>
+      <c r="G414" t="s">
+        <v>478</v>
+      </c>
+      <c r="H414" t="s">
+        <v>18</v>
+      </c>
+      <c r="I414" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>414</v>
+      </c>
+      <c r="B415" t="s">
+        <v>9</v>
+      </c>
+      <c r="C415">
+        <v>8005263760</v>
+      </c>
+      <c r="D415" s="3">
+        <v>46064.574062500003</v>
+      </c>
+      <c r="E415" t="s">
+        <v>23</v>
+      </c>
+      <c r="F415" t="s">
+        <v>11</v>
+      </c>
+      <c r="G415" t="s">
+        <v>479</v>
+      </c>
+      <c r="H415" t="s">
+        <v>35</v>
+      </c>
+      <c r="I415" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 13/02/2026 15:38:16,49
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAD60D4-4B8D-45B2-8B5C-69AC8D0DAE96}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77640EB1-4CB6-4E9C-B73B-C49D2DB7AC09}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="506">
   <si>
     <t>ID</t>
   </si>
@@ -1543,6 +1543,84 @@
   </si>
   <si>
     <t>A água é muito boa, porém em caso de falta de energia elétrica, morremos de sede….</t>
+  </si>
+  <si>
+    <t>A visita NÃO ACONTECEU!!!! Apesar de ter sido marcada a visita para o período da TARDE, o técnico veio no período da MANHÃ!!!! Eu não podia atende-lo pois estava no banho me preparando para uma aula, e o meu Marly estava se arrumando para a fisioterapia que ele tinha em seguida. Me ligaram do atendimento Brastemp, eu expliquei a situação e a moça que me informou que ele viria às 13hs, Mas ele NÃO apareceu!!!!!</t>
+  </si>
+  <si>
+    <t>Até hoje não foi resolvido, continuamos tomando água quente</t>
+  </si>
+  <si>
+    <t>dei zero para o atendimento de solicitar o técnico, pois demorou quase 2 meses, para poder vir fazer a manutenção preventiva. quanto o tecnico, fez o seu trabalho em 20 mn e foi embora.</t>
+  </si>
+  <si>
+    <t>não houve visita técnica.</t>
+  </si>
+  <si>
+    <t>NÃO VIERAM</t>
+  </si>
+  <si>
+    <t>Muito demorado agenda</t>
+  </si>
+  <si>
+    <t>O purificador é bom quando funciona...Meu problema é que veio um técnico viu o problema, pediu a peça, mas demorou para vir a peça e quando veio precisa de mais uma...O filtro está parado faz 1 mês</t>
+  </si>
+  <si>
+    <t>Não posso reclamar do purificador.. mas sim sobre assistência técnica..Vieram na minha casa constou que o purificador tinha que trocar .. foi agendado para depois de 1 mês (Janeiro).. ninguém veio e nem deu satisfação… liguei reagendaram para Fevereiro, fiquei praticamente 2 meses sem purificador .. mas o pagamento está em dia.. não descontaram os dias que tive que comprar água</t>
+  </si>
+  <si>
+    <t>Muito ruim. Meu purificador ficou vazando água na bancada toda. To esperando nova vista agendada para amanhã</t>
+  </si>
+  <si>
+    <t>Acho um bom produto, mas caro. Pelo valor mensal , vc compra um filtro premium por ano.</t>
+  </si>
+  <si>
+    <t>O purificador é ótimo. Mas o serviço de agendamento fica a desejar.</t>
+  </si>
+  <si>
+    <t>Meu purificador não está gelando.O técnico ficou de retornar e até o dia de hoje não retornou.Eu minha família estamos sem água gelada.</t>
+  </si>
+  <si>
+    <t>A visita de revisão de 6 meses achei ruim, pois a técnica não veio com o filtro para substituição. Acreditávamos que o filtro seria substituído nesta revisão, mas ela informou que agora ia solicitar. Por que não vem com o filtro? Teremos que aguardar novo contato para novo agendamento.</t>
+  </si>
+  <si>
+    <t>Não houve visita. Não cancelaram, não avisaram que não viriam. Achei total descaso.</t>
+  </si>
+  <si>
+    <t>Eu gosto muito da água do purificador já uso  essa água a algum tempo, mais ultimamente está complicado estou tendo o mesmo problema a alguns meses já foi feita a troca do aparelho por 2 vezes sempre pelo mesmo motivo. E o problema continua a água só sai quente e agora está quente mesmo sai até fumaça e demora muito pra para um técnico vir ver o problema e depois mais tempão pra fazer a troca com isso já tenho uns 3 meses sem filtro e pelo jeito vou continuar pois o problema continua.Agua fervendo</t>
+  </si>
+  <si>
+    <t>Boa noite!A pessoa responsável foi cordial e prestativa. Mas notamos que ficamos com um vazamento na torneira. Tentei contato pelo WhatsApp que fez a venda para programar o retorno da pessoa aqui e nao consegui mais contato. Ninguem me retorna. Inclusive gostaria de saber qual é o canal para solução de problemas. Obrigada</t>
+  </si>
+  <si>
+    <t>O aparelho está velho, fazendo barulho e vcs dizem que é normal! A qualidade da prestação de serviço só cai!</t>
+  </si>
+  <si>
+    <t>Não funciona a água com gás. O técnico esteve em casa,trocou umas peças, e nada de funcionar Péssimo atendimento</t>
+  </si>
+  <si>
+    <t>Existem dois contratos com a nossa empresa referente a dois purificadores, e quando o técnico veio aqui, fez a manutenção de apenas um, e solicitou para agendarmos outra visita para o segundo bebedouro conforme normas da Brastemp. A logística de vocês não era essa, pois quando o técnico vinha, realizava o procedimento nos dois equipamentos, evitando o transtorno e o custo de ter que voltar aqui outra vez, daqui 30 dias (prazo disponível na central). Nunca foi dessa forma, mas com a mudança de gestão, isso mudou para pior.</t>
+  </si>
+  <si>
+    <t>Na verdade, minha insatisfação está com o prestador de serviços e/ou a empresa. Ele veio, e não tive nenhum problema de comportamento ou doisa semelhante. No entanto, ele identificou que o aparelho está com uma peça defeituosa. Informou que avisaria a empresa e que entrariam em contato comigo para agendar a substituição. Avisou que ficaria pingando até está troca e realmente ficou. No entanto, até o presente momento, ninguém entrou em contato comigo para falar sobre a substituição desta peça. Pago em dia o produto, mas a manutenção não está de acordo.</t>
+  </si>
+  <si>
+    <t>Demorou muito para  vocês virem, fiquei 15 dias comprando água .</t>
+  </si>
+  <si>
+    <t>A pessoa que veio é ótima educada e prestativa, mas não resolveu o meu problema, continuou sem água fria</t>
+  </si>
+  <si>
+    <t>A comunicação entre o cliente/usuário e a brastemp é ruim, a cada atualização o aparelho fica ruim, perdendo funções importantes p a rotina de uma casa: perdeu a primeira função, a de ter a possibilidade de ter água em caso de falta de energia, depois perdeu a função, que era excelente, de timer (ele programava p desligar sozinho com 200ml, 500ml e 1l) essa função era excelente e providencial. Uso agora o modelo mais novo e os botões de acionamento são os piores de todas as versões que já tive (tive todas). Volta com o botão de timer, por favor.</t>
+  </si>
+  <si>
+    <t>Aparelho da problema desde o dia da instalação</t>
+  </si>
+  <si>
+    <t>O purificador estava cheio de mofo. Acredito que as manutenções anteriores tenham sido superficiais. Fato é que inclusive nesta, se não insistíssemos com o técnico ele não teria feita a manutenção correta. Lembrando que eu abri o chamado há quase 20 dias pois o cheio e gosto de ovo na água estavam insuportáveis. Impossibilitando o consumo. Aproveito para pedir o reembolso do dias que não pude utilizar o purificador e fiquei tendo que comprar águas no supermercado Meu custo foi superior a 100 reais.</t>
+  </si>
+  <si>
+    <t>O técnico veio quarta-feira dia 11/02/26 realizou o serviço do vazamento, porém, hoje voltou a vazar de novo.</t>
   </si>
 </sst>
 </file>
@@ -1911,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I415"/>
+  <dimension ref="A1:I441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="E406" sqref="E406"/>
+    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
+      <selection activeCell="D428" sqref="D428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13965,6 +14043,760 @@
         <v>39</v>
       </c>
     </row>
+    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>415</v>
+      </c>
+      <c r="B416" t="s">
+        <v>9</v>
+      </c>
+      <c r="C416">
+        <v>8005291277</v>
+      </c>
+      <c r="D416" s="3">
+        <v>46064.658518518518</v>
+      </c>
+      <c r="E416" t="s">
+        <v>23</v>
+      </c>
+      <c r="F416" t="s">
+        <v>16</v>
+      </c>
+      <c r="G416" t="s">
+        <v>480</v>
+      </c>
+      <c r="H416" t="s">
+        <v>18</v>
+      </c>
+      <c r="I416" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>416</v>
+      </c>
+      <c r="B417" t="s">
+        <v>9</v>
+      </c>
+      <c r="C417">
+        <v>8005284760</v>
+      </c>
+      <c r="D417" s="3">
+        <v>46065.372743055559</v>
+      </c>
+      <c r="E417" t="s">
+        <v>98</v>
+      </c>
+      <c r="F417" t="s">
+        <v>16</v>
+      </c>
+      <c r="G417" t="s">
+        <v>481</v>
+      </c>
+      <c r="H417" t="s">
+        <v>35</v>
+      </c>
+      <c r="I417" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>417</v>
+      </c>
+      <c r="B418" t="s">
+        <v>9</v>
+      </c>
+      <c r="C418">
+        <v>8005267408</v>
+      </c>
+      <c r="D418" s="3">
+        <v>46065.383090277777</v>
+      </c>
+      <c r="E418" t="s">
+        <v>23</v>
+      </c>
+      <c r="F418" t="s">
+        <v>16</v>
+      </c>
+      <c r="G418" t="s">
+        <v>482</v>
+      </c>
+      <c r="H418" t="s">
+        <v>32</v>
+      </c>
+      <c r="I418" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>418</v>
+      </c>
+      <c r="B419" t="s">
+        <v>9</v>
+      </c>
+      <c r="C419">
+        <v>8005295105</v>
+      </c>
+      <c r="D419" s="3">
+        <v>46065.385636574072</v>
+      </c>
+      <c r="E419" t="s">
+        <v>44</v>
+      </c>
+      <c r="F419" t="s">
+        <v>16</v>
+      </c>
+      <c r="G419" t="s">
+        <v>483</v>
+      </c>
+      <c r="H419" t="s">
+        <v>18</v>
+      </c>
+      <c r="I419" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>419</v>
+      </c>
+      <c r="B420" t="s">
+        <v>9</v>
+      </c>
+      <c r="C420">
+        <v>8005303841</v>
+      </c>
+      <c r="D420" s="3">
+        <v>46065.392291666663</v>
+      </c>
+      <c r="E420" t="s">
+        <v>23</v>
+      </c>
+      <c r="F420" t="s">
+        <v>16</v>
+      </c>
+      <c r="G420" t="s">
+        <v>484</v>
+      </c>
+      <c r="H420" t="s">
+        <v>18</v>
+      </c>
+      <c r="I420" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>420</v>
+      </c>
+      <c r="B421" t="s">
+        <v>9</v>
+      </c>
+      <c r="C421">
+        <v>8005257619</v>
+      </c>
+      <c r="D421" s="3">
+        <v>46065.419849537036</v>
+      </c>
+      <c r="E421" t="s">
+        <v>53</v>
+      </c>
+      <c r="F421" t="s">
+        <v>16</v>
+      </c>
+      <c r="G421" t="s">
+        <v>485</v>
+      </c>
+      <c r="H421" t="s">
+        <v>32</v>
+      </c>
+      <c r="I421" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>421</v>
+      </c>
+      <c r="B422" t="s">
+        <v>9</v>
+      </c>
+      <c r="C422">
+        <v>8005291791</v>
+      </c>
+      <c r="D422" s="3">
+        <v>46065.454837962963</v>
+      </c>
+      <c r="E422" t="s">
+        <v>20</v>
+      </c>
+      <c r="F422" t="s">
+        <v>16</v>
+      </c>
+      <c r="G422" t="s">
+        <v>486</v>
+      </c>
+      <c r="H422" t="s">
+        <v>154</v>
+      </c>
+      <c r="I422" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>422</v>
+      </c>
+      <c r="B423" t="s">
+        <v>9</v>
+      </c>
+      <c r="C423">
+        <v>8005237745</v>
+      </c>
+      <c r="D423" s="3">
+        <v>46065.505393518521</v>
+      </c>
+      <c r="E423" t="s">
+        <v>27</v>
+      </c>
+      <c r="F423" t="s">
+        <v>16</v>
+      </c>
+      <c r="G423" t="s">
+        <v>487</v>
+      </c>
+      <c r="H423" t="s">
+        <v>154</v>
+      </c>
+      <c r="I423" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>423</v>
+      </c>
+      <c r="B424" t="s">
+        <v>9</v>
+      </c>
+      <c r="C424">
+        <v>8005285541</v>
+      </c>
+      <c r="D424" s="3">
+        <v>46065.511319444442</v>
+      </c>
+      <c r="E424" t="s">
+        <v>98</v>
+      </c>
+      <c r="F424" t="s">
+        <v>16</v>
+      </c>
+      <c r="G424" t="s">
+        <v>488</v>
+      </c>
+      <c r="H424" t="s">
+        <v>35</v>
+      </c>
+      <c r="I424" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>424</v>
+      </c>
+      <c r="B425" t="s">
+        <v>9</v>
+      </c>
+      <c r="C425">
+        <v>8005303305</v>
+      </c>
+      <c r="D425" s="3">
+        <v>46065.514027777783</v>
+      </c>
+      <c r="E425" t="s">
+        <v>15</v>
+      </c>
+      <c r="F425" t="s">
+        <v>16</v>
+      </c>
+      <c r="G425" t="s">
+        <v>489</v>
+      </c>
+      <c r="H425" t="s">
+        <v>13</v>
+      </c>
+      <c r="I425" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>425</v>
+      </c>
+      <c r="B426" t="s">
+        <v>9</v>
+      </c>
+      <c r="C426">
+        <v>8005241764</v>
+      </c>
+      <c r="D426" s="3">
+        <v>46065.536782407413</v>
+      </c>
+      <c r="E426" t="s">
+        <v>23</v>
+      </c>
+      <c r="F426" t="s">
+        <v>11</v>
+      </c>
+      <c r="G426" t="s">
+        <v>490</v>
+      </c>
+      <c r="H426" t="s">
+        <v>13</v>
+      </c>
+      <c r="I426" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>426</v>
+      </c>
+      <c r="B427" t="s">
+        <v>9</v>
+      </c>
+      <c r="C427">
+        <v>8005283681</v>
+      </c>
+      <c r="D427" s="3">
+        <v>46065.55097222222</v>
+      </c>
+      <c r="E427" t="s">
+        <v>65</v>
+      </c>
+      <c r="F427" t="s">
+        <v>16</v>
+      </c>
+      <c r="G427" t="s">
+        <v>491</v>
+      </c>
+      <c r="H427" t="s">
+        <v>18</v>
+      </c>
+      <c r="I427" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>427</v>
+      </c>
+      <c r="B428" t="s">
+        <v>9</v>
+      </c>
+      <c r="C428">
+        <v>8005285931</v>
+      </c>
+      <c r="D428" s="3">
+        <v>46065.721574074072</v>
+      </c>
+      <c r="E428" t="s">
+        <v>20</v>
+      </c>
+      <c r="F428" t="s">
+        <v>11</v>
+      </c>
+      <c r="G428" t="s">
+        <v>492</v>
+      </c>
+      <c r="H428" t="s">
+        <v>18</v>
+      </c>
+      <c r="I428" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>428</v>
+      </c>
+      <c r="B429" t="s">
+        <v>9</v>
+      </c>
+      <c r="C429">
+        <v>8005259426</v>
+      </c>
+      <c r="D429" s="3">
+        <v>46065.837685185194</v>
+      </c>
+      <c r="E429" t="s">
+        <v>53</v>
+      </c>
+      <c r="F429" t="s">
+        <v>16</v>
+      </c>
+      <c r="G429" t="s">
+        <v>493</v>
+      </c>
+      <c r="H429" t="s">
+        <v>18</v>
+      </c>
+      <c r="I429" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>429</v>
+      </c>
+      <c r="B430" t="s">
+        <v>9</v>
+      </c>
+      <c r="C430">
+        <v>8005279203</v>
+      </c>
+      <c r="D430" s="3">
+        <v>46065.852824074071</v>
+      </c>
+      <c r="E430" t="s">
+        <v>23</v>
+      </c>
+      <c r="F430" t="s">
+        <v>11</v>
+      </c>
+      <c r="G430" t="s">
+        <v>494</v>
+      </c>
+      <c r="H430" t="s">
+        <v>35</v>
+      </c>
+      <c r="I430" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>430</v>
+      </c>
+      <c r="B431" t="s">
+        <v>61</v>
+      </c>
+      <c r="C431">
+        <v>8005300765</v>
+      </c>
+      <c r="D431" s="3">
+        <v>46065.854409722233</v>
+      </c>
+      <c r="E431" t="s">
+        <v>70</v>
+      </c>
+      <c r="F431" t="s">
+        <v>16</v>
+      </c>
+      <c r="G431" t="s">
+        <v>495</v>
+      </c>
+      <c r="H431" t="s">
+        <v>18</v>
+      </c>
+      <c r="I431" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>431</v>
+      </c>
+      <c r="B432" t="s">
+        <v>9</v>
+      </c>
+      <c r="C432">
+        <v>8005285560</v>
+      </c>
+      <c r="D432" s="3">
+        <v>46066.37226851852</v>
+      </c>
+      <c r="E432" t="s">
+        <v>20</v>
+      </c>
+      <c r="F432" t="s">
+        <v>16</v>
+      </c>
+      <c r="G432" t="s">
+        <v>496</v>
+      </c>
+      <c r="H432" t="s">
+        <v>35</v>
+      </c>
+      <c r="I432" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>432</v>
+      </c>
+      <c r="B433" t="s">
+        <v>9</v>
+      </c>
+      <c r="C433">
+        <v>8005280193</v>
+      </c>
+      <c r="D433" s="3">
+        <v>46066.40116898148</v>
+      </c>
+      <c r="E433" t="s">
+        <v>15</v>
+      </c>
+      <c r="F433" t="s">
+        <v>16</v>
+      </c>
+      <c r="G433" t="s">
+        <v>497</v>
+      </c>
+      <c r="H433" t="s">
+        <v>35</v>
+      </c>
+      <c r="I433" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>433</v>
+      </c>
+      <c r="B434" t="s">
+        <v>9</v>
+      </c>
+      <c r="C434">
+        <v>8005280801</v>
+      </c>
+      <c r="D434" s="3">
+        <v>46066.414884259262</v>
+      </c>
+      <c r="E434" t="s">
+        <v>20</v>
+      </c>
+      <c r="F434" t="s">
+        <v>16</v>
+      </c>
+      <c r="G434" t="s">
+        <v>498</v>
+      </c>
+      <c r="H434" t="s">
+        <v>32</v>
+      </c>
+      <c r="I434" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>434</v>
+      </c>
+      <c r="B435" t="s">
+        <v>9</v>
+      </c>
+      <c r="C435">
+        <v>8005257620</v>
+      </c>
+      <c r="D435" s="3">
+        <v>46066.467534722222</v>
+      </c>
+      <c r="E435" t="s">
+        <v>27</v>
+      </c>
+      <c r="F435" t="s">
+        <v>16</v>
+      </c>
+      <c r="G435" t="s">
+        <v>499</v>
+      </c>
+      <c r="H435" t="s">
+        <v>18</v>
+      </c>
+      <c r="I435" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>435</v>
+      </c>
+      <c r="B436" t="s">
+        <v>9</v>
+      </c>
+      <c r="C436">
+        <v>8005282612</v>
+      </c>
+      <c r="D436" s="3">
+        <v>46066.502013888887</v>
+      </c>
+      <c r="E436" t="s">
+        <v>20</v>
+      </c>
+      <c r="F436" t="s">
+        <v>16</v>
+      </c>
+      <c r="G436" t="s">
+        <v>500</v>
+      </c>
+      <c r="H436" t="s">
+        <v>32</v>
+      </c>
+      <c r="I436" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>436</v>
+      </c>
+      <c r="B437" t="s">
+        <v>9</v>
+      </c>
+      <c r="C437">
+        <v>8005300267</v>
+      </c>
+      <c r="D437" s="3">
+        <v>46066.503460648149</v>
+      </c>
+      <c r="E437" t="s">
+        <v>10</v>
+      </c>
+      <c r="F437" t="s">
+        <v>16</v>
+      </c>
+      <c r="G437" t="s">
+        <v>501</v>
+      </c>
+      <c r="H437" t="s">
+        <v>35</v>
+      </c>
+      <c r="I437" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>437</v>
+      </c>
+      <c r="B438" t="s">
+        <v>9</v>
+      </c>
+      <c r="C438">
+        <v>8005277871</v>
+      </c>
+      <c r="D438" s="3">
+        <v>46066.503738425927</v>
+      </c>
+      <c r="E438" t="s">
+        <v>74</v>
+      </c>
+      <c r="F438" t="s">
+        <v>11</v>
+      </c>
+      <c r="G438" t="s">
+        <v>502</v>
+      </c>
+      <c r="H438" t="s">
+        <v>35</v>
+      </c>
+      <c r="I438" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>438</v>
+      </c>
+      <c r="B439" t="s">
+        <v>9</v>
+      </c>
+      <c r="C439">
+        <v>8005295803</v>
+      </c>
+      <c r="D439" s="3">
+        <v>46066.503981481481</v>
+      </c>
+      <c r="E439" t="s">
+        <v>68</v>
+      </c>
+      <c r="F439" t="s">
+        <v>16</v>
+      </c>
+      <c r="G439" t="s">
+        <v>503</v>
+      </c>
+      <c r="H439" t="s">
+        <v>35</v>
+      </c>
+      <c r="I439" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>439</v>
+      </c>
+      <c r="B440" t="s">
+        <v>9</v>
+      </c>
+      <c r="C440">
+        <v>8005280807</v>
+      </c>
+      <c r="D440" s="3">
+        <v>46066.555960648147</v>
+      </c>
+      <c r="E440" t="s">
+        <v>20</v>
+      </c>
+      <c r="F440" t="s">
+        <v>16</v>
+      </c>
+      <c r="G440" t="s">
+        <v>504</v>
+      </c>
+      <c r="H440" t="s">
+        <v>18</v>
+      </c>
+      <c r="I440" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>440</v>
+      </c>
+      <c r="B441" t="s">
+        <v>9</v>
+      </c>
+      <c r="C441">
+        <v>8005303612</v>
+      </c>
+      <c r="D441" s="3">
+        <v>46066.560902777783</v>
+      </c>
+      <c r="E441" t="s">
+        <v>98</v>
+      </c>
+      <c r="F441" t="s">
+        <v>11</v>
+      </c>
+      <c r="G441" t="s">
+        <v>505</v>
+      </c>
+      <c r="H441" t="s">
+        <v>278</v>
+      </c>
+      <c r="I441" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 17/02/2026 10:13:07,11
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77640EB1-4CB6-4E9C-B73B-C49D2DB7AC09}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C76B3E-0A2B-4971-9E56-E609FD71B3BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="513">
   <si>
     <t>ID</t>
   </si>
@@ -1621,6 +1621,27 @@
   </si>
   <si>
     <t>O técnico veio quarta-feira dia 11/02/26 realizou o serviço do vazamento, porém, hoje voltou a vazar de novo.</t>
+  </si>
+  <si>
+    <t>Deixou a desejar, não tem o controle de volume de água.</t>
+  </si>
+  <si>
+    <t>Vocês agendam para a troca e não trocam? informaram que nao era preciso a troca do filtro? que se a agua ficar turva era pra eu ligar pra vcs!? aguardo retorno e explicação. obrigada</t>
+  </si>
+  <si>
+    <t>Péssimo atendimento.Meu purificador está com a água com odor e sabor horríveis, mesmo após a troca do elemento filtrante, e além disso, não para de vazar.Já fiz vários contatos com a Brastemp agendando visita e o técnico não aparece.Estou sem água, em pleno feriado, e com a minha mensalidade em dia.</t>
+  </si>
+  <si>
+    <t>Após a troca a água está com gosto de metal, inviabilizando o consumo.Estou consumindo garrafão de água mineral desde o dia da troca do aparelho. Deveria o técnico ter retornado a minha residência no dia seguinte,após a reclamação do ocorrido no epígrafe  citado acima,pela comunicação imediata q fizemos do ocorrido. No entanto a resposta de vcs foi q somente no dia 27 haverá retorno do técnico para correção,após a avaliação da empresa em 48hs,e sem me retornar sobre a análise.Temos um contrato longo e até agora tem sido satisfatório o atendimento. Mas neste caso é imperdoável o péssimo atendimento prestado. O técnico foi recebido pelo meu marido, José Gorgulho,em nossa residência.</t>
+  </si>
+  <si>
+    <t>Que visita ???A que estava marcada para ontem, na parte da manhã, não existiu e nem foi informado o porquê da NÃO VISITA ?!?!?!</t>
+  </si>
+  <si>
+    <t>Estou desde o dia 16 de janeiro lutando para a Brastemp consertar o purificador que tenho como parte de assinatura e a empresa so enrolando, causando prejuízo financeiro.</t>
+  </si>
+  <si>
+    <t>Achei que o técnico abriria e limparia o filtro por dentro ,olharia com mais detalhes como foi feito das outras vezes, desta vez levou’nem 5 min. Do colocou augusto medidor dele e foi embora  o prestador foi educado mas não fez a limpeza como os outros</t>
   </si>
 </sst>
 </file>
@@ -1989,10 +2010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I441"/>
+  <dimension ref="A1:I448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
-      <selection activeCell="D428" sqref="D428"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="D430" sqref="D430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14797,6 +14818,209 @@
         <v>22</v>
       </c>
     </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>441</v>
+      </c>
+      <c r="B442" t="s">
+        <v>9</v>
+      </c>
+      <c r="C442">
+        <v>8005268967</v>
+      </c>
+      <c r="D442" s="3">
+        <v>46066.721226851849</v>
+      </c>
+      <c r="E442" t="s">
+        <v>20</v>
+      </c>
+      <c r="F442" t="s">
+        <v>16</v>
+      </c>
+      <c r="G442" t="s">
+        <v>506</v>
+      </c>
+      <c r="H442" t="s">
+        <v>18</v>
+      </c>
+      <c r="I442" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>442</v>
+      </c>
+      <c r="B443" t="s">
+        <v>9</v>
+      </c>
+      <c r="C443">
+        <v>8005269229</v>
+      </c>
+      <c r="D443" s="3">
+        <v>46067.394606481481</v>
+      </c>
+      <c r="E443" t="s">
+        <v>20</v>
+      </c>
+      <c r="F443" t="s">
+        <v>16</v>
+      </c>
+      <c r="G443" t="s">
+        <v>507</v>
+      </c>
+      <c r="H443" t="s">
+        <v>18</v>
+      </c>
+      <c r="I443" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>443</v>
+      </c>
+      <c r="B444" t="s">
+        <v>9</v>
+      </c>
+      <c r="C444">
+        <v>8005291990</v>
+      </c>
+      <c r="D444" s="3">
+        <v>46067.460833333331</v>
+      </c>
+      <c r="E444" t="s">
+        <v>53</v>
+      </c>
+      <c r="F444" t="s">
+        <v>16</v>
+      </c>
+      <c r="G444" t="s">
+        <v>508</v>
+      </c>
+      <c r="H444" t="s">
+        <v>35</v>
+      </c>
+      <c r="I444" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>444</v>
+      </c>
+      <c r="B445" t="s">
+        <v>9</v>
+      </c>
+      <c r="C445">
+        <v>8005292916</v>
+      </c>
+      <c r="D445" s="3">
+        <v>46067.4997337963</v>
+      </c>
+      <c r="E445" t="s">
+        <v>53</v>
+      </c>
+      <c r="F445" t="s">
+        <v>16</v>
+      </c>
+      <c r="G445" t="s">
+        <v>509</v>
+      </c>
+      <c r="H445" t="s">
+        <v>35</v>
+      </c>
+      <c r="I445" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>445</v>
+      </c>
+      <c r="B446" t="s">
+        <v>9</v>
+      </c>
+      <c r="C446">
+        <v>8005299129</v>
+      </c>
+      <c r="D446" s="3">
+        <v>46067.511400462965</v>
+      </c>
+      <c r="E446" t="s">
+        <v>37</v>
+      </c>
+      <c r="F446" t="s">
+        <v>11</v>
+      </c>
+      <c r="G446" t="s">
+        <v>510</v>
+      </c>
+      <c r="H446" t="s">
+        <v>18</v>
+      </c>
+      <c r="I446" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>446</v>
+      </c>
+      <c r="B447" t="s">
+        <v>9</v>
+      </c>
+      <c r="C447">
+        <v>8005290263</v>
+      </c>
+      <c r="D447" s="3">
+        <v>46068.373749999999</v>
+      </c>
+      <c r="E447" t="s">
+        <v>53</v>
+      </c>
+      <c r="F447" t="s">
+        <v>16</v>
+      </c>
+      <c r="G447" t="s">
+        <v>511</v>
+      </c>
+      <c r="H447" t="s">
+        <v>18</v>
+      </c>
+      <c r="I447" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>447</v>
+      </c>
+      <c r="B448" t="s">
+        <v>9</v>
+      </c>
+      <c r="C448">
+        <v>8005286062</v>
+      </c>
+      <c r="D448" s="3">
+        <v>46069.42597222222</v>
+      </c>
+      <c r="E448" t="s">
+        <v>20</v>
+      </c>
+      <c r="F448" t="s">
+        <v>16</v>
+      </c>
+      <c r="G448" t="s">
+        <v>512</v>
+      </c>
+      <c r="H448" t="s">
+        <v>18</v>
+      </c>
+      <c r="I448" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao de arquivos - 21/02/2026 11:55:07,71
</commit_message>
<xml_diff>
--- a/NPS Classificado.xlsx
+++ b/NPS Classificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://algarnet-my.sharepoint.com/personal/eduardacjr_algartech_com/Documents/Área de Trabalho/Dashboards/NPSMedalliaequaltricsculligan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C76B3E-0A2B-4971-9E56-E609FD71B3BE}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{855DE731-06B6-4F67-B5F3-79AE1FB3CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7631074-5B3A-46E7-B758-81F1D81D5395}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2811" uniqueCount="533">
   <si>
     <t>ID</t>
   </si>
@@ -1642,6 +1642,66 @@
   </si>
   <si>
     <t>Achei que o técnico abriria e limparia o filtro por dentro ,olharia com mais detalhes como foi feito das outras vezes, desta vez levou’nem 5 min. Do colocou augusto medidor dele e foi embora  o prestador foi educado mas não fez a limpeza como os outros</t>
+  </si>
+  <si>
+    <t>Ele é muito bom! Porém a mensalidade está se tornando um fardo! Esse ano troco por outro purificador!</t>
+  </si>
+  <si>
+    <t>Adoro o atendimento de vcs mais , desta vez nao trocou meu filtro.</t>
+  </si>
+  <si>
+    <t>O aparelho está fazendo barulho. Está atrapalhando dormir a noite.</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Água fresca e gostosa</t>
+  </si>
+  <si>
+    <t>O pós-venda não está funcionando</t>
+  </si>
+  <si>
+    <t>É a segunda vez que o técnico vem e não resolve o problema.Inicialmente trocou o filtro e depois de 3 dias o filtro apresentou o mesmo problema, daí o técnico voltou e disse que precisa substituir a peça.Substituir peça de um produto novo???? Estranho.E passa um prazo extenso para resolver, e preciso ligar para pedir prioridade.</t>
+  </si>
+  <si>
+    <t>Instalaram o equipamento, funcionou e no mesmo dia parou de funcionar a água gelada. Já solicitamos a presença do técnico há mais 03 dias e não fomos atendidos No aguardo</t>
+  </si>
+  <si>
+    <t>Mesmo solicitando um tecnico com urgencia, o purificador estava vazando agua, so agendaram 4 dias depois, disseram que foi por causa do carnaval, mas o vazamento não sai em bloquinho!!!!!!!</t>
+  </si>
+  <si>
+    <t>Estamos a 3 semanas aguardando a troca do purificador que NÃO está gelando ..protocolo ( 8005280980 )..local que tem 30 pessoas tomando água quente 🥵</t>
+  </si>
+  <si>
+    <t>Uma demora sem fim para o conserto</t>
+  </si>
+  <si>
+    <t>Boa tarde muito mal instalado o puricador o rapaz nem ferramentas tinha para concluir o serviço solicito a reinstalação aqui ficou tudo feio a instalação</t>
+  </si>
+  <si>
+    <t>Péssima , até agora não funcionou, colocou um aparelho e só funcionou só um dia , já reclamei, marcaram uma visita hoje até às 13 horas , poderia dá uma preferência, obrigado.</t>
+  </si>
+  <si>
+    <t>Possuo a locação do purificador Brastemp a 10 anos e o produto é excelente .Infelizmente , pela primeira vez considerei em rescindir o contrato .Ocorre que estou com problemas no purificador sem poder usa-lo , já houveram duas visitas técnicas e , apesar do grande esforço dos técnicos , chegou-se à conclusão que seria necessário a troca do mesmo . A água gelada não funciona e nem sai ,  e a água natural sai muito quente . Apesar da situação grave já ocorrendo a trinta dias , sem poder utiliza-lo , a troca está marcada apenas para o dia 31/03/2026 . Pelo péssimo atendimento e negligência , o que senti começando a ocorrer recente , e apesar do produto ser excelente , ainda estou analisando a possibilidade de rescisão do contrato e compra de outro filtro de água . Inclusive , financeiramente seria vantajoso , pois  com o valor de 01 ano de locação conseguiria comprar um purificador de ótima qualidade .</t>
+  </si>
+  <si>
+    <t>Boa. Duradouro</t>
+  </si>
+  <si>
+    <t>O purificador e muito bom e asistencia e boa mas o valor que e alto ainda mais que reformei o apartamebto e estou ha praticamente 2 anks morando fora e pagando sem usar o aparelho</t>
+  </si>
+  <si>
+    <t>O purificador é bom, mas o sistema de marcação de visitas é deficiente</t>
+  </si>
+  <si>
+    <t>Muito frustrante o atendimento de manutenção. Minha instalação não foi concluída até hoje, apesar de várias remarcações para atendimento.</t>
+  </si>
+  <si>
+    <t>Apesar do conceito e do produto serem bons, a área de tecnologia, agendamento e solicitações de serviços é terrível. Não consigo imaginar algo pior. Agendamentos que não se completam, excesso de ligações de agendamento que falham, solicitações no agendamento ignoradas. Agendamentos duplicados. A área de TI é terrível</t>
+  </si>
+  <si>
+    <t>Foi feito a troca dos filtros , mas ficou pingando o ponto de água na parede(mangueira) com a manipulação do aparelho. Deveria fazer um check list para tentar identificar esses problemas</t>
   </si>
 </sst>
 </file>
@@ -2010,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I448"/>
+  <dimension ref="A1:I468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="D430" sqref="D430"/>
+    <sheetView tabSelected="1" topLeftCell="B442" workbookViewId="0">
+      <selection activeCell="G447" sqref="G447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15021,6 +15081,586 @@
         <v>51</v>
       </c>
     </row>
+    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>448</v>
+      </c>
+      <c r="B449" t="s">
+        <v>9</v>
+      </c>
+      <c r="C449">
+        <v>8005278265</v>
+      </c>
+      <c r="D449" s="3">
+        <v>46070.536539351851</v>
+      </c>
+      <c r="E449" t="s">
+        <v>41</v>
+      </c>
+      <c r="F449" t="s">
+        <v>16</v>
+      </c>
+      <c r="G449" t="s">
+        <v>513</v>
+      </c>
+      <c r="H449" t="s">
+        <v>13</v>
+      </c>
+      <c r="I449" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>449</v>
+      </c>
+      <c r="B450" t="s">
+        <v>9</v>
+      </c>
+      <c r="C450">
+        <v>8005285427</v>
+      </c>
+      <c r="D450" s="3">
+        <v>46070.549305555563</v>
+      </c>
+      <c r="E450" t="s">
+        <v>53</v>
+      </c>
+      <c r="F450" t="s">
+        <v>11</v>
+      </c>
+      <c r="G450" t="s">
+        <v>514</v>
+      </c>
+      <c r="H450" t="s">
+        <v>18</v>
+      </c>
+      <c r="I450" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>450</v>
+      </c>
+      <c r="B451" t="s">
+        <v>9</v>
+      </c>
+      <c r="C451">
+        <v>8005283658</v>
+      </c>
+      <c r="D451" s="3">
+        <v>46070.565648148149</v>
+      </c>
+      <c r="E451" t="s">
+        <v>15</v>
+      </c>
+      <c r="F451" t="s">
+        <v>16</v>
+      </c>
+      <c r="G451" t="s">
+        <v>515</v>
+      </c>
+      <c r="H451" t="s">
+        <v>35</v>
+      </c>
+      <c r="I451" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>451</v>
+      </c>
+      <c r="B452" t="s">
+        <v>9</v>
+      </c>
+      <c r="C452">
+        <v>8005285843</v>
+      </c>
+      <c r="D452" s="3">
+        <v>46070.623692129629</v>
+      </c>
+      <c r="E452" t="s">
+        <v>20</v>
+      </c>
+      <c r="F452" t="s">
+        <v>11</v>
+      </c>
+      <c r="G452" t="s">
+        <v>516</v>
+      </c>
+      <c r="H452" t="s">
+        <v>13</v>
+      </c>
+      <c r="I452" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>452</v>
+      </c>
+      <c r="B453" t="s">
+        <v>9</v>
+      </c>
+      <c r="C453">
+        <v>8005293582</v>
+      </c>
+      <c r="D453" s="3">
+        <v>46070.685486111113</v>
+      </c>
+      <c r="E453" t="s">
+        <v>464</v>
+      </c>
+      <c r="F453" t="s">
+        <v>11</v>
+      </c>
+      <c r="G453" t="s">
+        <v>517</v>
+      </c>
+      <c r="H453" t="s">
+        <v>13</v>
+      </c>
+      <c r="I453" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>453</v>
+      </c>
+      <c r="B454" t="s">
+        <v>9</v>
+      </c>
+      <c r="C454">
+        <v>8005300015</v>
+      </c>
+      <c r="D454" s="3">
+        <v>46071.391458333332</v>
+      </c>
+      <c r="E454" t="s">
+        <v>53</v>
+      </c>
+      <c r="F454" t="s">
+        <v>16</v>
+      </c>
+      <c r="G454" t="s">
+        <v>518</v>
+      </c>
+      <c r="H454" t="s">
+        <v>13</v>
+      </c>
+      <c r="I454" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>454</v>
+      </c>
+      <c r="B455" t="s">
+        <v>9</v>
+      </c>
+      <c r="C455">
+        <v>8005304089</v>
+      </c>
+      <c r="D455" s="3">
+        <v>46071.535034722219</v>
+      </c>
+      <c r="E455" t="s">
+        <v>20</v>
+      </c>
+      <c r="F455" t="s">
+        <v>16</v>
+      </c>
+      <c r="G455" t="s">
+        <v>519</v>
+      </c>
+      <c r="H455" t="s">
+        <v>18</v>
+      </c>
+      <c r="I455" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>455</v>
+      </c>
+      <c r="B456" t="s">
+        <v>61</v>
+      </c>
+      <c r="C456">
+        <v>8005295235</v>
+      </c>
+      <c r="D456" s="3">
+        <v>46071.627256944441</v>
+      </c>
+      <c r="E456" t="s">
+        <v>53</v>
+      </c>
+      <c r="F456" t="s">
+        <v>16</v>
+      </c>
+      <c r="G456" t="s">
+        <v>520</v>
+      </c>
+      <c r="H456" t="s">
+        <v>35</v>
+      </c>
+      <c r="I456" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>456</v>
+      </c>
+      <c r="B457" t="s">
+        <v>9</v>
+      </c>
+      <c r="C457">
+        <v>8005308413</v>
+      </c>
+      <c r="D457" s="3">
+        <v>46072.391539351847</v>
+      </c>
+      <c r="E457" t="s">
+        <v>15</v>
+      </c>
+      <c r="F457" t="s">
+        <v>16</v>
+      </c>
+      <c r="G457" t="s">
+        <v>521</v>
+      </c>
+      <c r="H457" t="s">
+        <v>32</v>
+      </c>
+      <c r="I457" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>457</v>
+      </c>
+      <c r="B458" t="s">
+        <v>9</v>
+      </c>
+      <c r="C458">
+        <v>8005169116</v>
+      </c>
+      <c r="D458" s="3">
+        <v>46072.397615740738</v>
+      </c>
+      <c r="E458" t="s">
+        <v>20</v>
+      </c>
+      <c r="F458" t="s">
+        <v>16</v>
+      </c>
+      <c r="G458" t="s">
+        <v>522</v>
+      </c>
+      <c r="H458" t="s">
+        <v>154</v>
+      </c>
+      <c r="I458" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>458</v>
+      </c>
+      <c r="B459" t="s">
+        <v>9</v>
+      </c>
+      <c r="C459">
+        <v>8005299637</v>
+      </c>
+      <c r="D459" s="3">
+        <v>46072.496122685188</v>
+      </c>
+      <c r="E459" t="s">
+        <v>20</v>
+      </c>
+      <c r="F459" t="s">
+        <v>16</v>
+      </c>
+      <c r="G459" t="s">
+        <v>523</v>
+      </c>
+      <c r="H459" t="s">
+        <v>32</v>
+      </c>
+      <c r="I459" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="460" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>459</v>
+      </c>
+      <c r="B460" t="s">
+        <v>61</v>
+      </c>
+      <c r="C460">
+        <v>8005306854</v>
+      </c>
+      <c r="D460" s="3">
+        <v>46072.659386574072</v>
+      </c>
+      <c r="E460" t="s">
+        <v>41</v>
+      </c>
+      <c r="F460" t="s">
+        <v>16</v>
+      </c>
+      <c r="G460" t="s">
+        <v>524</v>
+      </c>
+      <c r="H460" t="s">
+        <v>18</v>
+      </c>
+      <c r="I460" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>460</v>
+      </c>
+      <c r="B461" t="s">
+        <v>61</v>
+      </c>
+      <c r="C461">
+        <v>8005255862</v>
+      </c>
+      <c r="D461" s="3">
+        <v>46073.40221064815</v>
+      </c>
+      <c r="E461" t="s">
+        <v>53</v>
+      </c>
+      <c r="F461" t="s">
+        <v>16</v>
+      </c>
+      <c r="G461" t="s">
+        <v>525</v>
+      </c>
+      <c r="H461" t="s">
+        <v>35</v>
+      </c>
+      <c r="I461" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>461</v>
+      </c>
+      <c r="B462" t="s">
+        <v>9</v>
+      </c>
+      <c r="C462">
+        <v>8005304885</v>
+      </c>
+      <c r="D462" s="3">
+        <v>46073.421550925923</v>
+      </c>
+      <c r="E462" t="s">
+        <v>49</v>
+      </c>
+      <c r="F462" t="s">
+        <v>16</v>
+      </c>
+      <c r="G462" t="s">
+        <v>526</v>
+      </c>
+      <c r="H462" t="s">
+        <v>154</v>
+      </c>
+      <c r="I462" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>462</v>
+      </c>
+      <c r="B463" t="s">
+        <v>9</v>
+      </c>
+      <c r="C463">
+        <v>8005304787</v>
+      </c>
+      <c r="D463" s="3">
+        <v>46073.44326388889</v>
+      </c>
+      <c r="E463" t="s">
+        <v>37</v>
+      </c>
+      <c r="F463" t="s">
+        <v>11</v>
+      </c>
+      <c r="G463" t="s">
+        <v>527</v>
+      </c>
+      <c r="H463" t="s">
+        <v>13</v>
+      </c>
+      <c r="I463" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>463</v>
+      </c>
+      <c r="B464" t="s">
+        <v>9</v>
+      </c>
+      <c r="C464">
+        <v>8005293236</v>
+      </c>
+      <c r="D464" s="3">
+        <v>46073.486342592587</v>
+      </c>
+      <c r="E464" t="s">
+        <v>20</v>
+      </c>
+      <c r="F464" t="s">
+        <v>16</v>
+      </c>
+      <c r="G464" t="s">
+        <v>528</v>
+      </c>
+      <c r="H464" t="s">
+        <v>13</v>
+      </c>
+      <c r="I464" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>464</v>
+      </c>
+      <c r="B465" t="s">
+        <v>9</v>
+      </c>
+      <c r="C465">
+        <v>8005286266</v>
+      </c>
+      <c r="D465" s="3">
+        <v>46073.524375000001</v>
+      </c>
+      <c r="E465" t="s">
+        <v>262</v>
+      </c>
+      <c r="F465" t="s">
+        <v>16</v>
+      </c>
+      <c r="G465" t="s">
+        <v>529</v>
+      </c>
+      <c r="H465" t="s">
+        <v>82</v>
+      </c>
+      <c r="I465" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>465</v>
+      </c>
+      <c r="B466" t="s">
+        <v>9</v>
+      </c>
+      <c r="C466">
+        <v>8005274003</v>
+      </c>
+      <c r="D466" s="3">
+        <v>46073.552395833343</v>
+      </c>
+      <c r="E466" t="s">
+        <v>53</v>
+      </c>
+      <c r="F466" t="s">
+        <v>16</v>
+      </c>
+      <c r="G466" t="s">
+        <v>530</v>
+      </c>
+      <c r="H466" t="s">
+        <v>18</v>
+      </c>
+      <c r="I466" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>466</v>
+      </c>
+      <c r="B467" t="s">
+        <v>9</v>
+      </c>
+      <c r="C467">
+        <v>8005286210</v>
+      </c>
+      <c r="D467" s="3">
+        <v>46073.762187499997</v>
+      </c>
+      <c r="E467" t="s">
+        <v>20</v>
+      </c>
+      <c r="F467" t="s">
+        <v>11</v>
+      </c>
+      <c r="G467" t="s">
+        <v>531</v>
+      </c>
+      <c r="H467" t="s">
+        <v>82</v>
+      </c>
+      <c r="I467" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>467</v>
+      </c>
+      <c r="B468" t="s">
+        <v>9</v>
+      </c>
+      <c r="C468">
+        <v>8005286288</v>
+      </c>
+      <c r="D468" s="3">
+        <v>46073.766284722216</v>
+      </c>
+      <c r="E468" t="s">
+        <v>74</v>
+      </c>
+      <c r="F468" t="s">
+        <v>11</v>
+      </c>
+      <c r="G468" t="s">
+        <v>532</v>
+      </c>
+      <c r="H468" t="s">
+        <v>18</v>
+      </c>
+      <c r="I468" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>